<commit_message>
Cleaned data, adjusted from inflation, and started analysis
</commit_message>
<xml_diff>
--- a/project2/Data/weeklyincome_occupation_gender_combined_clean_all.xlsx
+++ b/project2/Data/weeklyincome_occupation_gender_combined_clean_all.xlsx
@@ -610,1156 +610,1156 @@
     <t>[58.16326530612245, 57.065217391304344, 56.39686684073107, 58.96103896103896, 59.654178674351584, 54.98489425981873, 52.28758169934641, 55.00000000000001, 54.04624277456648, 58.13148788927336, 59.04761904761905, 65.97014925373135, 56.334231805929925, 63.660477453580896, 59.02578796561605, 62.0]</t>
   </si>
   <si>
-    <t>[184.0, 171.0, 166.0, 169.0, 152.0, 154.0, 163.0, 148.0, 155.0, 162.0, 160.0, 152.0, 143.0, 137.0, 140.0, 143.0]</t>
-  </si>
-  <si>
-    <t>[390.0, 390.0, 393.0, 387.0, 365.0, 376.0, 377.0, 328.0, 333.0, 341.0, 346.0, 329.0, 314.0, 300.0, 318.0, 301.0]</t>
-  </si>
-  <si>
-    <t>[369.0, 392.0, 392.0, 363.0, 360.0, 363.0, 394.0, 393.0, 392.0, 379.0, 402.0, 353.0, 350.0, 320.0, 346.0, 344.0]</t>
-  </si>
-  <si>
-    <t>[349.0, 400.0, 391.0, 347.0, 327.0, 353.0, 392.0, 409.0, 396.0, 382.0, 405.0, 374.0, 338.0, 328.0, 344.0, 323.0]</t>
-  </si>
-  <si>
-    <t>[752.0, 495.0, 543.0, 415.0, 674.0, 455.0, 545.0, 658.0, 619.0, 531.0, 396.0, 382.0, 485.0, 490.0, 565.0, 493.0]</t>
-  </si>
-  <si>
-    <t>[288.0, 354.0, 321.0, 345.0, 214.0, 283.0, 465.0, 347.0, 382.0, 262.0, 322.0, 345.0, 299.0, 220.0, 294.0, 204.0]</t>
-  </si>
-  <si>
-    <t>[490.0, 459.0, 603.0, 345.0, 474.0, 534.0, 530.0, 533.0, 524.0, 484.0, 577.0, 483.0, 497.0, 450.0, 543.0, 367.0]</t>
-  </si>
-  <si>
-    <t>[193.0, 268.0, 76.0, 254.0, 234.0, 220.0, 213.0, 52.0, 314.0, 377.0, 381.0, 233.0, 192.0, 446.0, 319.0, 157.0]</t>
-  </si>
-  <si>
-    <t>[522.0, 497.0, 513.0, 602.0, 544.0, 454.0, 417.0, 513.0, 524.0, 482.0, 512.0, 543.0, 527.0, 494.0, 558.0, 491.0]</t>
-  </si>
-  <si>
-    <t>[431.0, 468.0, 454.0, 221.0, 527.0, 296.0, 239.0, 215.0, 288.0, 476.0, 296.0, 508.0, 424.0, 359.0, 301.0, 370.0]</t>
-  </si>
-  <si>
-    <t>[202.0, 282.0, 231.0, 178.0, 90.0, 151.0, 395.0, 342.0, 344.0, 354.0, 256.0, 320.0, 255.0, 260.0, 207.0, 453.0]</t>
-  </si>
-  <si>
-    <t>[318.0, 318.0, 248.0, 333.0, 268.0, 413.0, 514.0, 471.0, 259.0, 339.0, 398.0, 411.0, 258.0, 317.0, 267.0, 294.0]</t>
-  </si>
-  <si>
-    <t>[214.0, 220.0, 221.0, 140.0, 211.0, 181.0, 143.0, 135.0, 170.0, 152.0, 111.0, 147.0, 181.0, 191.0, 115.0, 122.0]</t>
-  </si>
-  <si>
-    <t>[398.0, 313.0, 356.0, 266.0, 233.0, 188.0, 354.0, 290.0, 347.0, 305.0, 438.0, 351.0, 364.0, 301.0, 192.0, 195.0]</t>
-  </si>
-  <si>
-    <t>[221.0, 290.0, 342.0, 314.0, 111.0, 284.0, 228.0, 473.0, 385.0, 191.0, 296.0, 238.0, 227.0, 141.0, 144.0, 211.0]</t>
-  </si>
-  <si>
-    <t>[279.0, 229.0, 214.0, 177.0, 164.0, 146.0, 268.0, 248.0, 248.0, 249.0, 383.0, 150.0, 218.0, 206.0, 246.0, 78.0]</t>
-  </si>
-  <si>
-    <t>[278.0, 335.0, 355.0, 323.0, 328.0, 284.0, 322.0, 288.0, 313.0, 277.0, 282.0, 299.0, 306.0, 259.0, 261.0, 270.0]</t>
-  </si>
-  <si>
-    <t>[-2.0, -6.0, 177.0, -99.0, 164.0, -59.0, 6.0, 79.0, 139.0, 188.0, 25.0, 57.0, -2.0, 222.0, 326.0, 142.0]</t>
-  </si>
-  <si>
-    <t>[205.0, 336.0, 244.0, 171.0, 426.0, 295.0, 210.0, 340.0, 390.0, 194.0, 252.0, 305.0, 348.0, 381.0, 293.0, 290.0]</t>
-  </si>
-  <si>
-    <t>[296.0, 324.0, 423.0, 357.0, 237.0, 239.0, 354.0, 294.0, 320.0, 288.0, 270.0, 328.0, 316.0, 288.0, 259.0, 285.0]</t>
-  </si>
-  <si>
-    <t>[440.0, 683.0, 761.0, 705.0, 633.0, 416.0, 516.0, 594.0, 685.0, 362.0, 435.0, 330.0, 709.0, 351.0, 397.0, 442.0]</t>
-  </si>
-  <si>
-    <t>[495.0, 374.0, 405.0, 280.0, 273.0, 298.0, 224.0, 516.0, 331.0, 364.0, 306.0, 285.0, 379.0, 191.0, 306.0, 447.0]</t>
-  </si>
-  <si>
-    <t>[401.0, 377.0, 366.0, 380.0, 338.0, 351.0, 339.0, 292.0, 279.0, 311.0, 302.0, 313.0, 293.0, 266.0, 282.0, 266.0]</t>
-  </si>
-  <si>
-    <t>[259.0, 317.0, 193.0, 258.0, 270.0, 278.0, 268.0, 243.0, 214.0, 155.0, 232.0, 247.0, 188.0, 167.0, 183.0, 224.0]</t>
-  </si>
-  <si>
-    <t>[217.0, 176.0, 154.0, 199.0, 194.0, 266.0, 215.0, 92.0, 66.0, 85.0, 258.0, 194.0, 195.0, 115.0, 145.0, 142.0]</t>
-  </si>
-  <si>
-    <t>[250.0, 320.0, 310.0, 336.0, 279.0, 367.0, 312.0, 218.0, 145.0, 239.0, 204.0, 191.0, 138.0, 282.0, 280.0, 331.0]</t>
-  </si>
-  <si>
-    <t>[99.0, 215.0, 64.0, 227.0, 212.0, 118.0, 104.0, -55.0, 144.0, 73.0, 25.0, 141.0, 123.0, -49.0, 37.0, 42.0]</t>
-  </si>
-  <si>
-    <t>[269.0, 211.0, 322.0, 195.0, 255.0, 260.0, 222.0, 203.0, 253.0, 257.0, 285.0, 277.0, 209.0, 188.0, 259.0, 267.0]</t>
-  </si>
-  <si>
-    <t>[201.0, 178.0, 200.0, 312.0, 185.0, 241.0, 211.0, 118.0, 181.0, 250.0, 225.0, 212.0, 249.0, 236.0, 128.0, 197.0]</t>
-  </si>
-  <si>
-    <t>[91.0, 7.0, -15.0, 6.0, 54.0, 5.0, -22.0, 66.0, -38.0, 47.0, 0.0, 109.0, 45.0, 60.0, 143.0, 33.0]</t>
-  </si>
-  <si>
-    <t>[61.0, 35.0, 155.0, 81.0, 53.0, 160.0, 11.0, 104.0, 77.0, 90.0, 33.0, 10.0, 21.0, 98.0, 31.0, 50.0]</t>
-  </si>
-  <si>
-    <t>[667.0, 704.0, 752.0, 742.0, 764.0, 754.0, 871.0, 755.0, 700.0, 756.0, 734.0, 649.0, 833.0, 685.0, 716.0, 684.0]</t>
-  </si>
-  <si>
-    <t>[440.0, 352.0, 467.0, 197.0, 325.0, 420.0, 419.0, 253.0, 434.0, 485.0, 366.0, 402.0, 558.0, 394.0, 455.0, 206.0]</t>
-  </si>
-  <si>
-    <t>[301.0, 267.0, 221.0, 237.0, 244.0, 203.0, 275.0, 240.0, 203.0, 232.0, 202.0, 223.0, 206.0, 207.0, 227.0, 196.0]</t>
-  </si>
-  <si>
-    <t>[350.0, 206.0, 204.0, 261.0, 266.0, 238.0, 311.0, 265.0, 297.0, 312.0, 189.0, 277.0, 313.0, 249.0, 276.0, 233.0]</t>
-  </si>
-  <si>
-    <t>[166.0, 152.0, 145.0, 120.0, 140.0, 88.0, 207.0, 89.0, 93.0, 149.0, 123.0, 91.0, 96.0, 96.0, 141.0, 86.0]</t>
-  </si>
-  <si>
-    <t>[134.0, 135.0, 72.0, 143.0, 124.0, 107.0, 72.0, 60.0, 73.0, 88.0, 75.0, 101.0, 60.0, 101.0, 131.0, 79.0]</t>
-  </si>
-  <si>
-    <t>[255.0, 308.0, 349.0, 207.0, 324.0, 326.0, 188.0, 366.0, 213.0, 236.0, 141.0, 302.0, 253.0, 146.0, 219.0, 204.0]</t>
-  </si>
-  <si>
-    <t>[154.0, 218.0, 188.0, 146.0, 154.0, 234.0, 170.0, 139.0, 143.0, 185.0, 174.0, 188.0, 209.0, 150.0, 174.0, 189.0]</t>
-  </si>
-  <si>
-    <t>[237.0, 315.0, 345.0, 181.0, 208.0, 229.0, 173.0, 229.0, 244.0, 226.0, 155.0, 197.0, 154.0, 267.0, 172.0, 199.0]</t>
-  </si>
-  <si>
-    <t>[381.0, 394.0, 257.0, 306.0, 274.0, 290.0, 8.0, 100.0, 325.0, 479.0, 267.0, 284.0, 161.0, 114.0, 252.0, 169.0]</t>
-  </si>
-  <si>
-    <t>[836.0, 518.0, 867.0, 382.0, 756.0, 590.0, 681.0, 408.0, 660.0, 686.0, 681.0, 734.0, 518.0, 728.0, 896.0, 688.0]</t>
-  </si>
-  <si>
-    <t>[115.0, 117.0, 118.0, 124.0, 114.0, 150.0, 103.0, 47.0, 162.0, 55.0, 157.0, 122.0, 103.0, 81.0, 136.0, 119.0]</t>
-  </si>
-  <si>
-    <t>[-92.0, 216.0, 237.0, 293.0, 60.0, 122.0, 101.0, 43.0, 161.0, 134.0, 192.0, 246.0, 5.0, 111.0, 53.0, 72.0]</t>
-  </si>
-  <si>
-    <t>[171.0, 363.0, 220.0, 198.0, 216.0, 50.0, 219.0, 90.0, 82.0, 125.0, 112.0, 205.0, 63.0, 184.0, 125.0, 151.0]</t>
-  </si>
-  <si>
-    <t>[130.0, 107.0, 108.0, 122.0, 122.0, 103.0, 108.0, 118.0, 120.0, 106.0, 119.0, 109.0, 104.0, 99.0, 102.0, 97.0]</t>
-  </si>
-  <si>
-    <t>[113.0, 64.0, 83.0, 87.0, 68.0, 60.0, 52.0, 38.0, 50.0, 80.0, 53.0, 75.0, 85.0, 14.0, 51.0, 73.0]</t>
-  </si>
-  <si>
-    <t>[45.0, 90.0, 36.0, 69.0, 62.0, 49.0, 63.0, 56.0, 61.0, 89.0, 61.0, 84.0, 76.0, 21.0, 37.0, 66.0]</t>
-  </si>
-  <si>
-    <t>[309.0, 204.0, 166.0, 196.0, 269.0, 181.0, 183.0, 195.0, 194.0, 199.0, 200.0, 166.0, 180.0, 215.0, 176.0, 161.0]</t>
-  </si>
-  <si>
-    <t>[165.0, 156.0, 121.0, 93.0, 68.0, 130.0, 125.0, 136.0, 99.0, 103.0, 120.0, 108.0, 110.0, 101.0, 96.0, 150.0]</t>
-  </si>
-  <si>
-    <t>[315.0, 39.0, 70.0, -8.0, 300.0, 151.0, 201.0, 10.0, 220.0, 166.0, 198.0, 116.0, 126.0, 111.0, 4.0, 39.0]</t>
-  </si>
-  <si>
-    <t>[130.0, 68.0, 81.0, 77.0, 75.0, 49.0, 36.0, 70.0, 56.0, 58.0, 62.0, 59.0, 82.0, 103.0, 53.0, 81.0]</t>
-  </si>
-  <si>
-    <t>[60.0, 43.0, 57.0, 67.0, 44.0, 37.0, 44.0, 39.0, 36.0, 38.0, 56.0, 40.0, 34.0, 34.0, 45.0, 47.0]</t>
-  </si>
-  <si>
-    <t>[81.0, 45.0, 38.0, 27.0, 11.0, 29.0, 42.0, 43.0, 20.0, 29.0, 41.0, 36.0, 37.0, 36.0, 37.0, 31.0]</t>
-  </si>
-  <si>
-    <t>[40.0, 39.0, 19.0, 26.0, 10.0, 12.0, 51.0, 20.0, 23.0, 18.0, 30.0, 32.0, 10.0, 6.0, -4.0, 24.0]</t>
-  </si>
-  <si>
-    <t>[41.0, 85.0, 203.0, 76.0, 175.0, 111.0, 99.0, 88.0, 128.0, 142.0, 139.0, 147.0, 103.0, 5.0, 90.0, 105.0]</t>
-  </si>
-  <si>
-    <t>[73.0, 58.0, 63.0, 90.0, 86.0, 49.0, 60.0, 77.0, 69.0, 56.0, 69.0, 55.0, 53.0, 52.0, 72.0, 67.0]</t>
-  </si>
-  <si>
-    <t>[127.0, 110.0, 94.0, 98.0, 104.0, 88.0, 94.0, 96.0, 102.0, 100.0, 105.0, 96.0, 82.0, 84.0, 77.0, 92.0]</t>
-  </si>
-  <si>
-    <t>[116.0, 93.0, 88.0, 118.0, 125.0, 99.0, 103.0, 96.0, 94.0, 93.0, 96.0, 87.0, 72.0, 78.0, 82.0, 71.0]</t>
-  </si>
-  <si>
-    <t>[102.0, 69.0, 70.0, 68.0, 4.0, 61.0, 30.0, 81.0, 79.0, 73.0, 65.0, 82.0, 56.0, 62.0, 78.0, 54.0]</t>
-  </si>
-  <si>
-    <t>[121.0, 109.0, 131.0, 122.0, 152.0, 85.0, 141.0, 140.0, 87.0, 131.0, 150.0, 176.0, 118.0, 101.0, 120.0, 106.0]</t>
-  </si>
-  <si>
-    <t>[150.0, 162.0, 156.0, 150.0, 146.0, 141.0, 158.0, 136.0, 139.0, 147.0, 155.0, 164.0, 158.0, 170.0, 157.0, 156.0]</t>
-  </si>
-  <si>
-    <t>[298.0, 325.0, 314.0, 302.0, 271.0, 269.0, 317.0, 255.0, 289.0, 268.0, 280.0, 298.0, 274.0, 279.0, 283.0, 279.0]</t>
-  </si>
-  <si>
-    <t>[239.0, 252.0, 227.0, 211.0, 198.0, 166.0, 194.0, 160.0, 204.0, 173.0, 225.0, 208.0, 196.0, 198.0, 232.0, 209.0]</t>
-  </si>
-  <si>
-    <t>[5.0, 71.0, 72.0, 66.0, 25.0, 47.0, 32.0, 38.0, 34.0, 61.0, 50.0, 65.0, 60.0, 67.0, 67.0, 24.0]</t>
-  </si>
-  <si>
-    <t>[221.0, 181.0, 216.0, 200.0, 207.0, 234.0, 242.0, 154.0, 230.0, 181.0, 183.0, 229.0, 192.0, 205.0, 211.0, 217.0]</t>
-  </si>
-  <si>
-    <t>[-103.0, 13.0, 35.0, 426.0, 170.0, 137.0, 103.0, 189.0, 59.0, 354.0, 75.0, 217.0, 227.0, 287.0, 299.0, 286.0]</t>
-  </si>
-  <si>
-    <t>[239.0, 263.0, 490.0, 311.0, 248.0, 296.0, 385.0, 368.0, 324.0, 168.0, 342.0, 315.0, 237.0, 284.0, 355.0, 372.0]</t>
-  </si>
-  <si>
-    <t>[412.0, 430.0, 376.0, 448.0, 220.0, 247.0, 167.0, 196.0, 261.0, 189.0, 116.0, 226.0, 312.0, 271.0, 135.0, 101.0]</t>
-  </si>
-  <si>
-    <t>[230.0, 266.0, 268.0, 149.0, 247.0, 272.0, 339.0, 92.0, 141.0, 250.0, 218.0, 192.0, 258.0, 223.0, 141.0, 272.0]</t>
-  </si>
-  <si>
-    <t>[381.0, 341.0, 442.0, 317.0, 265.0, 172.0, 351.0, 316.0, 295.0, 194.0, 270.0, 326.0, 319.0, 273.0, 171.0, 345.0]</t>
-  </si>
-  <si>
-    <t>[27.0, 44.0, 39.0, 47.0, 64.0, 45.0, 71.0, 53.0, 44.0, 55.0, 61.0, 49.0, 62.0, 72.0, 65.0, 71.0]</t>
-  </si>
-  <si>
-    <t>[39.0, 27.0, 74.0, -2.0, 72.0, 81.0, 68.0, -2.0, 49.0, 44.0, 42.0, 65.0, 25.0, 29.0, 21.0, 83.0]</t>
-  </si>
-  <si>
-    <t>[9.0, 75.0, 53.0, 86.0, 92.0, 23.0, 99.0, 59.0, 28.0, 30.0, 39.0, 87.0, 82.0, 119.0, 67.0, 57.0]</t>
-  </si>
-  <si>
-    <t>[-13.0, 53.0, 19.0, 50.0, 84.0, 73.0, 80.0, 1.0, 18.0, 21.0, 35.0, 23.0, 95.0, 41.0, -9.0, 54.0]</t>
-  </si>
-  <si>
-    <t>[201.0, 62.0, 63.0, 104.0, 95.0, 130.0, 191.0, 102.0, 97.0, 133.0, 144.0, 98.0, 115.0, 57.0, 185.0, 61.0]</t>
-  </si>
-  <si>
-    <t>[175.0, 109.0, 89.0, 167.0, 174.0, 134.0, 119.0, 125.0, 55.0, 36.0, 136.0, 130.0, 116.0, 141.0, 91.0, 17.0]</t>
-  </si>
-  <si>
-    <t>[214.0, 245.0, 170.0, 246.0, 286.0, 174.0, 181.0, 194.0, 160.0, 284.0, 172.0, 227.0, 200.0, 117.0, 154.0, 121.0]</t>
-  </si>
-  <si>
-    <t>[64.0, 20.0, 19.0, 38.0, 27.0, 23.0, 55.0, 28.0, 35.0, 13.0, 43.0, 14.0, 51.0, 54.0, 43.0, 33.0]</t>
-  </si>
-  <si>
-    <t>[-12.0, 33.0, 7.0, 31.0, -10.0, 19.0, 32.0, -13.0, -24.0, 6.0, 4.0, 7.0, 32.0, 39.0, 18.0, 22.0]</t>
-  </si>
-  <si>
-    <t>[150.0, 117.0, 123.0, 103.0, 126.0, 95.0, 138.0, 106.0, 68.0, 47.0, 122.0, 97.0, -25.0, 95.0, 48.0, 42.0]</t>
-  </si>
-  <si>
-    <t>[-31.0, 110.0, 59.0, -13.0, 36.0, 24.0, 7.0, 118.0, 35.0, 53.0, 20.0, 34.0, 30.0, 82.0, 24.0, 0.0]</t>
-  </si>
-  <si>
-    <t>[196.0, 230.0, 214.0, 190.0, 255.0, 179.0, 199.0, 225.0, 189.0, 185.0, 98.0, 135.0, 142.0, 142.0, 173.0, 164.0]</t>
-  </si>
-  <si>
-    <t>[119.0, 114.0, 79.0, 40.0, 82.0, 104.0, 80.0, 74.0, 69.0, 56.0, 35.0, 34.0, 59.0, 61.0, 45.0, 66.0]</t>
-  </si>
-  <si>
-    <t>[24.0, -6.0, 147.0, 47.0, 66.0, 82.0, 18.0, 106.0, 64.0, 46.0, -59.0, 75.0, 88.0, 126.0, 102.0, 105.0]</t>
-  </si>
-  <si>
-    <t>[113.0, 147.0, 80.0, 81.0, 99.0, 114.0, 52.0, 56.0, 116.0, 143.0, -5.0, 24.0, 47.0, 15.0, 96.0, 46.0]</t>
-  </si>
-  <si>
-    <t>[201.0, 191.0, 173.0, 192.0, 185.0, 176.0, 182.0, 166.0, 167.0, 176.0, 175.0, 179.0, 175.0, 171.0, 172.0, 163.0]</t>
-  </si>
-  <si>
-    <t>[218.0, 205.0, 196.0, 210.0, 209.0, 199.0, 199.0, 184.0, 183.0, 206.0, 195.0, 198.0, 189.0, 185.0, 192.0, 177.0]</t>
-  </si>
-  <si>
-    <t>[188.0, 95.0, 64.0, 22.0, 92.0, 32.0, 100.0, 142.0, 141.0, 125.0, 147.0, 96.0, 136.0, 87.0, 118.0, 106.0]</t>
-  </si>
-  <si>
-    <t>[189.0, 216.0, 250.0, 261.0, 242.0, 252.0, 254.0, 251.0, 243.0, 241.0, 238.0, 229.0, 217.0, 193.0, 189.0, 209.0]</t>
-  </si>
-  <si>
-    <t>[106.0, 82.0, 149.0, 123.0, 45.0, 108.0, 122.0, 84.0, 55.0, 82.0, 100.0, 97.0, 67.0, 68.0, 69.0, 68.0]</t>
-  </si>
-  <si>
-    <t>[186.0, 196.0, 145.0, 185.0, 154.0, 148.0, 163.0, 144.0, 171.0, 146.0, 160.0, 172.0, 167.0, 162.0, 139.0, 137.0]</t>
-  </si>
-  <si>
-    <t>[136.0, 154.0, 102.0, 109.0, 34.0, 41.0, 136.0, 66.0, 158.0, 78.0, 98.0, 64.0, 113.0, 120.0, 148.0, 66.0]</t>
-  </si>
-  <si>
-    <t>[270.0, 218.0, 157.0, 119.0, 194.0, 155.0, 199.0, 201.0, 199.0, 178.0, 167.0, 173.0, 215.0, 158.0, 137.0, 132.0]</t>
-  </si>
-  <si>
-    <t>[79.0, 95.0, 71.0, 92.0, 70.0, 103.0, 43.0, 104.0, 89.0, 90.0, 91.0, 68.0, 72.0, 63.0, 55.0, 60.0]</t>
-  </si>
-  <si>
-    <t>[32.0, 38.0, 31.0, 38.0, 64.0, 18.0, 32.0, -1.0, 24.0, 64.0, 42.0, 52.0, 49.0, 48.0, 40.0, -5.0]</t>
-  </si>
-  <si>
-    <t>[886.0, 860.0, 832.0, 809.0, 791.0, 776.0, 768.0, 756.0, 747.0, 739.0, 722.0, 695.0, 671.0, 651.0, 638.0, 620.0]</t>
-  </si>
-  <si>
-    <t>[1246.0, 1224.0, 1188.0, 1158.0, 1137.0, 1132.0, 1108.0, 1082.0, 1063.0, 1044.0, 1025.0, 996.0, 967.0, 937.0, 918.0, 887.0]</t>
-  </si>
-  <si>
-    <t>[1355.0, 1327.0, 1284.0, 1258.0, 1227.0, 1208.0, 1171.0, 1160.0, 1155.0, 1138.0, 1128.0, 1080.0, 1045.0, 997.0, 965.0, 961.0]</t>
-  </si>
-  <si>
-    <t>[1429.0, 1392.0, 1370.0, 1351.0, 1295.0, 1285.0, 1248.0, 1237.0, 1230.0, 1208.0, 1204.0, 1161.0, 1127.0, 1083.0, 1052.0, 1023.0]</t>
-  </si>
-  <si>
-    <t>[2291.0, 2296.0, 2303.0, 2041.0, 2023.0, 2069.0, 2060.0, 1963.0, 1949.0, 1916.0, 1903.0, 1882.0, 1875.0, 1834.0, 1663.0, 1558.0]</t>
-  </si>
-  <si>
-    <t>[1338.0, 1328.0, 1266.0, 1260.0, 1276.0, 1370.0, 1264.0, 1191.0, 1237.0, 1270.0, 1229.0, 1221.0, 1165.0, 1099.0, 1129.0, 1136.0]</t>
-  </si>
-  <si>
-    <t>[1567.0, 1509.0, 1468.0, 1462.0, 1405.0, 1389.0, 1396.0, 1408.0, 1335.0, 1330.0, 1345.0, 1319.0, 1316.0, 1235.0, 1213.0, 1127.0]</t>
-  </si>
-  <si>
-    <t>[1877.0, 1843.0, 1738.0, 1728.0, 1730.0, 1728.0, 1672.0, 1579.0, 1600.0, 1726.0, 1576.0, 1553.0, 1435.0, 1428.0, 1439.0, 1401.0]</t>
-  </si>
-  <si>
-    <t>[1466.0, 1412.0, 1423.0, 1408.0, 1325.0, 1236.0, 1169.0, 1166.0, 1227.0, 1149.0, 1134.0, 1078.0, 1087.0, 1061.0, 986.0, 1004.0]</t>
-  </si>
-  <si>
-    <t>[1381.0, 1448.0, 1340.0, 1365.0, 1382.0, 1327.0, 1271.0, 1331.0, 1308.0, 1234.0, 1233.0, 1208.0, 1052.0, 1083.0, 1051.0, 971.0]</t>
-  </si>
-  <si>
-    <t>[1362.0, 1271.0, 1274.0, 1348.0, 1329.0, 1358.0, 1319.0, 1242.0, 1272.0, 1176.0, 1139.0, 1240.0, 1045.0, 1099.0, 1092.0, 1108.0]</t>
-  </si>
-  <si>
-    <t>[1381.0, 1367.0, 1381.0, 1423.0, 1272.0, 1259.0, 1255.0, 1228.0, 1202.0, 1208.0, 1170.0, 1131.0, 1125.0, 1114.0, 1019.0, 981.0]</t>
-  </si>
-  <si>
-    <t>[809.0, 753.0, 739.0, 742.0, 704.0, 701.0, 689.0, 660.0, 709.0, 668.0, 676.0, 645.0, 622.0, 651.0, 657.0, 648.0]</t>
-  </si>
-  <si>
-    <t>[1408.0, 1319.0, 1402.0, 1210.0, 1266.0, 1258.0, 1280.0, 1252.0, 1251.0, 1211.0, 1170.0, 1136.0, 1148.0, 1089.0, 973.0, 986.0]</t>
-  </si>
-  <si>
-    <t>[1018.0, 957.0, 959.0, 914.0, 919.0, 862.0, 907.0, 921.0, 869.0, 887.0, 847.0, 787.0, 753.0, 724.0, 681.0, 722.0]</t>
-  </si>
-  <si>
-    <t>[1141.0, 1136.0, 1079.0, 1022.0, 1008.0, 1042.0, 947.0, 1045.0, 968.0, 959.0, 965.0, 962.0, 862.0, 838.0, 819.0, 788.0]</t>
-  </si>
-  <si>
-    <t>[1216.0, 1174.0, 1161.0, 1137.0, 1107.0, 1091.0, 1058.0, 1038.0, 1036.0, 996.0, 974.0, 941.0, 930.0, 871.0, 847.0, 842.0]</t>
-  </si>
-  <si>
-    <t>[878.0, 886.0, 838.0, 926.0, 859.0, 899.0, 850.0, 882.0, 798.0, 884.0, 816.0, 750.0, 769.0, 802.0, 808.0, 737.0]</t>
-  </si>
-  <si>
-    <t>[1532.0, 1499.0, 1476.0, 1431.0, 1470.0, 1450.0, 1452.0, 1355.0, 1335.0, 1247.0, 1255.0, 1200.0, 1253.0, 1229.0, 1017.0, 1115.0]</t>
-  </si>
-  <si>
-    <t>[1209.0, 1173.0, 1153.0, 1132.0, 1072.0, 1109.0, 1110.0, 1056.0, 1065.0, 1003.0, 981.0, 968.0, 940.0, 887.0, 851.0, 862.0]</t>
-  </si>
-  <si>
-    <t>[1473.0, 1425.0, 1404.0, 1419.0, 1337.0, 1424.0, 1327.0, 1239.0, 1381.0, 1255.0, 1194.0, 1204.0, 1217.0, 1134.0, 1062.0, 1094.0]</t>
-  </si>
-  <si>
-    <t>[1168.0, 1070.0, 1054.0, 997.0, 997.0, 970.0, 934.0, 1024.0, 948.0, 901.0, 916.0, 938.0, 919.0, 861.0, 799.0, 786.0]</t>
-  </si>
-  <si>
-    <t>[1176.0, 1160.0, 1141.0, 1112.0, 1078.0, 1071.0, 1053.0, 1029.0, 1008.0, 994.0, 980.0, 951.0, 928.0, 902.0, 883.0, 845.0]</t>
-  </si>
-  <si>
-    <t>[1539.0, 1465.0, 1443.0, 1428.0, 1368.0, 1365.0, 1349.0, 1305.0, 1289.0, 1253.0, 1242.0, 1229.0, 1166.0, 1132.0, 1114.0, 1049.0]</t>
-  </si>
-  <si>
-    <t>[1591.0, 1483.0, 1398.0, 1438.0, 1409.0, 1372.0, 1324.0, 1277.0, 1218.0, 1243.0, 1218.0, 1232.0, 1147.0, 1086.0, 1118.0, 1065.0]</t>
-  </si>
-  <si>
-    <t>[1864.0, 1792.0, 1776.0, 1682.0, 1693.0, 1643.0, 1591.0, 1558.0, 1549.0, 1493.0, 1529.0, 1455.0, 1371.0, 1401.0, 1350.0, 1242.0]</t>
-  </si>
-  <si>
-    <t>[1085.0, 1068.0, 1060.0, 1079.0, 966.0, 980.0, 960.0, 915.0, 949.0, 915.0, 893.0, 877.0, 834.0, 823.0, 840.0, 748.0]</t>
-  </si>
-  <si>
-    <t>[1484.0, 1478.0, 1482.0, 1424.0, 1377.0, 1365.0, 1337.0, 1315.0, 1255.0, 1266.0, 1244.0, 1213.0, 1155.0, 1105.0, 1098.0, 1053.0]</t>
-  </si>
-  <si>
-    <t>[1270.0, 1286.0, 1209.0, 1206.0, 1168.0, 1152.0, 1134.0, 1108.0, 1062.0, 1059.0, 1035.0, 1053.0, 984.0, 965.0, 957.0, 891.0]</t>
-  </si>
-  <si>
-    <t>[941.0, 897.0, 904.0, 904.0, 849.0, 885.0, 848.0, 828.0, 808.0, 761.0, 787.0, 760.0, 733.0, 740.0, 735.0, 666.0]</t>
-  </si>
-  <si>
-    <t>[907.0, 906.0, 906.0, 877.0, 844.0, 845.0, 847.0, 817.0, 799.0, 787.0, 784.0, 757.0, 732.0, 700.0, 698.0, 692.0]</t>
-  </si>
-  <si>
-    <t>[1467.0, 1443.0, 1431.0, 1391.0, 1271.0, 1253.0, 1328.0, 1277.0, 1213.0, 1200.0, 1174.0, 1148.0, 1144.0, 1052.0, 1070.0, 1051.0]</t>
-  </si>
-  <si>
-    <t>[1947.0, 1901.0, 1897.0, 1886.0, 1807.0, 1880.0, 1909.0, 1774.0, 1757.0, 1757.0, 1751.0, 1591.0, 1728.0, 1609.0, 1561.0, 1560.0]</t>
-  </si>
-  <si>
-    <t>[1002.0, 1002.0, 984.0, 956.0, 953.0, 937.0, 915.0, 919.0, 913.0, 887.0, 866.0, 841.0, 819.0, 798.0, 781.0, 754.0]</t>
-  </si>
-  <si>
-    <t>[1439.0, 1312.0, 1247.0, 1258.0, 1256.0, 1172.0, 1216.0, 1209.0, 1166.0, 1169.0, 1149.0, 1131.0, 1058.0, 1072.0, 1034.0, 982.0]</t>
-  </si>
-  <si>
-    <t>[1010.0, 1023.0, 1009.0, 974.0, 980.0, 954.0, 942.0, 947.0, 946.0, 918.0, 890.0, 863.0, 838.0, 826.0, 806.0, 767.0]</t>
-  </si>
-  <si>
-    <t>[1141.0, 1139.0, 1111.0, 1066.0, 1037.0, 1031.0, 1009.0, 1015.0, 987.0, 978.0, 949.0, 944.0, 919.0, 878.0, 885.0, 856.0]</t>
-  </si>
-  <si>
-    <t>[957.0, 897.0, 938.0, 896.0, 846.0, 905.0, 785.0, 858.0, 789.0, 796.0, 858.0, 766.0, 805.0, 728.0, 776.0, 681.0]</t>
-  </si>
-  <si>
-    <t>[1086.0, 1066.0, 1040.0, 1001.0, 956.0, 988.0, 969.0, 929.0, 920.0, 888.0, 882.0, 829.0, 841.0, 819.0, 768.0, 745.0]</t>
-  </si>
-  <si>
-    <t>[1060.0, 1012.0, 1086.0, 993.0, 921.0, 961.0, 953.0, 950.0, 890.0, 836.0, 811.0, 776.0, 778.0, 816.0, 714.0, 727.0]</t>
-  </si>
-  <si>
-    <t>[2071.0, 1923.0, 1924.0, 1920.0, 1995.0, 1960.0, 1877.0, 1917.0, 1880.0, 1841.0, 1883.0, 1838.0, 1640.0, 1557.0, 1578.0, 1477.0]</t>
-  </si>
-  <si>
-    <t>[2001.0, 1918.0, 1916.0, 1824.0, 1661.0, 1885.0, 1887.0, 1860.0, 1975.0, 1738.0, 1731.0, 1475.0, 1602.0, 1547.0, 1660.0, 1405.0]</t>
-  </si>
-  <si>
-    <t>[1167.0, 1150.0, 1154.0, 1116.0, 1090.0, 1099.0, 1097.0, 1039.0, 1055.0, 1039.0, 1022.0, 984.0, 978.0, 935.0, 904.0, 899.0]</t>
-  </si>
-  <si>
-    <t>[893.0, 890.0, 887.0, 901.0, 824.0, 891.0, 869.0, 861.0, 880.0, 829.0, 783.0, 844.0, 793.0, 750.0, 727.0, 751.0]</t>
-  </si>
-  <si>
-    <t>[1140.0, 1162.0, 1041.0, 964.0, 991.0, 919.0, 961.0, 981.0, 980.0, 921.0, 957.0, 916.0, 843.0, 873.0, 884.0, 759.0]</t>
-  </si>
-  <si>
-    <t>[569.0, 544.0, 523.0, 509.0, 505.0, 493.0, 485.0, 486.0, 479.0, 470.0, 475.0, 454.0, 422.0, 413.0, 411.0, 403.0]</t>
-  </si>
-  <si>
-    <t>[561.0, 542.0, 525.0, 498.0, 498.0, 491.0, 482.0, 487.0, 471.0, 472.0, 465.0, 454.0, 423.0, 410.0, 407.0, 400.0]</t>
-  </si>
-  <si>
-    <t>[516.0, 500.0, 503.0, 467.0, 472.0, 457.0, 451.0, 453.0, 434.0, 438.0, 429.0, 423.0, 400.0, 388.0, 388.0, 377.0]</t>
-  </si>
-  <si>
-    <t>[848.0, 852.0, 809.0, 796.0, 833.0, 783.0, 791.0, 757.0, 747.0, 747.0, 748.0, 719.0, 693.0, 678.0, 700.0, 630.0]</t>
-  </si>
-  <si>
-    <t>[742.0, 771.0, 749.0, 754.0, 730.0, 683.0, 722.0, 682.0, 685.0, 688.0, 695.0, 648.0, 613.0, 605.0, 622.0, 629.0]</t>
-  </si>
-  <si>
-    <t>[1092.0, 1015.0, 1004.0, 1002.0, 1018.0, 1007.0, 979.0, 947.0, 961.0, 951.0, 893.0, 891.0, 866.0, 826.0, 844.0, 764.0]</t>
-  </si>
-  <si>
-    <t>[596.0, 596.0, 585.0, 567.0, 569.0, 532.0, 528.0, 519.0, 507.0, 507.0, 516.0, 510.0, 487.0, 481.0, 457.0, 445.0]</t>
-  </si>
-  <si>
-    <t>[501.0, 484.0, 465.0, 441.0, 439.0, 416.0, 410.0, 409.0, 406.0, 398.0, 402.0, 385.0, 371.0, 356.0, 360.0, 349.0]</t>
-  </si>
-  <si>
-    <t>[486.0, 466.0, 444.0, 416.0, 413.0, 402.0, 389.0, 390.0, 393.0, 389.0, 390.0, 365.0, 363.0, 336.0, 341.0, 334.0]</t>
-  </si>
-  <si>
-    <t>[463.0, 425.0, 419.0, 402.0, 406.0, 387.0, 383.0, 384.0, 381.0, 376.0, 352.0, 349.0, 330.0, 321.0, 321.0, 320.0]</t>
-  </si>
-  <si>
-    <t>[581.0, 554.0, 602.0, 521.0, 522.0, 513.0, 460.0, 545.0, 484.0, 494.0, 502.0, 479.0, 445.0, 420.0, 426.0, 408.0]</t>
-  </si>
-  <si>
-    <t>[496.0, 493.0, 470.0, 451.0, 436.0, 413.0, 411.0, 407.0, 401.0, 383.0, 391.0, 380.0, 363.0, 352.0, 348.0, 335.0]</t>
-  </si>
-  <si>
-    <t>[551.0, 522.0, 510.0, 486.0, 480.0, 475.0, 465.0, 465.0, 446.0, 444.0, 431.0, 422.0, 406.0, 394.0, 385.0, 390.0]</t>
-  </si>
-  <si>
-    <t>[571.0, 539.0, 526.0, 507.0, 502.0, 487.0, 484.0, 489.0, 463.0, 473.0, 460.0, 434.0, 415.0, 408.0, 405.0, 402.0]</t>
-  </si>
-  <si>
-    <t>[467.0, 450.0, 441.0, 416.0, 401.0, 413.0, 399.0, 399.0, 387.0, 377.0, 378.0, 366.0, 355.0, 335.0, 331.0, 323.0]</t>
-  </si>
-  <si>
-    <t>[544.0, 520.0, 505.0, 498.0, 487.0, 481.0, 468.0, 453.0, 455.0, 440.0, 475.0, 434.0, 407.0, 409.0, 402.0, 391.0]</t>
-  </si>
-  <si>
-    <t>[742.0, 718.0, 698.0, 673.0, 666.0, 659.0, 655.0, 638.0, 631.0, 624.0, 614.0, 598.0, 589.0, 575.0, 558.0, 545.0]</t>
-  </si>
-  <si>
-    <t>[798.0, 763.0, 744.0, 716.0, 705.0, 708.0, 689.0, 670.0, 666.0, 665.0, 656.0, 643.0, 628.0, 622.0, 604.0, 598.0]</t>
-  </si>
-  <si>
-    <t>[795.0, 764.0, 743.0, 711.0, 696.0, 709.0, 711.0, 676.0, 676.0, 688.0, 669.0, 647.0, 639.0, 631.0, 613.0, 611.0]</t>
-  </si>
-  <si>
-    <t>[465.0, 438.0, 414.0, 415.0, 394.0, 392.0, 376.0, 383.0, 376.0, 378.0, 360.0, 356.0, 344.0, 336.0, 322.0, 319.0]</t>
-  </si>
-  <si>
-    <t>[657.0, 615.0, 623.0, 590.0, 596.0, 598.0, 576.0, 545.0, 527.0, 523.0, 521.0, 513.0, 494.0, 494.0, 496.0, 488.0]</t>
-  </si>
-  <si>
-    <t>[998.0, 887.0, 1023.0, 925.0, 942.0, 938.0, 909.0, 893.0, 861.0, 940.0, 838.0, 741.0, 830.0, 870.0, 772.0, 670.0]</t>
-  </si>
-  <si>
-    <t>[859.0, 897.0, 839.0, 815.0, 765.0, 838.0, 827.0, 807.0, 741.0, 760.0, 767.0, 747.0, 752.0, 742.0, 726.0, 743.0]</t>
-  </si>
-  <si>
-    <t>[1230.0, 1147.0, 1040.0, 966.0, 948.0, 948.0, 935.0, 887.0, 899.0, 850.0, 926.0, 854.0, 843.0, 814.0, 800.0, 826.0]</t>
-  </si>
-  <si>
-    <t>[1161.0, 1157.0, 1047.0, 1020.0, 1015.0, 1042.0, 1064.0, 991.0, 958.0, 939.0, 986.0, 933.0, 938.0, 920.0, 867.0, 885.0]</t>
-  </si>
-  <si>
-    <t>[1019.0, 953.0, 983.0, 837.0, 852.0, 809.0, 789.0, 812.0, 820.0, 820.0, 794.0, 851.0, 766.0, 773.0, 744.0, 695.0]</t>
-  </si>
-  <si>
-    <t>[717.0, 701.0, 679.0, 656.0, 651.0, 638.0, 643.0, 623.0, 619.0, 612.0, 601.0, 581.0, 572.0, 550.0, 535.0, 523.0]</t>
-  </si>
-  <si>
-    <t>[742.0, 719.0, 722.0, 692.0, 665.0, 677.0, 677.0, 655.0, 630.0, 633.0, 606.0, 606.0, 584.0, 555.0, 543.0, 515.0]</t>
-  </si>
-  <si>
-    <t>[683.0, 654.0, 640.0, 621.0, 627.0, 621.0, 608.0, 588.0, 596.0, 592.0, 577.0, 541.0, 554.0, 524.0, 516.0, 514.0]</t>
-  </si>
-  <si>
-    <t>[605.0, 602.0, 583.0, 575.0, 540.0, 536.0, 531.0, 520.0, 530.0, 517.0, 503.0, 482.0, 472.0, 466.0, 462.0, 449.0]</t>
-  </si>
-  <si>
-    <t>[783.0, 710.0, 704.0, 698.0, 710.0, 676.0, 648.0, 651.0, 664.0, 657.0, 653.0, 602.0, 596.0, 584.0, 586.0, 551.0]</t>
-  </si>
-  <si>
-    <t>[931.0, 944.0, 981.0, 954.0, 966.0, 964.0, 990.0, 979.0, 936.0, 936.0, 908.0, 896.0, 858.0, 832.0, 791.0, 777.0]</t>
-  </si>
-  <si>
-    <t>[870.0, 911.0, 853.0, 838.0, 837.0, 745.0, 858.0, 812.0, 754.0, 717.0, 750.0, 746.0, 678.0, 694.0, 686.0, 634.0]</t>
-  </si>
-  <si>
-    <t>[632.0, 611.0, 596.0, 591.0, 592.0, 539.0, 556.0, 562.0, 542.0, 534.0, 543.0, 508.0, 513.0, 488.0, 501.0, 476.0]</t>
-  </si>
-  <si>
-    <t>[562.0, 559.0, 530.0, 520.0, 508.0, 496.0, 505.0, 492.0, 482.0, 483.0, 468.0, 445.0, 443.0, 427.0, 429.0, 414.0]</t>
-  </si>
-  <si>
-    <t>[759.0, 739.0, 713.0, 687.0, 691.0, 681.0, 669.0, 654.0, 659.0, 620.0, 616.0, 599.0, 583.0, 562.0, 552.0, 532.0]</t>
-  </si>
-  <si>
-    <t>[697.0, 682.0, 654.0, 620.0, 630.0, 598.0, 601.0, 604.0, 600.0, 602.0, 585.0, 556.0, 537.0, 518.0, 503.0, 502.0]</t>
-  </si>
-  <si>
-    <t>[824.0, 801.0, 786.0, 761.0, 756.0, 747.0, 740.0, 732.0, 719.0, 719.0, 702.0, 670.0, 653.0, 623.0, 621.0, 608.0]</t>
-  </si>
-  <si>
-    <t>[581.0, 539.0, 520.0, 464.0, 429.0, 448.0, 435.0, 430.0, 416.0, 416.0, 420.0, 372.0, 387.0, 372.0, 356.0, 369.0]</t>
-  </si>
-  <si>
-    <t>[808.0, 796.0, 784.0, 749.0, 756.0, 732.0, 740.0, 717.0, 709.0, 718.0, 688.0, 646.0, 619.0, 604.0, 604.0, 599.0]</t>
-  </si>
-  <si>
-    <t>[934.0, 878.0, 861.0, 839.0, 821.0, 821.0, 808.0, 806.0, 794.0, 781.0, 774.0, 749.0, 742.0, 705.0, 704.0, 673.0]</t>
-  </si>
-  <si>
-    <t>[707.0, 692.0, 665.0, 656.0, 642.0, 621.0, 624.0, 609.0, 599.0, 605.0, 594.0, 577.0, 557.0, 540.0, 523.0, 519.0]</t>
-  </si>
-  <si>
-    <t>[723.0, 701.0, 668.0, 663.0, 646.0, 623.0, 627.0, 605.0, 599.0, 610.0, 595.0, 581.0, 559.0, 538.0, 526.0, 519.0]</t>
-  </si>
-  <si>
-    <t>[605.0, 624.0, 590.0, 554.0, 547.0, 503.0, 564.0, 521.0, 507.0, 525.0, 506.0, 488.0, 487.0, 473.0, 443.0, 440.0]</t>
-  </si>
-  <si>
-    <t>[771.0, 765.0, 714.0, 710.0, 728.0, 741.0, 729.0, 675.0, 716.0, 671.0, 660.0, 625.0, 581.0, 596.0, 585.0, 571.0]</t>
-  </si>
-  <si>
-    <t>[529.0, 553.0, 488.0, 518.0, 490.0, 488.0, 481.0, 455.0, 472.0, 447.0, 449.0, 430.0, 415.0, 410.0, 368.0, 390.0]</t>
-  </si>
-  <si>
-    <t>[689.0, 681.0, 662.0, 646.0, 637.0, 619.0, 621.0, 614.0, 599.0, 599.0, 593.0, 570.0, 556.0, 543.0, 520.0, 520.0]</t>
-  </si>
-  <si>
-    <t>[655.0, 605.0, 641.0, 615.0, 602.0, 579.0, 601.0, 608.0, 574.0, 563.0, 561.0, 507.0, 519.0, 517.0, 500.0, 501.0]</t>
-  </si>
-  <si>
-    <t>[817.0, 797.0, 780.0, 747.0, 732.0, 730.0, 730.0, 705.0, 686.0, 685.0, 702.0, 665.0, 642.0, 624.0, 610.0, 603.0]</t>
-  </si>
-  <si>
-    <t>[603.0, 578.0, 566.0, 526.0, 533.0, 511.0, 510.0, 509.0, 497.0, 502.0, 501.0, 474.0, 474.0, 456.0, 443.0, 464.0]</t>
-  </si>
-  <si>
-    <t>[495.0, 480.0, 456.0, 438.0, 413.0, 422.0, 404.0, 397.0, 400.0, 408.0, 388.0, 374.0, 391.0, 372.0, 349.0, 348.0]</t>
-  </si>
-  <si>
-    <t>[789.0, 770.0, 749.0, 726.0, 719.0, 706.0, 691.0, 684.0, 669.0, 657.0, 638.0, 614.0, 600.0, 585.0, 573.0, 552.0]</t>
-  </si>
-  <si>
-    <t>[1078.0, 1052.0, 1027.0, 996.0, 981.0, 973.0, 951.0, 941.0, 923.0, 907.0, 892.0, 858.0, 840.0, 813.0, 780.0, 758.0]</t>
-  </si>
-  <si>
-    <t>[1168.0, 1134.0, 1099.0, 1073.0, 1056.0, 1049.0, 993.0, 977.0, 971.0, 955.0, 941.0, 908.0, 881.0, 847.0, 812.0, 799.0]</t>
-  </si>
-  <si>
-    <t>[1236.0, 1173.0, 1148.0, 1139.0, 1127.0, 1103.0, 1036.0, 1018.0, 1018.0, 1002.0, 979.0, 963.0, 926.0, 902.0, 871.0, 849.0]</t>
-  </si>
-  <si>
-    <t>[1736.0, 1920.0, 1876.0, 1836.0, 1572.0, 1811.0, 1730.0, 1464.0, 1598.0, 1553.0, 1603.0, 1536.0, 1422.0, 1413.0, 1310.0, 1243.0]</t>
-  </si>
-  <si>
-    <t>[1139.0, 1134.0, 1037.0, 1002.0, 1136.0, 1161.0, 971.0, 972.0, 972.0, 1110.0, 993.0, 987.0, 957.0, 932.0, 872.0, 966.0]</t>
-  </si>
-  <si>
-    <t>[1362.0, 1288.0, 1142.0, 1258.0, 1150.0, 1124.0, 1110.0, 1127.0, 1010.0, 1052.0, 1024.0, 1028.0, 985.0, 990.0, 898.0, 904.0]</t>
-  </si>
-  <si>
-    <t>[1727.0, 1629.0, 1680.0, 1563.0, 1529.0, 1549.0, 1527.0, 1543.0, 1415.0, 1411.0, 1260.0, 1363.0, 1300.0, 1094.0, 1228.0, 1280.0]</t>
-  </si>
-  <si>
-    <t>[1262.0, 1222.0, 1157.0, 1130.0, 1127.0, 1064.0, 988.0, 991.0, 1022.0, 961.0, 945.0, 909.0, 894.0, 853.0, 839.0, 823.0]</t>
-  </si>
-  <si>
-    <t>[1330.0, 1280.0, 1283.0, 1274.0, 1300.0, 1240.0, 1208.0, 1273.0, 1170.0, 1072.0, 1137.0, 1073.0, 967.0, 998.0, 958.0, 872.0]</t>
-  </si>
-  <si>
-    <t>[1229.0, 1138.0, 1169.0, 1226.0, 1276.0, 1290.0, 1072.0, 1026.0, 1050.0, 1029.0, 995.0, 1054.0, 903.0, 939.0, 946.0, 844.0]</t>
-  </si>
-  <si>
-    <t>[1245.0, 1243.0, 1280.0, 1252.0, 1171.0, 1130.0, 1052.0, 1061.0, 1137.0, 1093.0, 1000.0, 960.0, 1017.0, 972.0, 905.0, 878.0]</t>
-  </si>
-  <si>
-    <t>[708.0, 674.0, 632.0, 680.0, 595.0, 620.0, 601.0, 599.0, 626.0, 602.0, 628.0, 584.0, 534.0, 549.0, 598.0, 584.0]</t>
-  </si>
-  <si>
-    <t>[1331.0, 1177.0, 1254.0, 1156.0, 1215.0, 1224.0, 1190.0, 1166.0, 1163.0, 1143.0, 1066.0, 1063.0, 1064.0, 1026.0, 943.0, 954.0]</t>
-  </si>
-  <si>
-    <t>[927.0, 873.0, 815.0, 823.0, 865.0, 784.0, 817.0, 728.0, 726.0, 791.0, 758.0, 732.0, 692.0, 662.0, 623.0, 638.0]</t>
-  </si>
-  <si>
-    <t>[1057.0, 1052.0, 992.0, 965.0, 978.0, 1004.0, 883.0, 973.0, 915.0, 898.0, 871.0, 913.0, 792.0, 784.0, 768.0, 770.0]</t>
-  </si>
-  <si>
-    <t>[1105.0, 1055.0, 1018.0, 1004.0, 982.0, 979.0, 952.0, 937.0, 914.0, 894.0, 885.0, 832.0, 828.0, 778.0, 746.0, 744.0]</t>
-  </si>
-  <si>
-    <t>[880.0, 888.0, 765.0, 985.0, 806.0, 930.0, 847.0, 849.0, 756.0, 770.0, 801.0, 737.0, 770.0, 708.0, 609.0, 670.0]</t>
-  </si>
-  <si>
-    <t>[1437.0, 1315.0, 1342.0, 1348.0, 1239.0, 1319.0, 1325.0, 1174.0, 1164.0, 1177.0, 1139.0, 1083.0, 1069.0, 981.0, 922.0, 977.0]</t>
-  </si>
-  <si>
-    <t>[1108.0, 1065.0, 1018.0, 988.0, 999.0, 1029.0, 996.0, 956.0, 953.0, 902.0, 908.0, 858.0, 844.0, 784.0, 757.0, 756.0]</t>
-  </si>
-  <si>
-    <t>[1207.0, 979.0, 953.0, 1033.0, 1004.0, 1149.0, 1016.0, 941.0, 962.0, 1088.0, 935.0, 1047.0, 823.0, 888.0, 773.0, 800.0]</t>
-  </si>
-  <si>
-    <t>[948.0, 958.0, 926.0, 906.0, 915.0, 864.0, 850.0, 829.0, 823.0, 754.0, 812.0, 844.0, 776.0, 786.0, 695.0, 668.0]</t>
-  </si>
-  <si>
-    <t>[1024.0, 1014.0, 998.0, 963.0, 948.0, 944.0, 928.0, 919.0, 900.0, 880.0, 867.0, 835.0, 816.0, 792.0, 767.0, 739.0]</t>
-  </si>
-  <si>
-    <t>[1345.0, 1235.0, 1325.0, 1245.0, 1165.0, 1174.0, 1146.0, 1126.0, 1135.0, 1149.0, 1088.0, 1047.0, 1043.0, 1007.0, 972.0, 906.0]</t>
-  </si>
-  <si>
-    <t>[1445.0, 1363.0, 1312.0, 1302.0, 1253.0, 1162.0, 1148.0, 1238.0, 1177.0, 1182.0, 1003.0, 1074.0, 1034.0, 1014.0, 1006.0, 973.0]</t>
-  </si>
-  <si>
-    <t>[1644.0, 1543.0, 1553.0, 1415.0, 1457.0, 1370.0, 1362.0, 1388.0, 1445.0, 1311.0, 1351.0, 1318.0, 1272.0, 1174.0, 1149.0, 1005.0]</t>
-  </si>
-  <si>
-    <t>[1015.0, 919.0, 1014.0, 908.0, 837.0, 901.0, 881.0, 951.0, 835.0, 857.0, 878.0, 764.0, 755.0, 858.0, 813.0, 727.0]</t>
-  </si>
-  <si>
-    <t>[1259.0, 1307.0, 1207.0, 1257.0, 1158.0, 1143.0, 1136.0, 1140.0, 1040.0, 1061.0, 1001.0, 981.0, 972.0, 945.0, 880.0, 827.0]</t>
-  </si>
-  <si>
-    <t>[1156.0, 1183.0, 1119.0, 1067.0, 1062.0, 1030.0, 1015.0, 1038.0, 977.0, 940.0, 931.0, 939.0, 872.0, 837.0, 884.0, 773.0]</t>
-  </si>
-  <si>
-    <t>[913.0, 894.0, 907.0, 902.0, 831.0, 884.0, 855.0, 808.0, 818.0, 750.0, 787.0, 724.0, 716.0, 728.0, 689.0, 657.0]</t>
-  </si>
-  <si>
-    <t>[897.0, 900.0, 884.0, 862.0, 839.0, 818.0, 845.0, 798.0, 788.0, 774.0, 779.0, 754.0, 728.0, 682.0, 689.0, 685.0]</t>
-  </si>
-  <si>
-    <t>[1243.0, 1192.0, 1152.0, 1135.0, 1001.0, 1010.0, 1013.0, 1003.0, 974.0, 985.0, 962.0, 930.0, 901.0, 846.0, 845.0, 796.0]</t>
-  </si>
-  <si>
-    <t>[1762.0, 1753.0, 1619.0, 1717.0, 1590.0, 1566.0, 1636.0, 1631.0, 1461.0, 1449.0, 1509.0, 1381.0, 1333.0, 1354.0, 1255.0, 1413.0]</t>
-  </si>
-  <si>
-    <t>[934.0, 935.0, 933.0, 907.0, 897.0, 888.0, 858.0, 869.0, 862.0, 836.0, 818.0, 784.0, 763.0, 753.0, 729.0, 708.0]</t>
-  </si>
-  <si>
-    <t>[1253.0, 1208.0, 1152.0, 1144.0, 1143.0, 1100.0, 1055.0, 1093.0, 1011.0, 1030.0, 1056.0, 962.0, 915.0, 924.0, 886.0, 878.0]</t>
-  </si>
-  <si>
-    <t>[982.0, 987.0, 981.0, 957.0, 956.0, 937.0, 921.0, 933.0, 931.0, 891.0, 871.0, 847.0, 824.0, 813.0, 776.0, 757.0]</t>
-  </si>
-  <si>
-    <t>[1092.0, 1091.0, 1074.0, 1006.0, 984.0, 986.0, 978.0, 989.0, 962.0, 940.0, 920.0, 900.0, 890.0, 841.0, 824.0, 824.0]</t>
-  </si>
-  <si>
-    <t>[840.0, 820.0, 786.0, 817.0, 772.0, 729.0, 729.0, 739.0, 714.0, 723.0, 812.0, 685.0, 703.0, 657.0, 654.0, 627.0]</t>
-  </si>
-  <si>
-    <t>[997.0, 943.0, 951.0, 942.0, 870.0, 884.0, 885.0, 856.0, 834.0, 775.0, 777.0, 732.0, 733.0, 735.0, 688.0, 648.0]</t>
-  </si>
-  <si>
-    <t>[932.0, 857.0, 922.0, 918.0, 812.0, 866.0, 855.0, 816.0, 757.0, 730.0, 744.0, 697.0, 714.0, 653.0, 646.0, 619.0]</t>
-  </si>
-  <si>
-    <t>[1890.0, 1834.0, 1839.0, 1811.0, 1902.0, 1802.0, 1871.0, 1898.0, 1605.0, 1475.0, 1647.0, 1603.0, 1564.0, 1483.0, 1432.0, 1364.0]</t>
-  </si>
-  <si>
-    <t>[1677.0, 1759.0, 1476.0, 1533.0, 1246.0, 1497.0, 1418.0, 1527.0, 1618.0, 1228.0, 1230.0, 1062.0, 1329.0, 1134.0, 978.0, 989.0]</t>
-  </si>
-  <si>
-    <t>[1156.0, 1143.0, 1143.0, 1098.0, 1076.0, 1086.0, 1086.0, 1034.0, 1039.0, 1035.0, 1011.0, 976.0, 971.0, 930.0, 895.0, 887.0]</t>
-  </si>
-  <si>
-    <t>[911.0, 845.0, 834.0, 796.0, 818.0, 858.0, 842.0, 845.0, 836.0, 791.0, 750.0, 803.0, 792.0, 725.0, 710.0, 738.0]</t>
-  </si>
-  <si>
-    <t>[1061.0, 1041.0, 936.0, 908.0, 940.0, 909.0, 912.0, 964.0, 956.0, 893.0, 923.0, 845.0, 829.0, 789.0, 836.0, 718.0]</t>
-  </si>
-  <si>
-    <t>[511.0, 501.0, 487.0, 463.0, 461.0, 452.0, 435.0, 433.0, 423.0, 418.0, 418.0, 406.0, 390.0, 379.0, 374.0, 366.0]</t>
-  </si>
-  <si>
-    <t>[548.0, 533.0, 519.0, 490.0, 492.0, 486.0, 477.0, 483.0, 465.0, 464.0, 459.0, 447.0, 417.0, 408.0, 402.0, 396.0]</t>
-  </si>
-  <si>
-    <t>[513.0, 493.0, 498.0, 457.0, 466.0, 450.0, 445.0, 446.0, 427.0, 430.0, 424.0, 416.0, 395.0, 385.0, 383.0, 372.0]</t>
-  </si>
-  <si>
-    <t>[613.0, 690.0, 688.0, 655.0, 617.0, 643.0, 658.0, 602.0, 606.0, 599.0, 594.0, 588.0, 557.0, 514.0, 557.0, 505.0]</t>
-  </si>
-  <si>
-    <t>[646.0, 669.0, 672.0, 686.0, 687.0, 599.0, 643.0, 586.0, 625.0, 623.0, 605.0, 578.0, 545.0, 531.0, 558.0, 521.0]</t>
-  </si>
-  <si>
-    <t>[816.0, 985.0, 938.0, 1009.0, 743.0, 881.0, 815.0, 938.0, 772.0, 805.0, 731.0, 791.0, 758.0, 738.0, 841.0, 731.0]</t>
-  </si>
-  <si>
-    <t>[506.0, 548.0, 516.0, 515.0, 514.0, 500.0, 501.0, 474.0, 463.0, 462.0, 478.0, 465.0, 416.0, 405.0, 418.0, 387.0]</t>
-  </si>
-  <si>
-    <t>[473.0, 459.0, 434.0, 414.0, 419.0, 400.0, 389.0, 390.0, 387.0, 378.0, 376.0, 363.0, 355.0, 337.0, 339.0, 326.0]</t>
-  </si>
-  <si>
-    <t>[437.0, 436.0, 421.0, 400.0, 405.0, 382.0, 361.0, 363.0, 381.0, 371.0, 363.0, 341.0, 340.0, 314.0, 319.0, 317.0]</t>
-  </si>
-  <si>
-    <t>[446.0, 410.0, 413.0, 388.0, 401.0, 380.0, 357.0, 375.0, 367.0, 367.0, 338.0, 335.0, 326.0, 318.0, 323.0, 310.0]</t>
-  </si>
-  <si>
-    <t>[560.0, 515.0, 498.0, 493.0, 459.0, 483.0, 421.0, 505.0, 405.0, 418.0, 457.0, 404.0, 407.0, 417.0, 392.0, 361.0]</t>
-  </si>
-  <si>
-    <t>[478.0, 475.0, 441.0, 411.0, 415.0, 400.0, 396.0, 389.0, 381.0, 363.0, 367.0, 360.0, 348.0, 332.0, 327.0, 318.0]</t>
-  </si>
-  <si>
-    <t>[477.0, 463.0, 454.0, 419.0, 413.0, 417.0, 407.0, 406.0, 391.0, 388.0, 383.0, 376.0, 363.0, 344.0, 335.0, 329.0]</t>
-  </si>
-  <si>
-    <t>[491.0, 481.0, 476.0, 429.0, 415.0, 418.0, 408.0, 418.0, 400.0, 401.0, 397.0, 388.0, 375.0, 363.0, 343.0, 349.0]</t>
-  </si>
-  <si>
-    <t>[457.0, 439.0, 427.0, 407.0, 400.0, 406.0, 395.0, 392.0, 376.0, 371.0, 371.0, 357.0, 348.0, 328.0, 324.0, 317.0]</t>
-  </si>
-  <si>
-    <t>[517.0, 503.0, 482.0, 475.0, 455.0, 464.0, 428.0, 422.0, 432.0, 415.0, 441.0, 402.0, 388.0, 390.0, 380.0, 370.0]</t>
-  </si>
-  <si>
-    <t>[696.0, 672.0, 649.0, 627.0, 620.0, 615.0, 610.0, 602.0, 597.0, 590.0, 578.0, 550.0, 538.0, 520.0, 512.0, 502.0]</t>
-  </si>
-  <si>
-    <t>[651.0, 609.0, 590.0, 578.0, 570.0, 566.0, 521.0, 549.0, 516.0, 525.0, 516.0, 493.0, 487.0, 483.0, 464.0, 452.0]</t>
-  </si>
-  <si>
-    <t>[672.0, 639.0, 630.0, 614.0, 595.0, 612.0, 598.0, 599.0, 578.0, 597.0, 556.0, 538.0, 536.0, 525.0, 505.0, 496.0]</t>
-  </si>
-  <si>
-    <t>[463.0, 422.0, 403.0, 405.0, 387.0, 379.0, 368.0, 373.0, 366.0, 361.0, 349.0, 344.0, 327.0, 322.0, 313.0, 315.0]</t>
-  </si>
-  <si>
-    <t>[543.0, 523.0, 514.0, 494.0, 491.0, 485.0, 436.0, 466.0, 421.0, 443.0, 440.0, 409.0, 405.0, 401.0, 386.0, 382.0]</t>
-  </si>
-  <si>
-    <t>[1053.0, 882.0, 999.0, 729.0, 871.0, 868.0, 842.0, 772.0, 838.0, 847.0, 804.0, 683.0, 717.0, 730.0, 643.0, 594.0]</t>
-  </si>
-  <si>
-    <t>[809.0, 795.0, 676.0, 717.0, 698.0, 733.0, 641.0, 665.0, 649.0, 692.0, 652.0, 644.0, 653.0, 624.0, 615.0, 609.0]</t>
-  </si>
-  <si>
-    <t>[933.0, 902.0, 826.0, 699.0, 766.0, 766.0, 825.0, 757.0, 748.0, 747.0, 841.0, 713.0, 654.0, 648.0, 740.0, 760.0]</t>
-  </si>
-  <si>
-    <t>[1009.0, 956.0, 872.0, 917.0, 873.0, 859.0, 822.0, 927.0, 842.0, 736.0, 846.0, 784.0, 739.0, 737.0, 754.0, 675.0]</t>
-  </si>
-  <si>
-    <t>[883.0, 818.0, 780.0, 735.0, 726.0, 756.0, 680.0, 676.0, 683.0, 745.0, 682.0, 701.0, 646.0, 716.0, 663.0, 608.0]</t>
-  </si>
-  <si>
-    <t>[711.0, 691.0, 669.0, 646.0, 637.0, 628.0, 629.0, 615.0, 612.0, 602.0, 590.0, 570.0, 557.0, 533.0, 522.0, 513.0]</t>
-  </si>
-  <si>
-    <t>[739.0, 716.0, 716.0, 692.0, 660.0, 670.0, 672.0, 656.0, 628.0, 627.0, 603.0, 601.0, 582.0, 551.0, 542.0, 512.0]</t>
-  </si>
-  <si>
-    <t>[680.0, 637.0, 623.0, 604.0, 606.0, 616.0, 585.0, 569.0, 586.0, 587.0, 568.0, 521.0, 533.0, 505.0, 504.0, 503.0]</t>
-  </si>
-  <si>
-    <t>[606.0, 599.0, 581.0, 569.0, 532.0, 527.0, 524.0, 520.0, 529.0, 516.0, 502.0, 480.0, 467.0, 463.0, 463.0, 446.0]</t>
-  </si>
-  <si>
-    <t>[725.0, 691.0, 671.0, 655.0, 669.0, 617.0, 605.0, 626.0, 624.0, 614.0, 578.0, 551.0, 546.0, 556.0, 516.0, 527.0]</t>
-  </si>
-  <si>
-    <t>[808.0, 856.0, 931.0, 854.0, 851.0, 878.0, 907.0, 892.0, 897.0, 908.0, 803.0, 799.0, 780.0, 733.0, 743.0, 765.0]</t>
-  </si>
-  <si>
-    <t>[790.0, 798.0, 765.0, 732.0, 738.0, 690.0, 765.0, 722.0, 695.0, 644.0, 690.0, 658.0, 616.0, 650.0, 613.0, 601.0]</t>
-  </si>
-  <si>
-    <t>[590.0, 596.0, 583.0, 566.0, 576.0, 524.0, 522.0, 543.0, 518.0, 525.0, 516.0, 500.0, 480.0, 450.0, 469.0, 452.0]</t>
-  </si>
-  <si>
-    <t>[570.0, 538.0, 526.0, 506.0, 514.0, 484.0, 484.0, 501.0, 495.0, 479.0, 466.0, 441.0, 425.0, 409.0, 420.0, 403.0]</t>
-  </si>
-  <si>
-    <t>[753.0, 735.0, 708.0, 683.0, 685.0, 677.0, 665.0, 651.0, 657.0, 619.0, 614.0, 597.0, 584.0, 559.0, 550.0, 531.0]</t>
-  </si>
-  <si>
-    <t>[701.0, 670.0, 648.0, 622.0, 626.0, 596.0, 600.0, 594.0, 597.0, 594.0, 582.0, 550.0, 534.0, 509.0, 499.0, 502.0]</t>
-  </si>
-  <si>
-    <t>[638.0, 579.0, 580.0, 580.0, 509.0, 578.0, 550.0, 515.0, 537.0, 542.0, 607.0, 539.0, 518.0, 486.0, 453.0, 449.0]</t>
-  </si>
-  <si>
-    <t>[483.0, 471.0, 465.0, 437.0, 375.0, 368.0, 377.0, 371.0, 369.0, 372.0, 392.0, 348.0, 342.0, 327.0, 322.0, 318.0]</t>
-  </si>
-  <si>
-    <t>[785.0, 802.0, 639.0, 704.0, 691.0, 654.0, 723.0, 612.0, 646.0, 673.0, 747.0, 573.0, 533.0, 480.0, 504.0, 497.0]</t>
-  </si>
-  <si>
-    <t>[823.0, 736.0, 783.0, 761.0, 725.0, 710.0, 757.0, 751.0, 683.0, 644.0, 779.0, 726.0, 697.0, 691.0, 611.0, 629.0]</t>
-  </si>
-  <si>
-    <t>[561.0, 545.0, 531.0, 512.0, 504.0, 498.0, 493.0, 485.0, 473.0, 472.0, 462.0, 437.0, 426.0, 420.0, 406.0, 407.0]</t>
-  </si>
-  <si>
-    <t>[575.0, 564.0, 527.0, 519.0, 502.0, 498.0, 496.0, 483.0, 481.0, 472.0, 464.0, 443.0, 432.0, 423.0, 405.0, 406.0]</t>
-  </si>
-  <si>
-    <t>[518.0, 587.0, 554.0, 544.0, 506.0, 490.0, 520.0, 449.0, 481.0, 486.0, 453.0, 447.0, 417.0, 441.0, 397.0, 404.0]</t>
-  </si>
-  <si>
-    <t>[679.0, 637.0, 584.0, 583.0, 578.0, 583.0, 570.0, 541.0, 549.0, 513.0, 527.0, 506.0, 479.0, 486.0, 474.0, 448.0]</t>
-  </si>
-  <si>
-    <t>[496.0, 516.0, 425.0, 482.0, 477.0, 429.0, 431.0, 421.0, 438.0, 415.0, 401.0, 396.0, 389.0, 384.0, 341.0, 362.0]</t>
-  </si>
-  <si>
-    <t>[538.0, 514.0, 540.0, 494.0, 510.0, 497.0, 487.0, 490.0, 447.0, 472.0, 455.0, 424.0, 414.0, 412.0, 410.0, 410.0]</t>
-  </si>
-  <si>
-    <t>[599.0, 517.0, 589.0, 572.0, 582.0, 556.0, 516.0, 579.0, 502.0, 527.0, 507.0, 476.0, 466.0, 456.0, 440.0, 470.0]</t>
-  </si>
-  <si>
-    <t>[559.0, 589.0, 630.0, 632.0, 545.0, 583.0, 537.0, 511.0, 492.0, 512.0, 542.0, 499.0, 436.0, 473.0, 476.0, 474.0]</t>
-  </si>
-  <si>
-    <t>[541.0, 500.0, 509.0, 455.0, 476.0, 421.0, 476.0, 416.0, 419.0, 421.0, 417.0, 418.0, 412.0, 406.0, 402.0, 415.0]</t>
-  </si>
-  <si>
-    <t>[484.0, 462.0, 437.0, 424.0, 395.0, 416.0, 394.0, 397.0, 389.0, 389.0, 368.0, 362.0, 367.0, 358.0, 333.0, 350.0]</t>
-  </si>
-  <si>
-    <t>[973.0, 941.0, 915.0, 895.0, 871.0, 860.0, 854.0, 832.0, 824.0, 819.0, 798.0, 766.0, 743.0, 722.0, 713.0, 695.0]</t>
-  </si>
-  <si>
-    <t>[1468.0, 1442.0, 1420.0, 1383.0, 1346.0, 1349.0, 1328.0, 1269.0, 1256.0, 1248.0, 1238.0, 1187.0, 1154.0, 1113.0, 1098.0, 1059.0]</t>
-  </si>
-  <si>
-    <t>[1537.0, 1526.0, 1491.0, 1436.0, 1416.0, 1412.0, 1387.0, 1370.0, 1363.0, 1334.0, 1343.0, 1261.0, 1231.0, 1167.0, 1158.0, 1143.0]</t>
-  </si>
-  <si>
-    <t>[1585.0, 1573.0, 1539.0, 1486.0, 1454.0, 1456.0, 1428.0, 1427.0, 1414.0, 1384.0, 1384.0, 1337.0, 1264.0, 1230.0, 1215.0, 1172.0]</t>
-  </si>
-  <si>
-    <t>[2488.0, 2415.0, 2419.0, 2251.0, 2246.0, 2266.0, 2275.0, 2122.0, 2217.0, 2084.0, 1999.0, 1918.0, 1907.0, 1903.0, 1875.0, 1736.0]</t>
-  </si>
-  <si>
-    <t>[1427.0, 1488.0, 1358.0, 1347.0, 1350.0, 1444.0, 1436.0, 1319.0, 1354.0, 1372.0, 1315.0, 1332.0, 1256.0, 1152.0, 1166.0, 1170.0]</t>
-  </si>
-  <si>
-    <t>[1852.0, 1747.0, 1745.0, 1603.0, 1624.0, 1658.0, 1640.0, 1660.0, 1534.0, 1536.0, 1601.0, 1511.0, 1482.0, 1440.0, 1441.0, 1271.0]</t>
-  </si>
-  <si>
-    <t>[1920.0, 1897.0, 1756.0, 1817.0, 1763.0, 1769.0, 1740.0, 1595.0, 1729.0, 1788.0, 1641.0, 1596.0, 1492.0, 1540.0, 1547.0, 1437.0]</t>
-  </si>
-  <si>
-    <t>[1784.0, 1719.0, 1670.0, 1732.0, 1671.0, 1518.0, 1405.0, 1504.0, 1546.0, 1443.0, 1457.0, 1452.0, 1421.0, 1347.0, 1397.0, 1314.0]</t>
-  </si>
-  <si>
-    <t>[1761.0, 1748.0, 1737.0, 1495.0, 1827.0, 1536.0, 1447.0, 1488.0, 1458.0, 1548.0, 1433.0, 1581.0, 1391.0, 1357.0, 1259.0, 1242.0]</t>
-  </si>
-  <si>
-    <t>[1431.0, 1420.0, 1400.0, 1404.0, 1366.0, 1441.0, 1467.0, 1368.0, 1394.0, 1383.0, 1251.0, 1374.0, 1158.0, 1199.0, 1153.0, 1297.0]</t>
-  </si>
-  <si>
-    <t>[1563.0, 1561.0, 1528.0, 1585.0, 1439.0, 1543.0, 1566.0, 1532.0, 1396.0, 1432.0, 1398.0, 1371.0, 1275.0, 1289.0, 1172.0, 1172.0]</t>
-  </si>
-  <si>
-    <t>[922.0, 894.0, 853.0, 820.0, 806.0, 801.0, 744.0, 734.0, 796.0, 754.0, 739.0, 731.0, 715.0, 740.0, 713.0, 706.0]</t>
-  </si>
-  <si>
-    <t>[1729.0, 1490.0, 1610.0, 1422.0, 1448.0, 1412.0, 1544.0, 1456.0, 1510.0, 1448.0, 1504.0, 1414.0, 1428.0, 1327.0, 1135.0, 1149.0]</t>
-  </si>
-  <si>
-    <t>[1148.0, 1163.0, 1157.0, 1137.0, 976.0, 1068.0, 1045.0, 1201.0, 1111.0, 982.0, 1054.0, 970.0, 919.0, 803.0, 767.0, 849.0]</t>
-  </si>
-  <si>
-    <t>[1336.0, 1281.0, 1206.0, 1142.0, 1142.0, 1150.0, 1151.0, 1221.0, 1163.0, 1147.0, 1254.0, 1063.0, 1010.0, 990.0, 1014.0, 848.0]</t>
-  </si>
-  <si>
-    <t>[1383.0, 1390.0, 1373.0, 1327.0, 1310.0, 1263.0, 1274.0, 1225.0, 1227.0, 1171.0, 1167.0, 1131.0, 1134.0, 1037.0, 1007.0, 1014.0]</t>
-  </si>
-  <si>
-    <t>[878.0, 882.0, 942.0, 886.0, 970.0, 871.0, 853.0, 928.0, 895.0, 958.0, 826.0, 794.0, 768.0, 930.0, 935.0, 812.0]</t>
-  </si>
-  <si>
-    <t>[1642.0, 1651.0, 1586.0, 1519.0, 1665.0, 1614.0, 1535.0, 1514.0, 1554.0, 1371.0, 1391.0, 1388.0, 1417.0, 1362.0, 1215.0, 1267.0]</t>
-  </si>
-  <si>
-    <t>[1404.0, 1389.0, 1441.0, 1345.0, 1236.0, 1268.0, 1350.0, 1250.0, 1273.0, 1190.0, 1178.0, 1186.0, 1160.0, 1072.0, 1016.0, 1041.0]</t>
-  </si>
-  <si>
-    <t>[1647.0, 1662.0, 1714.0, 1738.0, 1637.0, 1565.0, 1532.0, 1535.0, 1647.0, 1450.0, 1370.0, 1377.0, 1532.0, 1239.0, 1170.0, 1242.0]</t>
-  </si>
-  <si>
-    <t>[1443.0, 1332.0, 1331.0, 1186.0, 1188.0, 1162.0, 1074.0, 1345.0, 1154.0, 1118.0, 1118.0, 1129.0, 1155.0, 977.0, 1001.0, 1115.0]</t>
-  </si>
-  <si>
-    <t>[1425.0, 1391.0, 1364.0, 1343.0, 1286.0, 1295.0, 1267.0, 1211.0, 1179.0, 1191.0, 1169.0, 1148.0, 1109.0, 1058.0, 1049.0, 1005.0]</t>
-  </si>
-  <si>
-    <t>[1604.0, 1552.0, 1518.0, 1503.0, 1435.0, 1452.0, 1414.0, 1369.0, 1349.0, 1304.0, 1320.0, 1294.0, 1231.0, 1174.0, 1155.0, 1130.0]</t>
-  </si>
-  <si>
-    <t>[1662.0, 1539.0, 1466.0, 1501.0, 1447.0, 1428.0, 1363.0, 1330.0, 1243.0, 1267.0, 1261.0, 1268.0, 1229.0, 1129.0, 1151.0, 1115.0]</t>
-  </si>
-  <si>
-    <t>[1894.0, 1863.0, 1863.0, 1751.0, 1736.0, 1737.0, 1674.0, 1606.0, 1590.0, 1550.0, 1555.0, 1509.0, 1410.0, 1456.0, 1429.0, 1336.0]</t>
-  </si>
-  <si>
-    <t>[1114.0, 1134.0, 1078.0, 1135.0, 1049.0, 1019.0, 985.0, 896.0, 979.0, 930.0, 903.0, 905.0, 878.0, 809.0, 850.0, 769.0]</t>
-  </si>
-  <si>
-    <t>[1528.0, 1518.0, 1529.0, 1452.0, 1413.0, 1403.0, 1358.0, 1343.0, 1293.0, 1318.0, 1286.0, 1258.0, 1181.0, 1133.0, 1139.0, 1094.0]</t>
-  </si>
-  <si>
-    <t>[1357.0, 1361.0, 1319.0, 1379.0, 1247.0, 1271.0, 1226.0, 1156.0, 1158.0, 1190.0, 1156.0, 1151.0, 1121.0, 1073.0, 1012.0, 970.0]</t>
-  </si>
-  <si>
-    <t>[1004.0, 901.0, 892.0, 908.0, 885.0, 889.0, 833.0, 874.0, 780.0, 797.0, 787.0, 833.0, 761.0, 788.0, 832.0, 690.0]</t>
-  </si>
-  <si>
-    <t>[958.0, 935.0, 1039.0, 943.0, 892.0, 978.0, 856.0, 902.0, 865.0, 864.0, 812.0, 764.0, 749.0, 780.0, 720.0, 735.0]</t>
-  </si>
-  <si>
-    <t>[1910.0, 1896.0, 1904.0, 1877.0, 1765.0, 1764.0, 1884.0, 1758.0, 1674.0, 1741.0, 1696.0, 1579.0, 1734.0, 1531.0, 1561.0, 1480.0]</t>
-  </si>
-  <si>
-    <t>[2202.0, 2105.0, 2086.0, 1914.0, 1915.0, 1986.0, 2055.0, 1884.0, 1895.0, 1934.0, 1875.0, 1783.0, 1891.0, 1748.0, 1710.0, 1619.0]</t>
-  </si>
-  <si>
-    <t>[1235.0, 1202.0, 1154.0, 1144.0, 1141.0, 1091.0, 1133.0, 1109.0, 1065.0, 1068.0, 1020.0, 1007.0, 969.0, 960.0, 956.0, 904.0]</t>
-  </si>
-  <si>
-    <t>[1603.0, 1414.0, 1356.0, 1405.0, 1409.0, 1338.0, 1366.0, 1358.0, 1308.0, 1342.0, 1245.0, 1239.0, 1228.0, 1173.0, 1162.0, 1111.0]</t>
-  </si>
-  <si>
-    <t>[1148.0, 1139.0, 1126.0, 1077.0, 1096.0, 1025.0, 1128.0, 1022.0, 1024.0, 1040.0, 994.0, 938.0, 920.0, 909.0, 917.0, 843.0]</t>
-  </si>
-  <si>
-    <t>[1226.0, 1226.0, 1146.0, 1149.0, 1108.0, 1093.0, 1050.0, 1049.0, 1035.0, 1028.0, 995.0, 1001.0, 950.0, 942.0, 955.0, 903.0]</t>
-  </si>
-  <si>
-    <t>[1095.0, 1128.0, 1135.0, 1024.0, 1096.0, 1055.0, 917.0, 1105.0, 927.0, 959.0, 953.0, 987.0, 956.0, 803.0, 873.0, 831.0]</t>
-  </si>
-  <si>
-    <t>[1151.0, 1161.0, 1139.0, 1088.0, 1024.0, 1118.0, 1055.0, 995.0, 977.0, 960.0, 951.0, 920.0, 942.0, 885.0, 862.0, 837.0]</t>
-  </si>
-  <si>
-    <t>[1169.0, 1172.0, 1267.0, 1099.0, 1020.0, 1095.0, 1028.0, 1045.0, 1001.0, 956.0, 899.0, 894.0, 868.0, 920.0, 818.0, 818.0]</t>
-  </si>
-  <si>
-    <t>[2271.0, 2228.0, 2096.0, 2117.0, 2176.0, 2092.0, 1879.0, 1998.0, 1930.0, 1954.0, 1914.0, 1887.0, 1725.0, 1597.0, 1684.0, 1533.0]</t>
-  </si>
-  <si>
-    <t>[2513.0, 2277.0, 2343.0, 1915.0, 2002.0, 2087.0, 2099.0, 1935.0, 2278.0, 1914.0, 1911.0, 1796.0, 1847.0, 1862.0, 1874.0, 1677.0]</t>
-  </si>
-  <si>
-    <t>[1271.0, 1260.0, 1261.0, 1222.0, 1190.0, 1236.0, 1189.0, 1081.0, 1201.0, 1090.0, 1168.0, 1098.0, 1074.0, 1011.0, 1031.0, 1006.0]</t>
-  </si>
-  <si>
-    <t>[819.0, 1061.0, 1071.0, 1089.0, 878.0, 980.0, 943.0, 888.0, 997.0, 925.0, 942.0, 1049.0, 797.0, 836.0, 763.0, 810.0]</t>
-  </si>
-  <si>
-    <t>[1232.0, 1404.0, 1156.0, 1106.0, 1156.0, 959.0, 1131.0, 1054.0, 1038.0, 1018.0, 1035.0, 1050.0, 892.0, 973.0, 961.0, 869.0]</t>
-  </si>
-  <si>
-    <t>[641.0, 608.0, 595.0, 585.0, 583.0, 555.0, 543.0, 551.0, 543.0, 524.0, 537.0, 515.0, 494.0, 478.0, 476.0, 463.0]</t>
-  </si>
-  <si>
-    <t>[661.0, 597.0, 602.0, 577.0, 560.0, 546.0, 529.0, 521.0, 515.0, 544.0, 512.0, 522.0, 502.0, 422.0, 453.0, 469.0]</t>
-  </si>
-  <si>
-    <t>[558.0, 583.0, 534.0, 526.0, 528.0, 499.0, 508.0, 502.0, 488.0, 519.0, 485.0, 500.0, 471.0, 406.0, 420.0, 438.0]</t>
-  </si>
-  <si>
-    <t>[922.0, 894.0, 854.0, 851.0, 886.0, 824.0, 841.0, 797.0, 800.0, 798.0, 794.0, 754.0, 737.0, 729.0, 733.0, 666.0]</t>
-  </si>
-  <si>
-    <t>[811.0, 825.0, 793.0, 779.0, 755.0, 729.0, 768.0, 722.0, 724.0, 726.0, 725.0, 686.0, 655.0, 632.0, 654.0, 671.0]</t>
-  </si>
-  <si>
-    <t>[1131.0, 1024.0, 1008.0, 1001.0, 1043.0, 1032.0, 1016.0, 948.0, 992.0, 971.0, 929.0, 907.0, 884.0, 849.0, 845.0, 770.0]</t>
-  </si>
-  <si>
-    <t>[636.0, 616.0, 597.0, 592.0, 589.0, 549.0, 537.0, 544.0, 519.0, 520.0, 540.0, 524.0, 498.0, 508.0, 471.0, 468.0]</t>
-  </si>
-  <si>
-    <t>[533.0, 502.0, 491.0, 481.0, 463.0, 437.0, 433.0, 429.0, 423.0, 416.0, 432.0, 403.0, 389.0, 371.0, 384.0, 373.0]</t>
-  </si>
-  <si>
-    <t>[518.0, 481.0, 459.0, 427.0, 416.0, 411.0, 403.0, 406.0, 401.0, 400.0, 404.0, 377.0, 377.0, 350.0, 356.0, 348.0]</t>
-  </si>
-  <si>
-    <t>[486.0, 449.0, 432.0, 414.0, 411.0, 392.0, 408.0, 395.0, 390.0, 385.0, 368.0, 367.0, 336.0, 324.0, 319.0, 334.0]</t>
-  </si>
-  <si>
-    <t>[601.0, 600.0, 701.0, 569.0, 634.0, 594.0, 520.0, 593.0, 533.0, 560.0, 596.0, 551.0, 510.0, 422.0, 482.0, 466.0]</t>
-  </si>
-  <si>
-    <t>[551.0, 533.0, 504.0, 501.0, 501.0, 449.0, 456.0, 466.0, 450.0, 419.0, 436.0, 415.0, 401.0, 384.0, 399.0, 385.0]</t>
-  </si>
-  <si>
-    <t>[604.0, 573.0, 548.0, 517.0, 517.0, 505.0, 501.0, 502.0, 493.0, 488.0, 488.0, 472.0, 445.0, 428.0, 412.0, 421.0]</t>
-  </si>
-  <si>
-    <t>[607.0, 574.0, 564.0, 547.0, 540.0, 517.0, 511.0, 514.0, 494.0, 494.0, 493.0, 475.0, 447.0, 441.0, 425.0, 420.0]</t>
-  </si>
-  <si>
-    <t>[559.0, 508.0, 497.0, 475.0, 404.0, 467.0, 425.0, 473.0, 455.0, 444.0, 436.0, 439.0, 404.0, 390.0, 402.0, 371.0]</t>
-  </si>
-  <si>
-    <t>[638.0, 612.0, 613.0, 597.0, 607.0, 549.0, 569.0, 562.0, 519.0, 546.0, 591.0, 578.0, 506.0, 491.0, 500.0, 476.0]</t>
-  </si>
-  <si>
-    <t>[846.0, 834.0, 805.0, 777.0, 766.0, 756.0, 768.0, 738.0, 736.0, 737.0, 733.0, 714.0, 696.0, 690.0, 669.0, 658.0]</t>
-  </si>
-  <si>
-    <t>[949.0, 934.0, 904.0, 880.0, 841.0, 835.0, 838.0, 804.0, 805.0, 793.0, 796.0, 791.0, 761.0, 762.0, 747.0, 731.0]</t>
-  </si>
-  <si>
-    <t>[911.0, 891.0, 857.0, 825.0, 793.0, 778.0, 792.0, 759.0, 782.0, 770.0, 781.0, 746.0, 732.0, 723.0, 737.0, 705.0]</t>
-  </si>
-  <si>
-    <t>[468.0, 493.0, 475.0, 471.0, 412.0, 426.0, 400.0, 411.0, 400.0, 422.0, 399.0, 409.0, 387.0, 389.0, 380.0, 339.0]</t>
-  </si>
-  <si>
-    <t>[764.0, 704.0, 730.0, 694.0, 698.0, 719.0, 678.0, 620.0, 651.0, 624.0, 623.0, 638.0, 597.0, 606.0, 597.0, 599.0]</t>
-  </si>
-  <si>
-    <t>[950.0, 895.0, 1034.0, 1155.0, 1041.0, 1005.0, 945.0, 961.0, 897.0, 1201.0, 879.0, 900.0, 944.0, 1017.0, 942.0, 880.0]</t>
-  </si>
-  <si>
-    <t>[1048.0, 1058.0, 1166.0, 1028.0, 946.0, 1029.0, 1026.0, 1033.0, 973.0, 860.0, 994.0, 959.0, 890.0, 908.0, 970.0, 981.0]</t>
-  </si>
-  <si>
-    <t>[1345.0, 1332.0, 1202.0, 1147.0, 986.0, 1013.0, 992.0, 953.0, 1009.0, 936.0, 957.0, 939.0, 966.0, 919.0, 875.0, 861.0]</t>
-  </si>
-  <si>
-    <t>[1239.0, 1222.0, 1140.0, 1066.0, 1120.0, 1131.0, 1161.0, 1019.0, 983.0, 986.0, 1064.0, 976.0, 997.0, 960.0, 895.0, 947.0]</t>
-  </si>
-  <si>
-    <t>[1264.0, 1159.0, 1222.0, 1052.0, 991.0, 928.0, 1031.0, 992.0, 978.0, 939.0, 952.0, 1027.0, 965.0, 989.0, 834.0, 953.0]</t>
-  </si>
-  <si>
-    <t>[738.0, 735.0, 708.0, 693.0, 701.0, 673.0, 700.0, 668.0, 656.0, 657.0, 651.0, 619.0, 619.0, 605.0, 587.0, 584.0]</t>
-  </si>
-  <si>
-    <t>[778.0, 743.0, 790.0, 690.0, 732.0, 751.0, 740.0, 654.0, 677.0, 671.0, 645.0, 666.0, 607.0, 580.0, 563.0, 595.0]</t>
-  </si>
-  <si>
-    <t>[689.0, 712.0, 676.0, 690.0, 698.0, 639.0, 684.0, 628.0, 614.0, 617.0, 607.0, 608.0, 615.0, 624.0, 571.0, 560.0]</t>
-  </si>
-  <si>
-    <t>[593.0, 652.0, 600.0, 619.0, 616.0, 600.0, 604.0, 521.0, 547.0, 537.0, 537.0, 503.0, 562.0, 504.0, 454.0, 500.0]</t>
-  </si>
-  <si>
-    <t>[926.0, 753.0, 734.0, 759.0, 764.0, 747.0, 796.0, 728.0, 721.0, 747.0, 722.0, 649.0, 661.0, 613.0, 701.0, 588.0]</t>
-  </si>
-  <si>
-    <t>[983.0, 965.0, 1020.0, 1021.0, 1025.0, 1012.0, 1026.0, 1017.0, 952.0, 944.0, 939.0, 929.0, 896.0, 874.0, 834.0, 782.0]</t>
-  </si>
-  <si>
-    <t>[1004.0, 1043.0, 935.0, 978.0, 1024.0, 864.0, 946.0, 916.0, 855.0, 928.0, 862.0, 885.0, 816.0, 767.0, 767.0, 722.0]</t>
-  </si>
-  <si>
-    <t>[654.0, 616.0, 602.0, 604.0, 603.0, 547.0, 577.0, 571.0, 553.0, 538.0, 559.0, 514.0, 531.0, 504.0, 512.0, 485.0]</t>
-  </si>
-  <si>
-    <t>[558.0, 571.0, 533.0, 537.0, 504.0, 503.0, 516.0, 488.0, 471.0, 485.0, 470.0, 448.0, 457.0, 448.0, 438.0, 425.0]</t>
-  </si>
-  <si>
-    <t>[903.0, 852.0, 831.0, 786.0, 811.0, 772.0, 803.0, 757.0, 725.0, 666.0, 736.0, 694.0, 559.0, 654.0, 598.0, 573.0]</t>
-  </si>
-  <si>
-    <t>[670.0, 780.0, 707.0, 609.0, 662.0, 620.0, 607.0, 712.0, 632.0, 647.0, 602.0, 584.0, 564.0, 591.0, 523.0, 502.0]</t>
-  </si>
-  <si>
-    <t>[834.0, 809.0, 794.0, 770.0, 764.0, 757.0, 749.0, 740.0, 726.0, 727.0, 705.0, 674.0, 660.0, 628.0, 626.0, 613.0]</t>
-  </si>
-  <si>
-    <t>[602.0, 585.0, 544.0, 477.0, 457.0, 472.0, 457.0, 445.0, 438.0, 428.0, 427.0, 382.0, 401.0, 388.0, 367.0, 384.0]</t>
-  </si>
-  <si>
-    <t>[809.0, 796.0, 786.0, 751.0, 757.0, 736.0, 741.0, 718.0, 710.0, 719.0, 688.0, 648.0, 621.0, 606.0, 606.0, 602.0]</t>
-  </si>
-  <si>
-    <t>[936.0, 883.0, 863.0, 842.0, 824.0, 824.0, 809.0, 807.0, 799.0, 787.0, 774.0, 750.0, 744.0, 706.0, 707.0, 675.0]</t>
-  </si>
-  <si>
-    <t>[762.0, 736.0, 704.0, 704.0, 689.0, 674.0, 675.0, 651.0, 640.0, 648.0, 637.0, 616.0, 601.0, 591.0, 578.0, 570.0]</t>
-  </si>
-  <si>
-    <t>[793.0, 769.0, 723.0, 729.0, 711.0, 697.0, 695.0, 667.0, 664.0, 678.0, 659.0, 641.0, 621.0, 608.0, 597.0, 583.0]</t>
-  </si>
-  <si>
-    <t>[706.0, 682.0, 618.0, 566.0, 598.0, 522.0, 620.0, 591.0, 622.0, 611.0, 600.0, 543.0, 553.0, 528.0, 515.0, 510.0]</t>
-  </si>
-  <si>
-    <t>[868.0, 853.0, 834.0, 844.0, 820.0, 835.0, 824.0, 792.0, 792.0, 754.0, 765.0, 735.0, 696.0, 679.0, 663.0, 657.0]</t>
-  </si>
-  <si>
-    <t>[602.0, 598.0, 574.0, 605.0, 522.0, 537.0, 553.0, 505.0, 493.0, 497.0, 501.0, 493.0, 456.0, 452.0, 410.0, 430.0]</t>
-  </si>
-  <si>
-    <t>[724.0, 710.0, 685.0, 679.0, 664.0, 645.0, 650.0, 634.0, 618.0, 618.0, 615.0, 596.0, 581.0, 574.0, 549.0, 547.0]</t>
-  </si>
-  <si>
-    <t>[735.0, 671.0, 691.0, 681.0, 616.0, 597.0, 652.0, 645.0, 660.0, 605.0, 605.0, 540.0, 579.0, 576.0, 588.0, 536.0]</t>
-  </si>
-  <si>
-    <t>[829.0, 807.0, 787.0, 751.0, 739.0, 738.0, 736.0, 712.0, 691.0, 690.0, 709.0, 672.0, 651.0, 631.0, 613.0, 606.0]</t>
-  </si>
-  <si>
-    <t>[620.0, 595.0, 580.0, 547.0, 546.0, 524.0, 519.0, 520.0, 508.0, 511.0, 508.0, 486.0, 484.0, 469.0, 457.0, 475.0]</t>
-  </si>
-  <si>
-    <t>[516.0, 500.0, 468.0, 462.0, 459.0, 434.0, 426.0, 396.0, 413.0, 453.0, 410.0, 414.0, 416.0, 406.0, 373.0, 345.0]</t>
+    <t>[184.0, 175.16842105263163, 173.70345217883425, 179.12353109773585, 161.38271604938268, 166.27503649635037, 178.59970370370377, 165.5987897125567, 178.89825218476904, 190.06218274111677, 187.06291495415746, 184.53578463558756, 178.53274814314648, 176.58626699198328, 186.56576576576572, 195.71206513693562]</t>
+  </si>
+  <si>
+    <t>[390.0, 399.50692520775624, 411.23769100169784, 410.1822871883062, 387.53086419753095, 405.97021897810214, 413.0802962962964, 367.0027231467475, 384.3426966292134, 400.06916243654837, 404.52355358836553, 399.4228496388705, 392.0229574611749, 386.68525618682474, 423.77081081081064, 411.9533678756477]</t>
+  </si>
+  <si>
+    <t>[369.0, 401.5556786703603, 410.19128466327106, 384.7446259673259, 382.2222222222222, 391.9340145985402, 431.7072592592592, 439.73192133131624, 452.43945068664175, 444.651649746193, 469.9955738223207, 428.56007879185836, 436.9682646860231, 412.4642732659463, 461.0839639639639, 470.80384900074023]</t>
+  </si>
+  <si>
+    <t>[349.0, 409.75069252077583, 409.1448783248445, 367.78618515333915, 347.1851851851852, 381.1369343065694, 429.5158518518517, 457.63449319213305, 457.05617977528095, 448.1713197969543, 473.503003477711, 454.0551543007223, 421.9864956110737, 422.77588009759484, 458.41873873873874, 442.06291635825323]</t>
+  </si>
+  <si>
+    <t>[752.0, 507.06648199446, 568.1986417657045, 439.8595586127833, 715.6049382716049, 491.2671532846714, 597.1585185185186, 736.2432677760969, 714.4388264669165, 622.9815989847716, 462.9807145115394, 463.76756401838475, 605.5131667792034, 631.5859184384803, 752.9261261261258, 674.7276091783867]</t>
+  </si>
+  <si>
+    <t>[288.0, 362.6293628808867, 335.89643463497464, 365.66638005159075, 227.20987654320993, 305.5573722627737, 509.5022222222224, 388.2620272314673, 440.89762796504374, 307.38451776649754, 376.4641163452418, 418.84766907419566, 373.2957461174883, 283.56918787033806, 391.78810810810796, 279.1976313841599]</t>
+  </si>
+  <si>
+    <t>[490.0, 470.18891966758997, 630.9830220713072, 365.66638005159075, 503.25925925925935, 576.5640875912409, 580.722962962963, 596.3794251134645, 604.7915106117355, 567.8401015228426, 674.5956370534302, 586.386736703874, 620.4949358541526, 580.027884280237, 723.6086486486486, 502.28201332346407]</t>
+  </si>
+  <si>
+    <t>[193.0, 274.5329639889196, 79.52688172043008, 269.2152479220408, 248.44444444444434, 237.5357664233577, 233.384888888889, 58.18335854765496, 362.4132334581773, 442.3052030456854, 445.44356623458725, 282.87393302692067, 239.7083051991899, 574.8720808644127, 425.10342342342324, 214.87268689859366]</t>
+  </si>
+  <si>
+    <t>[522.0, 509.1152354570638, 536.8064516129032, 638.061335626254, 577.5802469135804, 490.18744525547436, 456.9084444444445, 574.0012102874432, 604.7915106117352, 565.4936548223352, 598.6013278533039, 659.2298095863428, 657.9493585415262, 636.7417218543046, 743.5978378378377, 671.9903774981497]</t>
+  </si>
+  <si>
+    <t>[431.0, 479.40831024930753, 475.0684776457274, 234.23846374319305, 559.530864197531, 319.59357664233585, 261.8731851851853, 240.56580937972785, 332.40449438202245, 558.4543147208124, 346.0663926651912, 616.7380170715694, 529.3558406482107, 462.7333565702336, 401.11639639639634, 506.38786084381945]</t>
+  </si>
+  <si>
+    <t>[202.0, 288.87423822714686, 241.71986417657058, 188.6626540556033, 95.55555555555543, 163.03591240875903, 432.80296296296297, 382.66747352496213, 397.0387016229713, 415.32106598984774, 299.3006639266521, 388.4963887065003, 318.3625928426741, 335.1272220285814, 275.8508108108108, 619.9829755736491]</t>
+  </si>
+  <si>
+    <t>[318.0, 325.75180055401665, 259.50877192982466, 352.9475494411008, 284.5432098765432, 445.91941605839406, 563.1917037037038, 527.0069591527988, 298.93320848938833, 397.7227157360405, 465.3190009484665, 498.97504924491136, 322.10803511141125, 408.5974207040781, 355.8075675675675, 402.3730569948186]</t>
+  </si>
+  <si>
+    <t>[214.0, 225.36288088642664, 231.25580079230338, 148.38635712238465, 224.0246913580247, 195.4271532846716, 156.68562962962972, 151.0529500756429, 196.21098626716605, 178.3299492385786, 129.77489724944667, 178.46552856204858, 225.97501688048624, 246.18961310561178, 153.25045045045044, 166.97113249444863]</t>
+  </si>
+  <si>
+    <t>[398.0, 320.629916897507, 372.52065647990935, 281.93407853253075, 247.38271604938268, 202.98510948905118, 387.8791111111111, 324.48411497730694, 400.5012484394508, 357.8331218274111, 512.0847296870058, 426.1319763624424, 454.4469952734639, 387.9742070407808, 255.86162162162168, 266.88008882309396]</t>
+  </si>
+  <si>
+    <t>[221.0, 297.0692520775623, 357.8709677419356, 332.80940097449127, 117.85185185185173, 306.63708029197096, 249.82044444444455, 529.2447806354011, 444.360174781523, 224.08565989847716, 346.0663926651913, 288.94418910045954, 283.40513166779203, 181.74207040780766, 191.8962162162162, 288.77794226498884]</t>
+  </si>
+  <si>
+    <t>[279.0, 234.5822714681442, 223.9309564233165, 187.6027515047291, 174.12345679012356, 157.63737226277385, 293.64859259259254, 277.48986384266277, 286.2372034956304, 292.13261421319794, 447.78185267151434, 182.10768220617206, 272.16880486158016, 265.523875914953, 327.8227027027026, 106.75203552923767]</t>
+  </si>
+  <si>
+    <t>[278.0, 343.1662049861495, 371.47425014148257, 342.34852393235883, 348.2469135802469, 306.63708029197096, 352.81659259259254, 322.246293494705, 361.2590511860176, 324.9828680203045, 329.6983876067027, 363.00131319763625, 382.0351114112086, 333.83827117462533, 347.81189189189195, 369.5262768319765]</t>
+  </si>
+  <si>
+    <t>[-2.0, -6.146260387811594, 185.213921901528, -104.93035253654341, 174.12345679012356, -63.70277372262774, 6.574222222222147, 88.39394856278363, 160.43133583021222, 220.56598984771574, 29.228580461587057, 69.20091923834536, -2.4969615124915663, 286.1470895782502, 434.4317117117116, 194.3434492968173]</t>
+  </si>
+  <si>
+    <t>[205.0, 344.1905817174518, 255.32314657611778, 181.24333619948402, 452.2962962962963, 318.5138686131386, 230.09777777777776, 380.42965204236, 450.1310861423219, 227.6053299492387, 294.6240910527981, 370.2856204858831, 434.4713031735314, 491.0902753572673, 390.4554954954956, 396.89859363434493]</t>
+  </si>
+  <si>
+    <t>[296.0, 331.89806094182836, 442.6298811544991, 378.3852106620809, 251.62962962962956, 258.0502189781023, 387.87911111111134, 328.95975794251126, 369.3383270911361, 337.8883248730963, 315.6686689851406, 398.20879842416275, 394.51991897366656, 371.2178459393516, 345.14666666666653, 390.0555144337527]</t>
+  </si>
+  <si>
+    <t>[440.0, 699.6493074792244, 796.3152235427277, 747.2312983662941, 672.0740740740741, 449.1585401459856, 565.383111111111, 664.6329803328292, 790.6148564294633, 424.7068527918782, 508.57730003161555, 400.6369008535785, 885.1728561782581, 452.4217497385848, 529.0472072072073, 604.9282013323466]</t>
+  </si>
+  <si>
+    <t>[495.0, 383.1168975069253, 423.7945670628185, 296.7727142447693, 289.85185185185196, 321.7529927007299, 245.43762962962955, 577.3579425113464, 382.034332084894, 427.0532994923858, 357.75782484982597, 346.00459619172693, 473.1742066171506, 246.18961310561178, 407.7794594594594, 611.7712805329387]</t>
+  </si>
+  <si>
+    <t>[401.0, 386.190027700831, 382.98471986417667, 402.762969332187, 358.8641975308641, 378.9775182481752, 371.4435555555557, 326.72193645990933, 322.01685393258435, 364.87246192893394, 353.0812519759721, 379.9980302035457, 365.8048615800135, 342.8609271523178, 375.79675675675674, 364.05181347150267]</t>
+  </si>
+  <si>
+    <t>[259.0, 324.72742382271485, 201.95642331635554, 273.4548581255376, 286.66666666666674, 300.1588321167885, 293.64859259259265, 271.8953101361574, 246.9950062421974, 181.84961928934013, 271.2412266835281, 299.8706500328301, 234.71438217420678, 215.25479261066562, 243.86810810810812, 306.56994818652856]</t>
+  </si>
+  <si>
+    <t>[217.0, 180.2903047091413, 161.14657611771372, 210.92060762396113, 205.9753086419753, 287.2023357664234, 235.57629629629628, 102.93978819969743, 76.17602996254686, 99.72398477157367, 301.63895036357894, 235.52593565331563, 243.4537474679271, 148.22934820494947, 193.2288288288289, 194.3434492968172]</t>
+  </si>
+  <si>
+    <t>[250.0, 327.8005540166207, 324.38596491228054, 356.1272570937231, 296.2222222222222, 396.25284671532836, 341.85955555555574, 243.92254160363086, 167.35642946317103, 280.4003807106601, 238.50521656655087, 231.88378200919237, 172.2903443619175, 363.4841408156153, 373.13153153153144, 453.0118430792006]</t>
+  </si>
+  <si>
+    <t>[99.0, 220.24099722991684, 66.97000565930944, 240.5978790484379, 225.08641975308637, 127.40554744525548, 113.95318518518525, -61.5400907715582, 166.20224719101134, 85.64530456852799, 29.228580461586944, 171.18122127380184, 153.56313301823081, -63.158591843847944, 49.306666666666615, 57.48186528497422]</t>
+  </si>
+  <si>
+    <t>[269.0, 216.14349030470908, 336.9428409734014, 206.68099742046434, 270.7407407407409, 280.72408759124096, 243.2462222222223, 227.1388804841149, 292.00811485642953, 301.5184010152284, 333.205817262093, 336.29218647406447, 260.93247805536794, 242.32276054374347, 345.14666666666676, 365.42042931162086]</t>
+  </si>
+  <si>
+    <t>[201.0, 182.33905817174514, 209.2812676853423, 330.689595872743, 196.41975308641963, 260.20963503649637, 231.1934814814815, 132.03146747352503, 208.90699126092386, 293.30583756345163, 263.05722415428386, 257.3788575180565, 310.87170830519926, 304.19240153363535, 170.57441441441438, 269.6173205033308]</t>
+  </si>
+  <si>
+    <t>[91.0, 7.170637119113508, -15.696095076400638, 6.359415305245079, 57.33333333333337, 5.398540145985407, -24.105481481481547, 73.84810892586984, -43.85892634207244, 55.14149746192902, 0.0, 132.33158240315163, 56.181634031060184, 77.3370512373649, 190.5636036036035, 45.1643227239083]</t>
+  </si>
+  <si>
+    <t>[61.0, 35.85318559556788, 162.19298245614038, 85.85210662080829, 56.271604938271594, 172.7532846715328, 12.05274074074066, 116.36671709531015, 88.87203495630467, 105.59010152284259, 38.58172620929497, 12.140512147078084, 26.21809588116139, 126.317183687696, 41.310990990990945, 68.4307920059216]</t>
+  </si>
+  <si>
+    <t>[667.0, 721.1612188365652, 786.8975664968873, 786.4476927486389, 811.1604938271607, 814.0998540145988, 954.3579259259261, 844.7776096822995, 807.9275905118602, 886.9568527918784, 858.1511223521973, 787.919238345371, 1039.9844699527348, 882.9313349599163, 954.1506306306308, 936.1332346410068]</t>
+  </si>
+  <si>
+    <t>[440.0, 360.5806094182824, 488.6717600452746, 208.80080252221273, 345.06172839506166, 453.47737226277377, 459.0998518518518, 283.08441754916794, 500.9151061173534, 569.0133248730963, 427.9064179576351, 488.0485883125409, 696.6522619851453, 507.8466364586966, 606.3387387387386, 281.9348630643967]</t>
+  </si>
+  <si>
+    <t>[301.0, 273.5085872576177, 231.2558007923035, 251.19690455717978, 259.06172839506166, 219.1807299270073, 301.31851851851854, 268.53857791225425, 234.29900124843937, 272.18781725888323, 236.16693012962378, 270.73342087984236, 257.18703578663064, 266.8128267689092, 302.503063063063, 268.2487046632125]</t>
+  </si>
+  <si>
+    <t>[350.0, 211.0216066481994, 213.46689303904918, 276.6345657781601, 282.41975308641963, 256.97051094890503, 340.763851851852, 296.51134644478066, 342.79213483146054, 366.04568527918786, 220.96806828959848, 336.29218647406447, 390.77447670492916, 320.94876263506444, 367.80108108108107, 318.8874907475945]</t>
+  </si>
+  <si>
+    <t>[166.0, 155.70526315789482, 151.7289190718734, 127.18830610490113, 148.64197530864192, 95.01430656934303, 226.81066666666675, 99.5830559757942, 107.33895131086138, 174.8102791878173, 143.80461587100854, 110.47866053841108, 119.85415259959473, 123.73928197978398, 187.89837837837854, 117.70096225018506]</t>
+  </si>
+  <si>
+    <t>[134.0, 138.29085872576184, 75.3412563667232, 151.56606477500713, 131.65432098765427, 115.5287591240874, 78.89066666666668, 67.13464447806359, 84.25530586766536, 103.24365482233497, 87.68574138476129, 122.61917268548927, 74.90884537474699, 130.18403624956431, 174.57225225225216, 108.12065136935598]</t>
+  </si>
+  <si>
+    <t>[255.0, 315.5080332409973, 365.1958121109225, 219.3998280309545, 343.9999999999999, 351.9848175182482, 205.99229629629633, 409.52133131618757, 245.8408239700375, 276.88071065989845, 164.84919380335123, 366.64346684175973, 315.8656313301824, 188.1868246775881, 291.84216216216214, 279.19763138416]</t>
+  </si>
+  <si>
+    <t>[154.0, 223.3141274238227, 196.72439162422188, 154.74577242762984, 163.50617283950623, 252.65167883211677, 186.26962962962966, 155.52859304084734, 165.04806491885154, 217.04631979695432, 203.43092001264608, 228.241628365069, 260.93247805536816, 193.34262809341226, 231.87459459459456, 258.6683937823834]</t>
+  </si>
+  <si>
+    <t>[237.0, 322.6786703601109, 361.0101867572156, 191.8423617082259, 220.8395061728395, 247.25313868613148, 189.55674074074068, 256.2305597579425, 281.6204744069913, 265.1484771573605, 181.21719886184007, 239.16808929743934, 192.26603646185015, 344.149878006274, 229.20936936936937, 272.35455218356776]</t>
+  </si>
+  <si>
+    <t>[381.0, 403.6044321329639, 268.926428975665, 324.330180567498, 290.9135802469134, 313.1153284671532, 8.76562962962953, 111.89107413010561, 375.1092384519352, 561.9739847715734, 312.1612393297503, 344.7905449770192, 201.00540175557035, 146.94039735099318, 335.8183783783784, 231.29607698001473]</t>
+  </si>
+  <si>
+    <t>[836.0, 530.6271468144043, 907.2342954159592, 404.8827744339353, 802.6666666666665, 637.0277372262774, 746.1742222222224, 456.5155824508322, 761.7602996254682, 804.8312182741115, 796.1865317736324, 891.1135915955354, 646.7130317353142, 938.356221680028, 1194.0209009009006, 941.6076980014807]</t>
+  </si>
+  <si>
+    <t>[115.0, 119.85207756232694, 123.475947934352, 131.4279163083977, 121.03703703703695, 161.956204379562, 112.8574814814815, 52.588804841149795, 186.97752808988776, 64.52728426395925, 183.55548529876705, 148.1142481943532, 128.5935178933155, 104.40501917044276, 181.23531531531535, 162.86528497409313]</t>
+  </si>
+  <si>
+    <t>[-92.0, 221.26537396121898, 247.99830220713068, 310.55144740613366, 63.703703703703695, 131.72437956204374, 110.66607407407412, 48.11316187594559, 185.82334581772795, 157.21192893401007, 224.4754979449889, 298.6565988181221, 6.2424037812289725, 143.0735447891251, 70.62846846846855, 98.54034048852691]</t>
+  </si>
+  <si>
+    <t>[171.0, 371.848753462604, 230.2093944538766, 209.86070507308693, 229.33333333333348, 53.98540145985396, 239.95911111111104, 100.70196671709527, 94.64294631710368, 146.65291878172593, 130.94404046791033, 248.8804990151018, 78.65428764348417, 237.1669571279191, 166.5765765765766, 206.66099185788312]</t>
+  </si>
+  <si>
+    <t>[130.0, 109.60831024930746, 113.01188455008486, 129.30811120664941, 129.53086419753083, 111.20992700729931, 118.33600000000001, 132.03146747352497, 138.50187265917606, 124.36167512690355, 139.12804299715458, 132.33158240315174, 129.84199864956105, 127.60613454165212, 135.9264864864865, 132.75573649148788]</t>
+  </si>
+  <si>
+    <t>[113.0, 65.56011080332405, 86.85172608941707, 92.21152192605336, 72.19753086419746, 64.78248175182478, 56.97659259259251, 42.5186081694402, 57.70911360799005, 93.85786802030452, 61.96459057856464, 91.05384110308592, 106.12086428089128, 18.04531195538516, 67.96324324324326, 99.90895632864544]</t>
+  </si>
+  <si>
+    <t>[45.0, 92.19390581717454, 37.6706281833616, 73.13327601031813, 65.82716049382714, 52.905693430656925, 69.0293333333334, 62.659001512859334, 70.4051186017478, 104.41687817258884, 71.31773632627255, 101.9803020354563, 94.88453747467935, 27.067967933077682, 49.30666666666667, 90.32864544781648]</t>
+  </si>
+  <si>
+    <t>[309.0, 208.97285318559568, 173.70345217883414, 207.74089997133842, 285.60493827160496, 195.4271532846716, 200.51377777777782, 218.1875945537065, 223.91136079900127, 233.4714467005076, 233.8286436926968, 201.5325016414971, 224.7265361242404, 277.1244336005577, 234.53981981981974, 220.34715025906735]</t>
+  </si>
+  <si>
+    <t>[165.0, 159.80277008310247, 126.61516694963211, 98.57093723129844, 72.19753086419757, 140.36204379562048, 136.96296296296305, 152.171860816944, 114.2640449438203, 120.84200507614207, 140.29718621561813, 131.11753118844388, 137.3328831870358, 130.18403624956431, 127.93081081081084, 205.29237601776458]</t>
+  </si>
+  <si>
+    <t>[315.0, 39.95069252077565, 73.24844368986987, -8.479220406993363, 318.5185185185185, 163.03591240875926, 220.2364444444446, 11.189107413010788, 253.9200998751561, 194.75507614213188, 231.4903572557697, 140.82994090610634, 157.30857528696833, 143.0735447891252, 5.330450450450371, 53.37601776461884]</t>
+  </si>
+  <si>
+    <t>[130.0, 69.65761772853193, 84.75891341256363, 81.6124964173116, 79.62962962962968, 52.905693430656925, 39.44533333333334, 78.32375189107404, 64.63420724094885, 68.04695431472078, 72.48687954473598, 71.6290216677611, 102.37542201215388, 132.76193795747645, 70.62846846846844, 110.85788304959294]</t>
+  </si>
+  <si>
+    <t>[60.0, 44.048199445983414, 59.64516129032256, 71.01347090856979, 46.71604938271605, 39.94919708029198, 48.210962962962924, 43.637518910741335, 41.550561797752835, 44.582487309644705, 65.4720202339551, 48.56204858831251, 42.44834571235651, 43.82432903450683, 59.967567567567585, 64.32494448556622]</t>
+  </si>
+  <si>
+    <t>[81.0, 46.09695290858724, 39.76344086021504, 28.617368873602743, 11.679012345679041, 31.31153284671535, 46.0195555555556, 48.113161875945536, 23.083645443195962, 34.023477157360446, 47.93487195700288, 43.70584372948127, 46.19378798109386, 46.402230742418965, 49.30666666666667, 42.42709104367134]</t>
+  </si>
+  <si>
+    <t>[40.0, 39.95069252077559, 19.88172043010752, 27.5574663227286, 10.617283950617264, 12.956496350364944, 55.88088888888893, 22.37821482602118, 26.546192259675365, 21.118020304568574, 35.0742965539045, 38.84963887065004, 12.484807562457831, 7.733705123736513, -5.330450450450428, 32.84678016284232]</t>
+  </si>
+  <si>
+    <t>[41.0, 87.0720221606648, 212.42048670062252, 80.5525938664374, 185.80246913580243, 119.84759124087589, 108.47466666666668, 98.46414523449323, 147.73533083645447, 166.59771573604058, 162.51090736642425, 178.46552856204858, 128.59351789331532, 6.4447542697804465, 119.93513513513517, 143.70466321243526]</t>
+  </si>
+  <si>
+    <t>[73.0, 59.41385041551251, 65.92359932088289, 95.39122957867585, 91.30864197530866, 52.90569343065698, 65.74222222222227, 86.15612708018153, 79.63857677902615, 65.70050761421322, 80.67088207398041, 66.77281680892975, 66.16948008102634, 67.02544440571626, 95.94810810810804, 91.69726128793485]</t>
+  </si>
+  <si>
+    <t>[127.0, 112.68144044321332, 98.36219581211088, 103.87044998566927, 110.4197530864198, 95.01430656934303, 102.99614814814811, 107.41543116490169, 117.72659176029964, 117.32233502538071, 122.76003793866579, 116.54891661195006, 102.37542201215393, 108.2718717323109, 102.61117117117124, 125.91265729089571]</t>
+  </si>
+  <si>
+    <t>[116.0, 95.26703601108034, 92.08375778155067, 125.06850100315279, 132.71604938271605, 106.89109489051094, 112.85748148148144, 107.41543116490169, 108.49313358302123, 109.10977157360406, 112.23774897249444, 105.62245567957979, 89.89061444969616, 100.53816660857439, 109.27423423423426, 97.17172464840866]</t>
+  </si>
+  <si>
+    <t>[102.0, 70.68199445983379, 73.24844368986987, 72.07337345944399, 4.246913580246883, 65.86218978102193, 32.871111111111134, 90.63177004538579, 91.18039950062416, 85.64530456852799, 75.99430920012645, 99.55219960604069, 69.91492234976369, 79.9149529452771, 103.94378378378377, 73.90525536639524]</t>
+  </si>
+  <si>
+    <t>[121.0, 111.6570637119114, 137.07923033389926, 129.30811120664947, 161.38271604938274, 91.77518248175181, 154.49422222222228, 156.64750378214825, 100.41385767790263, 153.6922588832487, 175.37148276952257, 213.6730137885752, 147.320729237002, 130.18403624956431, 159.91351351351352, 145.07327905255363]</t>
+  </si>
+  <si>
+    <t>[150.0, 165.94903047091418, 163.23938879456705, 158.9853826311264, 155.01234567901236, 152.23883211678833, 173.12118518518525, 152.1718608169441, 160.43133583021222, 172.46383248730967, 181.21719886184007, 199.10439921208138, 197.25995948683328, 219.12164517253404, 209.22018018018014, 213.50407105847523]</t>
+  </si>
+  <si>
+    <t>[298.0, 332.9224376731303, 328.57159026598754, 320.0905703640012, 287.7283950617284, 290.4414598540146, 347.33807407407403, 285.32223903177, 333.55867665418225, 314.4238578680204, 327.3601011697755, 361.7872619829284, 342.0837272113438, 359.617288253747, 377.12936936936933, 381.84381939304217]</t>
+  </si>
+  <si>
+    <t>[239.0, 258.14293628808866, 237.53423882286359, 223.63943823445118, 210.22222222222229, 179.23153284671537, 212.56651851851848, 179.02571860816943, 235.45318352059917, 202.96763959390876, 263.05722415428386, 252.5226526592253, 244.70222822417293, 255.21226908330425, 309.1661261261261, 286.0407105847521]</t>
+  </si>
+  <si>
+    <t>[5.0, 72.73074792243767, 75.34125636672326, 69.95356835769559, 26.543209876543187, 50.746277372262796, 35.062518518518516, 42.518608169440256, 39.242197253433176, 71.56662436548226, 58.45716092317417, 78.91332895600789, 74.90884537474682, 86.35970721505754, 89.28504504504502, 32.84678016284238]</t>
+  </si>
+  <si>
+    <t>[221.0, 185.4121883656511, 226.02376910016972, 211.98051017483522, 219.77777777777783, 252.6516788321169, 265.1602962962963, 172.31225416036307, 265.46192259675405, 212.3534263959391, 213.95320897881766, 278.0177281680893, 239.70830519918974, 264.23492506099683, 281.1812612612613, 296.9896373056995]</t>
+  </si>
+  <si>
+    <t>[-103.0, 13.316897506925216, 36.62422184493494, 451.5184866723989, 180.49382716049388, 147.91999999999996, 112.85748148148139, 211.47413010590003, 68.09675405742826, 415.32106598984774, 87.68574138476129, 263.4491135915955, 283.40513166779203, 369.92889508539577, 398.45117117117115, 391.42413027387124]</t>
+  </si>
+  <si>
+    <t>[239.0, 269.41108033241005, 512.7391058290888, 329.6296933218689, 263.30864197530866, 319.59357664233585, 421.84592592592605, 411.7591527987897, 373.9550561797754, 197.1015228426396, 399.84698071451146, 382.4261326329612, 295.88993923024975, 366.06204252352734, 473.0774774774774, 509.1250925240563]</t>
+  </si>
+  <si>
+    <t>[412.0, 440.4819944598339, 393.44878324844376, 474.83634279163084, 233.58024691358025, 266.6878832116789, 182.98251851851853, 219.30650529500758, 301.24157303370794, 221.73921319796966, 135.62061334176417, 274.37557452396584, 389.5259959486833, 349.30568142209836, 179.90270270270264, 138.23019985196152]</t>
+  </si>
+  <si>
+    <t>[230.0, 272.4842105263157, 280.43689869835885, 157.92548008025233, 262.2469135802469, 293.68058394160585, 371.44355555555546, 102.93978819969743, 162.73970037453194, 293.30583756345186, 254.8732216250395, 233.09783322390024, 322.10803511141137, 287.4360404322065, 187.89837837837842, 372.2635085122133]</t>
+  </si>
+  <si>
+    <t>[381.0, 349.31246537396134, 462.51160158460664, 335.98910862711375, 281.3580246913581, 185.7097810218978, 384.5920000000001, 353.57579425113477, 340.48377028714106, 227.60532994923858, 315.6686689851408, 395.78069599474725, 398.26536124240386, 351.8835831300106, 227.87675675675666, 472.17246484085865]</t>
+  </si>
+  <si>
+    <t>[27.0, 45.07257617728533, 40.809847198641705, 49.81541989108632, 67.95061728395058, 48.58686131386867, 77.79496296296293, 59.302269288956154, 50.78401997503124, 64.52728426395936, 71.31773632627255, 59.48850952068278, 77.40580688723844, 92.80446148483793, 86.61981981981978, 97.1717246484086]</t>
+  </si>
+  <si>
+    <t>[39.0, 27.658171745152345, 77.43406904357676, -2.119805101748284, 76.44444444444446, 87.45635036496344, 74.5078518518518, -2.2378214826021576, 56.55493133583025, 51.62182741116749, 49.10401517546643, 78.91332895600794, 31.21201890614452, 37.379574764726385, 27.984864864864903, 113.59511472982979]</t>
+  </si>
+  <si>
+    <t>[9.0, 76.82825484764544, 55.459535936615794, 91.15161937517917, 97.6790123456791, 24.83328467153285, 108.47466666666662, 66.01573373676251, 32.31710362047431, 35.19670050761431, 45.596585520075905, 105.62245567957973, 102.37542201215399, 153.38515162077385, 89.28504504504497, 78.01110288675056]</t>
+  </si>
+  <si>
+    <t>[-13.0, 54.291966759002776, 19.88172043010752, 52.995127543708804, 89.18518518518522, 78.81868613138681, 87.65629629629632, 1.1189107413009651, 20.775280898876417, 24.637690355329937, 40.92001264622195, 27.92317793827965, 118.60567184334911, 52.84698501219941, -11.993513513513449, 73.9052553663953]</t>
+  </si>
+  <si>
+    <t>[201.0, 63.511357340720224, 65.92359932088289, 110.22986529091429, 100.8641975308642, 140.36204379562048, 209.27940740740746, 114.12889561270799, 111.9556803995007, 156.03870558375627, 168.35662345874175, 118.97701904136579, 143.57528696826466, 73.4701986754967, 246.5333333333333, 83.48556624722426]</t>
+  </si>
+  <si>
+    <t>[175.0, 111.6570637119114, 93.13016411997728, 177.00372599598745, 184.74074074074065, 144.68087591240885, 130.3887407407409, 139.86384266263246, 63.48002496878894, 42.236040609137035, 159.00347771103395, 157.82665791201578, 144.8237677245105, 181.74207040780766, 121.26774774774765, 23.266469282013304]</t>
+  </si>
+  <si>
+    <t>[214.0, 250.97229916897516, 177.88907753254102, 260.73602751504745, 303.6543209876544, 187.869197080292, 198.32237037037032, 217.06868381240542, 184.66916354556804, 333.1954314720813, 201.09263357571922, 275.5896257386736, 249.69615124915606, 150.8072499128616, 205.22234234234224, 165.6025166543302]</t>
+  </si>
+  <si>
+    <t>[64.0, 20.487534626038837, 19.88172043010752, 40.27629693321876, 28.666666666666742, 24.83328467153285, 60.263703703703754, 31.32950075642964, 40.396379525593034, 15.251903553299485, 50.27315839392975, 16.99671700590943, 63.67251856853477, 69.6033461136285, 57.302342342342286, 45.164322723908185]</t>
+  </si>
+  <si>
+    <t>[-12.0, 33.80443213296394, 7.324844368986987, 32.85697907709948, -10.61728395061732, 20.51445255474448, 35.06251851851846, -14.545839636913797, -27.700374531835223, 7.039340101522839, 4.6765728738539565, 8.498358502954716, 39.95138419986495, 50.269083304287165, 23.98702702702701, 30.109548482605533]</t>
+  </si>
+  <si>
+    <t>[150.0, 119.85207756232683, 128.70797962648555, 109.16996274004009, 133.77777777777783, 102.57226277372274, 151.2071111111111, 118.6045385779122, 78.48439450686647, 55.14149746192891, 142.6354726525451, 117.76296782665793, -31.21201890614452, 122.4503311258278, 63.96540540540536, 57.481865284974106]</t>
+  </si>
+  <si>
+    <t>[-31.0, 112.68144044321332, 61.737973967176, -13.778733161364244, 38.22222222222217, 25.912992700729887, 7.669925925925895, 132.0314674735249, 40.39637952559292, 62.18083756345186, 23.38286436926967, 41.2777413000656, 37.454422687373494, 105.69397002439871, 31.98270270270268, 0.0]</t>
+  </si>
+  <si>
+    <t>[196.0, 235.606648199446, 223.9309564233164, 201.38148466609357, 270.74074074074076, 193.2677372262774, 218.0450370370371, 251.7549167927383, 218.14044943820227, 217.04631979695432, 114.57603540942148, 163.89691398555476, 177.28426738690075, 183.03102126176373, 230.54198198198196, 224.45299777942262]</t>
+  </si>
+  <si>
+    <t>[119.0, 116.77894736842114, 82.6661007357103, 42.39610203496704, 87.06172839506172, 112.28963503649635, 87.65629629629632, 82.79939485627835, 79.63857677902621, 65.70050761421322, 40.92001264622195, 41.27774130006566, 73.66036461850103, 78.62600209132103, 59.967567567567585, 90.32864544781643]</t>
+  </si>
+  <si>
+    <t>[24.0, -6.146260387811708, 153.82173174872662, 49.81541989108621, 70.07407407407402, 88.5360583941607, 19.72266666666667, 118.6045385779122, 73.86766541822726, 53.9682741116751, -68.97944988934557, 91.05384110308603, 109.86630654962869, 162.40780759846632, 135.9264864864864, 143.7046632124352]</t>
+  </si>
+  <si>
+    <t>[113.0, 150.58337950138502, 83.71250707413697, 85.85210662080829, 105.11111111111109, 123.08671532846722, 56.976592592592624, 62.65900151285939, 133.8851435705368, 167.77093908629445, -5.845716092317502, 29.137229152987516, 58.67859554355175, 19.334262809341226, 127.93081081081084, 62.9563286454478]</t>
+  </si>
+  <si>
+    <t>[201.0, 195.65595567867047, 181.02829654782113, 203.50128976784185, 196.41975308641986, 190.02861313868607, 199.41807407407418, 185.7391830559758, 192.74843945068665, 206.48730964467006, 204.60006323110974, 217.31516743269867, 218.48413234301154, 220.4105960264901, 229.20936936936926, 223.0843819393042]</t>
+  </si>
+  <si>
+    <t>[218.0, 209.99722991689748, 205.09564233163553, 222.57953568357698, 221.90123456790127, 214.86189781021892, 218.0450370370371, 205.87957639939486, 211.21535580524346, 241.68401015228426, 227.9829276003794, 240.3821405121471, 235.9628629304525, 238.45590798187516, 255.86162162162168, 242.24500370096223]</t>
+  </si>
+  <si>
+    <t>[188.0, 97.31578947368428, 66.97000565930955, 23.317856119231806, 97.67901234567898, 34.55065693430663, 109.57037037037037, 158.88532526475035, 162.73970037453182, 146.65291878172593, 171.86405311413216, 116.54891661195006, 169.79338284942605, 112.13872429417916, 157.24828828828834, 145.07327905255374]</t>
+  </si>
+  <si>
+    <t>[189.0, 221.26537396121887, 261.6015846066779, 276.63456577816, 256.9382716049382, 272.0864233576642, 278.30874074074086, 280.8465960665658, 280.4662921348314, 282.7468274111675, 278.25608599430916, 278.0177281680893, 270.9203241053343, 248.76751481352392, 251.8637837837838, 286.040710584752]</t>
+  </si>
+  <si>
+    <t>[106.0, 83.99889196675895, 155.91454442558006, 130.3680137575236, 47.77777777777783, 116.60846715328472, 133.67585185185186, 93.98850226928892, 63.480024968788996, 96.20431472081219, 116.9143218463484, 117.76296782665793, 83.6482106684673, 87.64865806901366, 91.95027027027021, 93.06587712805327]</t>
+  </si>
+  <si>
+    <t>[186.0, 200.77783933518015, 151.72891907187318, 196.08197191172258, 163.50617283950612, 159.79678832116792, 178.59970370370365, 161.1231467473525, 197.36516853932585, 171.29060913705587, 187.06291495415746, 208.81680892974396, 208.49628629304527, 208.8100383408854, 185.23315315315313, 187.50037009622497]</t>
+  </si>
+  <si>
+    <t>[136.0, 157.75401662049865, 106.73344651952459, 115.52937804528517, 36.09876543209873, 44.268029197080295, 149.01570370370382, 73.84810892586995, 182.36079900124844, 91.51142131979702, 114.57603540942137, 77.69927774130008, 141.0783254557732, 154.67410247472992, 197.2266666666667, 90.32864544781648]</t>
+  </si>
+  <si>
+    <t>[270.0, 223.3141274238228, 164.28579513299383, 126.12840355402693, 205.9753086419753, 167.3547445255474, 218.0450370370371, 224.90105900151286, 229.68227215980028, 208.83375634517768, 195.24691748340183, 210.0308601444517, 268.42336259284275, 203.65423492506102, 182.56792792792794, 180.65729089563297]</t>
+  </si>
+  <si>
+    <t>[79.0, 97.31578947368428, 74.29485002829654, 97.51103468042419, 74.32098765432096, 111.20992700729931, 47.11525925925923, 116.36671709531021, 102.72222222222223, 105.59010152284264, 106.392032880177, 82.55548260013131, 89.89061444969616, 81.20390379923322, 73.29369369369363, 82.11695040710583]</t>
+  </si>
+  <si>
+    <t>[32.0, 38.926315789473676, 32.43859649122811, 40.2762969332187, 67.95061728395063, 19.434744525547444, 35.062518518518516, -1.1189107413010788, 27.700374531835223, 75.08629441624367, 49.104015175466316, 63.130663164806265, 61.17555705604326, 61.869640989891934, 53.30450450450451, -6.843079200592115]</t>
+  </si>
+  <si>
+    <t>[886.0, 880.9639889196677, 870.6100735710244, 857.4611636572085, 839.8271604938273, 837.8534306569344, 841.5004444444446, 845.8965204236007, 862.1741573033709, 867.0120558375635, 844.1214037306355, 843.7655942219304, 837.7305874409184, 839.1070059254096, 850.2068468468468, 848.5418208734272]</t>
+  </si>
+  <si>
+    <t>[1246.0, 1253.8371191135736, 1243.1307300509338, 1227.367153912296, 1207.1851851851852, 1222.229489051095, 1214.039703703704, 1210.661422087746, 1226.8957553058676, 1224.8451776649747, 1198.371798925071, 1209.1950098489822, 1207.2808912896694, 1207.7469501568492, 1223.3383783783784, 1213.9622501850483]</t>
+  </si>
+  <si>
+    <t>[1355.0, 1359.3479224376733, 1343.585738539898, 1333.3574089997137, 1302.7407407407409, 1304.2872992700732, 1283.069037037037, 1297.9364599092285, 1333.0805243445693, 1335.1281725888325, 1318.79355042681, 1311.1753118844385, 1304.6623902768401, 1285.084001394214, 1285.9711711711711, 1315.239822353812]</t>
+  </si>
+  <si>
+    <t>[1429.0, 1425.9324099722994, 1433.5766836445953, 1431.928346231012, 1374.9382716049383, 1387.4248175182483, 1367.4382222222223, 1384.09258698941, 1419.6441947565543, 1417.2538071065992, 1407.6484350300348, 1409.5134602757714, 1407.037812288994, 1395.9337748344371, 1401.9084684684683, 1400.0940044411548]</t>
+  </si>
+  <si>
+    <t>[2291.0, 2351.9689750692523, 2409.8737973967177, 2163.2611063341938, 2147.8765432098767, 2233.9159124087596, 2257.14962962963, 2196.421785173979, 2249.5012484394506, 2247.8959390862947, 2224.8795447360103, 2284.844386080105, 2340.9014179608375, 2363.935866155455, 2216.1347747747745, 2132.3034789045155]</t>
+  </si>
+  <si>
+    <t>[1338.0, 1360.3722991689751, 1324.7504244482172, 1335.4772141014619, 1354.7654320987656, 1479.2000000000003, 1384.9694814814816, 1332.6226928895612, 1427.723470661673, 1489.9936548223352, 1436.877015491622, 1482.3565331582404, 1454.4800810263337, 1416.5569884977344, 1504.5196396396395, 1554.7475943745376]</t>
+  </si>
+  <si>
+    <t>[1567.0, 1545.7844875346261, 1536.124504810413, 1549.5775293780455, 1491.7283950617284, 1499.7144525547446, 1529.6023703703706, 1575.4263237518912, 1540.8333333333335, 1560.3870558375636, 1572.497628833386, 1601.333552199606, 1643.0006752194465, 1591.8543046357618, 1616.459099099099, 1542.4300518134717]</t>
+  </si>
+  <si>
+    <t>[1877.0, 1887.9263157894738, 1818.6542161856253, 1831.5116079105765, 1836.7901234567903, 1865.735474452555, 1832.0165925925928, 1766.7600605143723, 1846.6916354556804, 2024.9835025380712, 1842.569712298451, 1885.4215364412344, 1791.5698852126943, 1840.6218194492856, 1917.6295495495494, 1917.4307920059218]</t>
+  </si>
+  <si>
+    <t>[1466.0, 1446.4199445983381, 1489.036219581211, 1492.34279163084, 1406.7901234567903, 1334.5191240875913, 1280.8776296296298, 1304.649924357035, 1416.181647940075, 1348.0336294416245, 1325.8084097375909, 1308.747209455023, 1357.098582039163, 1367.5768560474035, 1313.956036036036, 1374.0903034789046]</t>
+  </si>
+  <si>
+    <t>[1381.0, 1483.297506925208, 1402.184493491794, 1446.7669819432506, 1467.3086419753088, 1432.7725547445257, 1392.6394074074076, 1489.2701966717095, 1509.6704119850187, 1447.7576142131982, 1441.553588365476, 1466.5738673670387, 1313.4017555705607, 1395.9337748344371, 1400.5758558558557, 1328.9259807549965]</t>
+  </si>
+  <si>
+    <t>[1362.0, 1301.9828254847646, 1333.121675155631, 1428.7486385783895, 1411.0370370370372, 1466.2435036496352, 1445.2331851851854, 1389.6871406959153, 1468.119850187266, 1379.7106598984772, 1331.6541258299083, 1505.4235062376888, 1304.6623902768401, 1416.5569884977344, 1455.212972972973, 1516.4263508512215]</t>
+  </si>
+  <si>
+    <t>[1381.0, 1400.3229916897508, 1445.0871533672891, 1508.2413298939528, 1350.5185185185185, 1359.3524087591243, 1375.1081481481483, 1374.0223903177005, 1387.3270911360798, 1417.2538071065992, 1367.8975656022762, 1373.091923834537, 1404.5408507765026, 1435.8912513070757, 1357.9322522522523, 1342.6121391561808]</t>
+  </si>
+  <si>
+    <t>[809.0, 771.3556786703602, 773.2942840973401, 786.4476927486387, 747.4567901234568, 756.8753284671534, 754.9398518518519, 738.481089258699, 818.3152309612984, 783.7131979695432, 790.3408156813152, 783.0630334865397, 776.5550303848752, 839.1070059254096, 875.5264864864864, 886.8630643967433]</t>
+  </si>
+  <si>
+    <t>[1408.0, 1351.1529085872578, 1467.06168647425, 1282.482086557753, 1344.1481481481483, 1358.2727007299272, 1402.5007407407409, 1400.876248108926, 1443.8820224719102, 1420.7734771573605, 1367.8975656022762, 1379.1621799080763, 1433.2559081701554, 1403.6674799581738, 1296.632072072072, 1349.455218356773]</t>
+  </si>
+  <si>
+    <t>[1018.0, 980.3285318559558, 1003.5036785512167, 968.750931498997, 975.7283950617284, 930.7083211678834, 993.8032592592593, 1030.5167927382754, 1002.9843945068665, 1040.649111675127, 990.2643060385709, 955.4583059750493, 940.1060094530724, 933.2004182642036, 907.5091891891891, 988.1406365655072]</t>
+  </si>
+  <si>
+    <t>[1141.0, 1163.691966759003, 1129.0724391624221, 1083.220406993408, 1070.2222222222222, 1125.055766423358, 1037.6314074074076, 1169.2617246596067, 1117.2484394506866, 1125.121192893401, 1128.2232058172622, 1167.9172685489166, 1076.1904118838625, 1080.140815615197, 1091.4097297297296, 1078.4692820133237]</t>
+  </si>
+  <si>
+    <t>[1216.0, 1202.6182825484766, 1214.8777589134127, 1205.1092003439383, 1175.3333333333335, 1177.9614598540147, 1159.2545185185186, 1161.4293494704993, 1195.732833957553, 1168.530456852792, 1138.7454947834335, 1142.4221930400524, 1161.0871033085755, 1122.6761937957476, 1128.722882882883, 1152.374537379719]</t>
+  </si>
+  <si>
+    <t>[878.0, 907.5977839335181, 876.8885116015846, 981.4697621094872, 912.0246913580247, 970.6575182481753, 931.3481481481483, 986.8792738275341, 921.0374531835206, 1037.1294416243657, 954.0208662662029, 910.5384110308602, 960.0817015530048, 1033.7385848727781, 1076.7509909909909, 1008.6698741672836]</t>
+  </si>
+  <si>
+    <t>[1532.0, 1535.5407202216068, 1544.4957555178269, 1516.7205503009461, 1560.7407407407409, 1565.5766423357666, 1590.961777777778, 1516.124054462935, 1540.8333333333335, 1463.0095177664975, 1467.2747391716725, 1456.8614576493762, 1564.3463875759624, 1584.1205995120251, 1355.2670270270269, 1526.0066617320506]</t>
+  </si>
+  <si>
+    <t>[1209.0, 1201.5939058171746, 1206.506508205999, 1199.8096875895674, 1138.172839506173, 1197.3962043795623, 1216.2311111111112, 1181.5697428139183, 1229.2041198501872, 1176.7430203045685, 1146.9294973126778, 1175.2015758371635, 1173.5719108710332, 1143.2994074590451, 1134.0533333333333, 1179.7468541820874]</t>
+  </si>
+  <si>
+    <t>[1473.0, 1459.7368421052633, 1469.1544991511037, 1504.001719690456, 1419.530864197531, 1537.5042335766425, 1453.998814814815, 1386.330408472012, 1593.925717852684, 1472.395304568528, 1395.9570028454, 1461.7176625082075, 1519.4010803511144, 1461.6702683861974, 1415.2345945945945, 1497.2657290895634]</t>
+  </si>
+  <si>
+    <t>[1168.0, 1096.0831024930749, 1102.9122807017543, 1056.7228432215536, 1058.5432098765432, 1047.316788321168, 1023.3872592592594, 1145.7645990922845, 1094.1647940074906, 1057.0742385786803, 1070.9351881125513, 1138.7800393959292, 1147.3538149898718, 1109.786685256187, 1064.7574774774773, 1075.7320503330868]</t>
+  </si>
+  <si>
+    <t>[1176.0, 1188.2770083102494, 1193.9496321448783, 1178.6116365720839, 1144.5432098765432, 1156.367299270073, 1153.776, 1151.3591527987899, 1163.4157303370787, 1166.1840101522844, 1145.7603540942143, 1154.5627051871306, 1158.5901417960838, 1162.6336702683864, 1176.696936936937, 1156.4803849000741]</t>
+  </si>
+  <si>
+    <t>[1539.0, 1500.7119113573408, 1509.9643463497453, 1513.5408426483236, 1452.4444444444446, 1473.8014598540149, 1478.1042962962965, 1460.1785173978822, 1487.7409488139826, 1470.0488578680204, 1452.0758773316472, 1492.0689428759028, 1455.7285617825796, 1459.092366678285, 1484.5304504504504, 1435.678016284234]</t>
+  </si>
+  <si>
+    <t>[1591.0, 1519.1506925207757, 1462.8760611205432, 1524.1398681570654, 1495.9753086419753, 1481.3594160583943, 1450.711703703704, 1428.8490166414524, 1405.7940074906367, 1458.3166243654823, 1424.0164400885235, 1495.7110965200263, 1432.0074274139097, 1399.8006273963053, 1489.8609009009008, 1457.575869726129]</t>
+  </si>
+  <si>
+    <t>[1864.0, 1835.683102493075, 1858.4176570458403, 1782.7560905703642, 1797.5061728395062, 1773.9602919708032, 1743.2645925925929, 1743.26293494705, 1787.8283395755307, 1751.6224619289342, 1787.619981030667, 1766.4445173998686, 1711.6671168129644, 1805.8201463924713, 1799.0270270270269, 1699.8208734270913]</t>
+  </si>
+  <si>
+    <t>[1085.0, 1094.034349030471, 1109.1907187323147, 1143.634852393236, 1025.6296296296298, 1058.1138686131387, 1051.8755555555556, 1023.803328290469, 1095.3189762796505, 1073.4993654822335, 1044.0448940878912, 1064.7229152987525, 1041.2329507089805, 1060.8065528058557, 1119.3945945945945, 1023.7246484085864]</t>
+  </si>
+  <si>
+    <t>[1484.0, 1514.028808864266, 1550.774193548387, 1509.3012324448268, 1462.0, 1473.8014598540149, 1464.955851851852, 1471.3676248108927, 1448.4987515605494, 1485.30076142132, 1454.414163768574, 1472.6441234405777, 1441.995273463876, 1424.290693621471, 1463.2086486486485, 1441.152479644708]</t>
+  </si>
+  <si>
+    <t>[1270.0, 1317.3484764542939, 1265.1052631578948, 1278.2424763542565, 1240.0987654320988, 1243.8236496350366, 1242.5280000000002, 1239.7531013615735, 1225.741573033708, 1242.443527918782, 1210.063231109706, 1278.3959290873277, 1228.5050641458477, 1243.8375740676195, 1275.3102702702702, 1219.436713545522]</t>
+  </si>
+  <si>
+    <t>[941.0, 918.8659279778394, 945.9513299377476, 958.1519059902553, 901.4074074074075, 955.5416058394162, 929.1567407407408, 926.4580937972769, 932.5792759051186, 892.8229695431472, 920.1157129307619, 922.6789231779383, 915.1363943281567, 953.823631927501, 979.4702702702702, 911.498149518875]</t>
+  </si>
+  <si>
+    <t>[907.0, 928.0853185595569, 948.044142614601, 929.5345371166525, 896.0987654320988, 912.353284671533, 928.0610370370372, 914.1500756429652, 922.1916354556804, 923.3267766497463, 916.6082832753715, 919.0367695338149, 913.887913571911, 902.2655977692576, 930.1636036036035, 947.0821613619543]</t>
+  </si>
+  <si>
+    <t>[1467.0, 1478.1756232686982, 1497.4074702886248, 1474.324448265979, 1349.4567901234568, 1352.8741605839418, 1455.0945185185187, 1428.8490166414524, 1400.0230961298378, 1407.8680203045687, 1372.5741384761302, 1393.73079448457, 1428.2619851451723, 1355.9762983617986, 1425.8954954954954, 1438.4152479644708]</t>
+  </si>
+  <si>
+    <t>[1947.0, 1947.3401662049864, 1985.0328239954727, 1998.9762109486962, 1918.5432098765434, 2029.8510948905111, 2091.698370370371, 1984.9476550680788, 2027.898252184769, 2061.353426395939, 2047.1697755295604, 1931.5554826001312, 2157.374746792708, 2073.9219240153366, 2080.2082882882883, 2135.040710584752]</t>
+  </si>
+  <si>
+    <t>[1002.0, 1026.4254847645432, 1029.6638370118847, 1013.2668386357125, 1011.8271604938273, 1011.6864233576644, 1002.568888888889, 1028.2789712556732, 1053.7684144818977, 1040.649111675127, 1012.4780271893771, 1021.0170715692711, 1022.5057393652938, 1028.5827814569536, 1040.7704504504504, 1031.936343449297]</t>
+  </si>
+  <si>
+    <t>[1439.0, 1343.9822714681443, 1304.8687040181098, 1333.3574089997137, 1333.530864197531, 1265.4178102189783, 1332.375703703704, 1352.7630862329804, 1345.7765293383272, 1371.4980964467006, 1343.345558014543, 1373.091923834537, 1320.8926401080353, 1381.7553154409202, 1377.9214414414414, 1343.9807549962993]</t>
+  </si>
+  <si>
+    <t>[1010.0, 1047.9373961218837, 1055.8239954725523, 1032.3450845514476, 1040.4938271604938, 1030.0414598540146, 1032.152888888889, 1059.608472012103, 1091.856429463171, 1077.019035532995, 1040.5374644325009, 1047.726198292843, 1046.2268737339637, 1064.673405367724, 1074.0857657657657, 1049.7283493708364]</t>
+  </si>
+  <si>
+    <t>[1141.0, 1166.7650969529088, 1162.557441992077, 1129.8561192318718, 1101.0123456790125, 1113.1789781021898, 1105.5650370370372, 1135.694402420575, 1139.177902621723, 1147.4124365482235, 1109.5169143218463, 1146.064346684176, 1147.3538149898718, 1131.6988497734403, 1179.3621621621621, 1171.5351591413769]</t>
+  </si>
+  <si>
+    <t>[957.0, 918.8659279778394, 981.5291454442558, 949.6726855832619, 898.2222222222223, 977.1357664233578, 860.1274074074075, 960.0254160363087, 910.6498127340824, 933.8857868020306, 1003.1248814416692, 929.9632304661851, 1005.0270087778529, 938.3562216800279, 1034.1073873873872, 932.0273871206515]</t>
+  </si>
+  <si>
+    <t>[1086.0, 1091.9855955678672, 1088.2625919637803, 1060.9624534250504, 1015.0123456790124, 1066.7515328467155, 1061.736888888889, 1039.4680786686838, 1061.8476903870162, 1041.8223350253809, 1031.184318684793, 1006.4484569927774, 1049.972316002701, 1055.6507493900315, 1023.4464864864865, 1019.618800888231]</t>
+  </si>
+  <si>
+    <t>[1060.0, 1036.6692520775625, 1136.3972835314091, 1052.483233018057, 977.8518518518518, 1037.5994160583944, 1044.2056296296298, 1062.965204236006, 1027.2222222222222, 980.8147208121828, 948.1751501738855, 942.1037426132633, 971.3180283592169, 1051.7838968281633, 951.4854054054053, 994.9837157660993]</t>
+  </si>
+  <si>
+    <t>[2071.0, 1969.876454293629, 2013.2857951329938, 2035.0128976784183, 2118.1481481481483, 2116.2277372262774, 2056.6358518518523, 2144.9518910741303, 2169.8626716604244, 2159.904187817259, 2201.4966803667403, 2231.426132632961, 2047.5084402430793, 2006.8964796096202, 2102.862702702703, 2021.4455958549224]</t>
+  </si>
+  <si>
+    <t>[2001.0, 1964.7545706371193, 2004.91454442558, 1933.2622527944973, 1763.530864197531, 2035.2496350364966, 2067.5928888888893, 2081.1739788199698, 2279.5099875156056, 2039.0621827411169, 2023.7869111602909, 1790.725541694025, 2000.0661715057397, 1994.0069710700593, 2212.1369369369368, 1922.9052553663955]</t>
+  </si>
+  <si>
+    <t>[1167.0, 1178.03324099723, 1207.5529145444257, 1182.8512467755806, 1157.283950617284, 1186.5991240875915, 1201.9869629629632, 1162.5482602118004, 1217.6622971285892, 1218.9790609137058, 1194.8643692696808, 1194.6263952724885, 1221.0141796083728, 1205.169048448937, 1204.6818018018018, 1230.3856402664694]</t>
+  </si>
+  <si>
+    <t>[893.0, 911.6952908587259, 928.1624221844935, 954.9721983376328, 874.8641975308642, 962.0198540145986, 952.1665185185186, 963.3821482602118, 1015.6803995006243, 972.6021573604062, 915.439140056908, 1024.6592252133946, 990.0452397029036, 966.7131404670617, 968.8093693693693, 1027.8304959289417]</t>
+  </si>
+  <si>
+    <t>[1140.0, 1190.3257617728534, 1089.308998302207, 1021.7460590427058, 1052.172839506173, 992.2516788321169, 1052.9712592592593, 1097.651437216339, 1131.0986267166043, 1080.5387055837564, 1118.8700600695543, 1112.0709126723573, 1052.4692775151925, 1125.25409550366, 1178.0295495495495, 1038.779422649889]</t>
+  </si>
+  <si>
+    <t>[569.0, 557.2609418282549, 547.2705149971704, 539.4903983949557, 536.1728395061729, 532.2960583941607, 531.4162962962963, 543.7906202723148, 552.8533083645443, 551.4149746192894, 555.3430287701549, 551.1792514773473, 526.8588791357191, 532.336702683862, 547.7037837837837, 551.5521835677276]</t>
+  </si>
+  <si>
+    <t>[561.0, 555.2121883656511, 549.3633276740238, 527.8314703353398, 528.7407407407408, 530.1366423357665, 528.1291851851853, 544.9095310136157, 543.6198501872659, 553.761421319797, 543.6515965855201, 551.1792514773473, 528.107359891965, 528.4698501219938, 542.3733333333333, 547.4463360473724]</t>
+  </si>
+  <si>
+    <t>[516.0, 512.1883656509696, 526.3423882286361, 494.9744912582403, 501.13580246913585, 493.42656934306575, 494.1623703703704, 506.8665658093798, 500.91510611735333, 513.8718274111676, 501.5624407208346, 513.5436638214052, 499.392302498312, 500.11293133495997, 517.0536936936936, 515.9681717246485]</t>
+  </si>
+  <si>
+    <t>[848.0, 872.7689750692522, 846.54272778721, 843.6824304958442, 884.4197530864197, 845.411386861314, 866.7016296296298, 847.0154311649017, 862.1741573033709, 876.3978426395939, 874.519127410686, 872.902823374918, 865.1971640783256, 873.9086789822238, 932.8288288288288, 862.2279792746115]</t>
+  </si>
+  <si>
+    <t>[742.0, 789.7944598337951, 783.7583474816072, 799.1665233591289, 775.0617283950618, 737.440583941606, 791.0980740740741, 763.0971255673222, 790.6148564294632, 807.1776649746193, 812.5545368321214, 786.7051871306631, 765.3187035786632, 779.8152666434298, 828.885045045045, 860.859363434493]</t>
+  </si>
+  <si>
+    <t>[1092.0, 1039.7423822714682, 1050.5919637804188, 1062.0223559759245, 1080.8395061728395, 1087.26598540146, 1072.6939259259261, 1059.608472012103, 1109.1691635455682, 1115.7354060913706, 1044.0448940878912, 1081.719632304662, 1081.1843349088456, 1064.673405367724, 1124.725045045045, 1045.6225018504813]</t>
+  </si>
+  <si>
+    <t>[596.0, 610.5285318559557, 612.1477079796265, 600.9647463456579, 604.1234567901234, 574.4046715328468, 578.5315555555557, 580.7146747352497, 585.1704119850187, 594.8242385786803, 603.2779007271578, 619.1661195009849, 608.0101282916949, 619.9853607528756, 609.0039639639639, 609.0340488527017]</t>
+  </si>
+  <si>
+    <t>[501.0, 495.79833795013855, 486.57894736842104, 467.4170249355117, 466.0987654320988, 449.15854014598546, 449.23851851851856, 457.63449319213316, 468.5980024968789, 466.9428934010153, 469.9955738223206, 467.4097176625082, 463.1863605671844, 458.8665040083653, 479.7405405405405, 477.6469282013324]</t>
+  </si>
+  <si>
+    <t>[486.0, 477.35955678670365, 464.6044142614601, 440.9194611636573, 438.4938271604938, 434.0426277372263, 426.2287407407408, 436.375189107413, 453.5936329588015, 456.383883248731, 455.96585520075877, 443.12869336835195, 453.19851451721814, 433.08748692924365, 454.4209009009009, 457.11769059955594]</t>
+  </si>
+  <si>
+    <t>[463.0, 435.3601108033242, 438.4442558007923, 426.08082545141883, 431.0617283950618, 417.8470072992701, 419.65451851851856, 429.66172465960665, 439.74344569288394, 441.1319796954315, 411.53841289914635, 423.7038739330269, 411.9986495611074, 413.7532241199024, 427.76864864864865, 437.9570688378979]</t>
+  </si>
+  <si>
+    <t>[581.0, 567.5047091412744, 629.9366157328806, 552.2092290054458, 554.2222222222223, 553.8902189781022, 504.02370370370375, 609.8063540090772, 558.6242197253433, 579.5723350253808, 586.9098956686689, 581.5305318450427, 555.5739365293721, 541.3593586615546, 567.6929729729729, 558.3952627683199]</t>
+  </si>
+  <si>
+    <t>[496.0, 505.017728531856, 491.8109790605546, 478.01605044425344, 462.9135802469136, 445.91941605839423, 450.3342222222223, 455.39667170953106, 462.8270911360799, 449.3445431472081, 457.13499841922226, 461.33946158896913, 453.19851451721814, 453.710700592541, 463.74918918918917, 458.48630643967437]</t>
+  </si>
+  <si>
+    <t>[551.0, 534.7246537396122, 533.6672325976231, 515.1126397248496, 509.6296296296297, 512.8613138686133, 509.5022222222223, 520.2934947049924, 514.7652933832709, 520.9111675126904, 503.9007271577616, 512.3296126066973, 506.8831870357867, 507.8466364586964, 513.0558558558558, 533.760177646188]</t>
+  </si>
+  <si>
+    <t>[571.0, 552.1390581717452, 550.4097340124505, 537.3705932932073, 532.9876543209876, 525.8178102189781, 530.3205925925927, 547.1473524962179, 534.3863920099875, 554.9346446700508, 537.8058804932026, 526.898227183191, 518.1195138419987, 525.8919484140816, 539.708108108108, 550.1835677276092]</t>
+  </si>
+  <si>
+    <t>[467.0, 460.96952908587264, 461.46519524618, 440.9194611636573, 425.7530864197531, 445.91941605839423, 437.18577777777784, 446.44538577912255, 446.6685393258427, 442.3052030456853, 441.93613657919695, 444.34274458305975, 443.21066846725193, 431.7985360752876, 441.09477477477475, 442.0629163582532]</t>
+  </si>
+  <si>
+    <t>[544.0, 532.6759002770084, 528.4352009054895, 527.8314703353398, 517.0617283950618, 519.3395620437957, 512.7893333333334, 506.8665658093798, 525.1529338327091, 516.2182741116752, 555.3430287701549, 526.898227183191, 508.1316677920325, 527.1808992680377, 535.7102702702703, 535.1287934863064]</t>
+  </si>
+  <si>
+    <t>[742.0, 735.5024930747924, 730.391624221845, 713.3144167383206, 707.1111111111112, 711.527591240876, 717.685925925926, 713.8650529500757, 728.289013732834, 732.0913705583757, 717.8539361365791, 726.0026263952725, 735.3551654287644, 741.1467410247474, 743.5978378378378, 745.8956328645448]</t>
+  </si>
+  <si>
+    <t>[798.0, 781.5994459833796, 778.5263157894736, 758.8902264259101, 748.5185185185186, 764.433284671533, 754.9398518518519, 749.6701966717096, 768.685393258427, 780.1935279187818, 766.9579513120456, 780.634931057124, 784.0459149223499, 801.7274311606832, 804.898018018018, 818.4322723908217]</t>
+  </si>
+  <si>
+    <t>[795.0, 782.6238227146815, 777.479909451047, 753.5907136715392, 738.962962962963, 765.51299270073, 779.0453333333335, 756.3836611195159, 780.227215980025, 807.1776649746193, 782.1568131520708, 785.4911359159554, 797.7792032410534, 813.327988846288, 816.8915315315315, 836.2242783123613]</t>
+  </si>
+  <si>
+    <t>[465.0, 448.67700831024933, 433.21222410865875, 439.85955861278313, 418.320987654321, 423.2455474452555, 411.98459259259266, 428.5428139183056, 433.97253433208493, 443.4784263959391, 420.89155864685426, 432.2022324359816, 429.4773801485483, 433.08748692924365, 429.10126126126124, 436.5884529977795]</t>
+  </si>
+  <si>
+    <t>[657.0, 629.9916897506926, 651.9111488398415, 625.3425050157639, 632.7901234567902, 645.6654014598541, 631.1253333333334, 609.8063540090772, 608.2540574282148, 613.5958121827412, 609.1236168194752, 622.8082731451084, 616.7494935854153, 636.7417218543047, 660.9758558558558, 667.8845299777943]</t>
+  </si>
+  <si>
+    <t>[998.0, 908.6221606648201, 1070.4736842105262, 980.409859558613, 1000.1481481481482, 1012.7661313868614, 995.9946666666668, 999.1872919818458, 993.7509363295881, 1102.8299492385788, 979.7420170723996, 899.6119500984898, 1036.2390276839974, 1121.3872429417916, 1028.7769369369369, 916.9726128793487]</t>
+  </si>
+  <si>
+    <t>[859.0, 918.8659279778394, 877.9349179400114, 863.8205789624536, 812.2222222222223, 904.7953284671534, 906.1469629629631, 902.9609682299547, 855.249063670412, 891.6497461928934, 896.7328485614922, 906.8962573867367, 938.8575286968265, 956.4015336354131, 967.4767567567567, 1016.8815692079942]</t>
+  </si>
+  <si>
+    <t>[1230.0, 1174.9601108033241, 1088.2625919637803, 1023.8658641444542, 1006.5185185185186, 1023.5632116788322, 1024.482962962963, 992.4738275340394, 1037.6098626716605, 997.2398477157361, 1082.6266202971863, 1036.7997373604728, 1052.4692775151925, 1049.205995120251, 1066.0900900900901, 1130.476683937824]</t>
+  </si>
+  <si>
+    <t>[1161.0, 1185.2038781163437, 1095.5874363327673, 1081.1006018916596, 1077.6543209876543, 1125.055766423358, 1165.8287407407408, 1108.8405446293496, 1105.7066167290886, 1101.656725888325, 1152.7752134049952, 1132.70978332239, 1171.0749493585417, 1185.8347856395958, 1155.375135135135, 1211.2250185048115]</t>
+  </si>
+  <si>
+    <t>[1019.0, 976.231024930748, 1028.6174306734579, 887.1384350816854, 904.5925925925926, 873.4837956204381, 864.5102222222223, 908.55552193646, 946.4294631710362, 962.0431472081219, 928.2997154600063, 1033.1575837163493, 956.3362592842675, 996.3590101080516, 991.4637837837837, 951.1880088823095]</t>
+  </si>
+  <si>
+    <t>[717.0, 718.0880886426594, 710.5099037917374, 695.2960733734595, 691.1851851851852, 688.8537226277373, 704.5374814814816, 697.0813918305598, 714.4388264669163, 718.01269035533, 702.655074296554, 705.3637557452397, 714.1309925725861, 708.9229696758453, 712.9477477477477, 715.7860843819394]</t>
+  </si>
+  <si>
+    <t>[742.0, 736.5268698060943, 755.505376344086, 733.4525652049299, 706.0493827160494, 730.9623357664234, 741.7914074074075, 732.8865355521937, 727.1348314606741, 742.65038071066, 708.5007903888713, 735.715036112935, 729.1127616475355, 715.3677239456257, 723.6086486486486, 704.8371576609919]</t>
+  </si>
+  <si>
+    <t>[683.0, 669.9423822714682, 669.7000565930956, 658.1994840928634, 665.7037037037037, 670.498686131387, 666.187851851852, 657.9195158850227, 687.892634207241, 694.5482233502538, 674.5956370534303, 656.8017071569271, 691.6583389601622, 675.4102474729872, 687.6281081081081, 703.4685418208735]</t>
+  </si>
+  <si>
+    <t>[605.0, 616.6747922437673, 610.054895302773, 609.4439667526512, 573.3333333333334, 578.7235036496351, 581.8186666666668, 581.8335854765508, 611.7166042446942, 606.5564720812183, 588.0790388871325, 585.1726854891662, 589.2829169480082, 600.6510979435344, 615.667027027027, 614.5085122131755]</t>
+  </si>
+  <si>
+    <t>[783.0, 727.3074792243768, 736.6700622524052, 739.811980510175, 753.8271604938273, 729.8826277372264, 710.0160000000001, 728.4108925869895, 766.3770287141074, 770.8077411167513, 763.450521656655, 730.8588312541037, 744.0945307224849, 752.7472987103521, 780.910990990991, 754.1073279052555]</t>
+  </si>
+  <si>
+    <t>[931.0, 967.0116343490306, 1026.5246179966043, 1011.1470335339641, 1025.6296296296298, 1040.8385401459855, 1084.746666666667, 1095.4136157337368, 1080.314606741573, 1098.1370558375636, 1061.5820423648436, 1087.7898883782009, 1071.1964888588793, 1072.4071104914606, 1054.0965765765766, 1063.414507772021]</t>
+  </si>
+  <si>
+    <t>[870.0, 933.2072022160665, 892.5846066779853, 888.1983376325596, 888.6666666666667, 804.3824817518249, 940.113777777778, 908.55552193646, 870.2534332084895, 841.2011421319797, 876.857413847613, 905.6822061720289, 846.4699527346388, 894.5318926455211, 914.1722522522522, 867.7024426350853]</t>
+  </si>
+  <si>
+    <t>[632.0, 625.8941828254848, 623.6581777023204, 626.4024075666381, 628.5432098765432, 581.9626277372264, 609.2112592592594, 628.8278366111952, 625.5667915106118, 626.501269035533, 634.8447676256718, 616.7380170715693, 640.4706279540851, 629.0080167305682, 667.6389189189189, 651.4611398963731]</t>
+  </si>
+  <si>
+    <t>[562.0, 572.626592797784, 554.5953593661574, 551.1493264545716, 539.3580246913581, 535.5351824817519, 553.3303703703705, 550.504084720121, 556.3158551810237, 566.6668781725889, 547.1590262409105, 540.252790544977, 553.0769750168805, 550.3820146392471, 571.6908108108108, 566.6069578090304]</t>
+  </si>
+  <si>
+    <t>[759.0, 757.014404432133, 746.0877192982456, 728.153052450559, 733.6543209876544, 735.2811678832118, 733.0257777777779, 731.7676248108926, 760.6061173533084, 727.3984771573605, 720.1922225735061, 727.2166776099803, 727.8642808912898, 724.3903799233183, 735.6021621621621, 728.1036269430052]</t>
+  </si>
+  <si>
+    <t>[697.0, 698.6249307479226, 684.3497453310696, 657.1395815419892, 668.8888888888889, 645.6654014598541, 658.517925925926, 675.8220877458397, 692.5093632958801, 706.280456852792, 683.9487828011381, 675.0124753775443, 670.4341661039839, 667.6765423492507, 670.3041441441441, 687.0451517394523]</t>
+  </si>
+  <si>
+    <t>[824.0, 820.5257617728532, 822.4753820033956, 806.585841215248, 802.6666666666667, 806.5418978102191, 810.8207407407408, 819.0426626323753, 829.8570536828964, 843.5475888324873, 820.7385393613657, 813.414313854235, 815.2579338284944, 803.0163820146392, 827.5524324324324, 832.118430792006]</t>
+  </si>
+  <si>
+    <t>[581.0, 552.1390581717452, 544.1312959818902, 491.79478360561774, 455.4814814814815, 483.70919708029203, 476.6311111111112, 481.1316187594554, 480.1398252184769, 488.0609137055838, 491.04015175466327, 451.6270518713066, 483.1620526671169, 479.4897176716626, 474.4100900900901, 505.01924500370103]</t>
+  </si>
+  <si>
+    <t>[808.0, 815.4038781163435, 820.3825693265421, 793.867010604758, 802.6666666666667, 790.3462773722629, 810.8207407407408, 802.2590015128593, 818.3152309612984, 842.3743654822335, 804.370534302877, 784.2770847012475, 772.8095881161379, 778.5263157894738, 804.898018018018, 819.8008882309401]</t>
+  </si>
+  <si>
+    <t>[934.0, 899.4027700831026, 900.955857385399, 889.2582401834338, 871.6790123456791, 886.4402919708031, 885.3285925925927, 901.8420574886536, 916.4207240948814, 916.2874365482235, 904.9168510907366, 909.3243598161523, 926.3727211343688, 908.7103520390381, 938.1592792792792, 921.078460399704]</t>
+  </si>
+  <si>
+    <t>[707.0, 708.8686980609419, 695.8602150537635, 695.2960733734595, 681.6296296296297, 670.498686131387, 683.7191111111111, 681.416641452345, 691.3551810237203, 709.8001269035534, 694.4710717673095, 700.5075508864084, 695.4037812288994, 696.0334611362845, 696.9563963963964, 710.3116210214656]</t>
+  </si>
+  <si>
+    <t>[723.0, 718.0880886426594, 698.9994340690436, 702.7153912295788, 685.8765432098766, 672.6581021897811, 687.0062222222223, 676.9409984871407, 691.3551810237203, 715.6662436548224, 695.640214985773, 705.3637557452397, 697.900742741391, 693.4555594283723, 700.9542342342341, 710.3116210214656]</t>
+  </si>
+  <si>
+    <t>[605.0, 639.21108033241, 617.37973967176, 587.1860131842936, 580.7654320987655, 543.0931386861314, 617.976888888889, 582.9524962178517, 585.1704119850187, 615.9422588832488, 591.5864685425229, 592.456992777413, 608.0101282916949, 609.673753921227, 590.3473873873874, 602.1909696521096]</t>
+  </si>
+  <si>
+    <t>[771.0, 783.6481994459834, 747.1341256366724, 752.5308111206651, 772.9382716049383, 800.0636496350365, 798.7680000000001, 755.2647503782149, 826.394506866417, 787.2328680203046, 771.6345241858994, 758.7820091923835, 725.3673193787982, 768.2147089578251, 779.5783783783784, 781.4796447076241]</t>
+  </si>
+  <si>
+    <t>[529.0, 566.4803324099723, 510.64629315223544, 549.0295213528233, 520.2469135802469, 526.8975182481753, 527.0334814814815, 509.1043872919819, 544.7740324594257, 524.4308375634519, 524.9453050901043, 522.0420223243598, 518.1195138419987, 528.4698501219938, 490.4014414414414, 533.760177646188]</t>
+  </si>
+  <si>
+    <t>[689.0, 697.6005540166205, 692.7209960384833, 684.6970478647178, 676.320987654321, 668.3392700729928, 680.4320000000001, 687.0111951588502, 691.3551810237203, 702.7607868020306, 693.301928548846, 692.0091923834538, 694.1553004726537, 699.9003136981527, 692.9585585585585, 711.6802368615841]</t>
+  </si>
+  <si>
+    <t>[655.0, 619.7479224376732, 670.7464629315224, 651.8400687876183, 639.1604938271605, 625.1509489051095, 658.517925925926, 680.2977307110439, 662.5006242197254, 660.5247461928934, 655.8893455580145, 615.5239658568614, 647.9615124915598, 666.3875914952946, 666.3063063063063, 685.6765358993339]</t>
+  </si>
+  <si>
+    <t>[817.0, 816.4282548476456, 816.1969439728354, 791.7472055030096, 777.1851851851852, 788.1868613138687, 799.8637037037038, 788.8320726172466, 791.769038701623, 803.6579949238579, 820.7385393613657, 807.344057780696, 801.5246455097907, 804.3053328685954, 812.8936936936936, 825.2753515914138]</t>
+  </si>
+  <si>
+    <t>[603.0, 592.0897506925209, 592.265987549519, 557.5087417598166, 565.9012345679013, 551.7308029197081, 558.808888888889, 569.5255673222391, 573.6285892634207, 588.9581218274112, 585.7407524502055, 575.4602757715036, 591.7798784604997, 587.7615894039735, 590.3473873873874, 635.037749814952]</t>
+  </si>
+  <si>
+    <t>[495.0, 491.70083102493084, 477.16129032258067, 464.23731728288914, 438.4938271604938, 455.63678832116796, 442.66429629629636, 444.20756429652045, 461.6729088639201, 478.67512690355335, 453.6275687638318, 454.0551543007223, 488.1559756921, 479.4897176716626, 465.08180180180176, 476.278312361214]</t>
+  </si>
+  <si>
+    <t>[789.0, 788.7700831024931, 783.7583474816072, 769.4892519346519, 763.3827160493828, 762.2738686131388, 757.1312592592593, 765.3349470499244, 772.1479400749064, 770.8077411167513, 745.9133733797028, 745.4274458305975, 749.0884537474681, 754.0362495643082, 763.587027027027, 755.4759437453739]</t>
+  </si>
+  <si>
+    <t>[1078.0, 1077.64432132964, 1074.6593095642331, 1055.6629406706795, 1041.5555555555557, 1050.5559124087592, 1042.0142222222223, 1052.8950075642965, 1065.3102372034957, 1064.113578680203, 1042.8757508694277, 1041.655942219304, 1048.7238352464553, 1047.9170442662949, 1039.4378378378378, 1037.4108068097707]</t>
+  </si>
+  <si>
+    <t>[1168.0, 1161.643213296399, 1150.0005659309563, 1137.2754370879911, 1121.1851851851852, 1132.6137226277374, 1088.033777777778, 1093.1757942511347, 1120.7109862671662, 1120.4282994923858, 1100.1637685741384, 1102.3585029546946, 1099.9115462525322, 1091.7413733008018, 1082.0814414414415, 1093.5240562546264]</t>
+  </si>
+  <si>
+    <t>[1236.0, 1201.5939058171746, 1201.2744765138652, 1207.2290054456867, 1196.567901234568, 1190.9179562043796, 1135.1490370370373, 1139.0511346444782, 1174.9575530586767, 1175.5697969543148, 1144.591210875751, 1169.1313197636243, 1156.0931802835923, 1162.6336702683864, 1160.7055855855856, 1161.9548482605478]</t>
+  </si>
+  <si>
+    <t>[1736.0, 1966.8033240997233, 1963.0582908885117, 1945.9810834049874, 1669.0370370370372, 1955.3512408759127, 1895.5674074074077, 1638.0853252647505, 1844.3832709113608, 1822.0158629441626, 1874.136579196965, 1864.7826657912015, 1775.3396353814992, 1821.2875566399443, 1745.7225225225225, 1701.1894892672096]</t>
+  </si>
+  <si>
+    <t>[1139.0, 1161.643213296399, 1085.1233729485002, 1062.0223559759245, 1206.1234567901236, 1253.5410218978104, 1063.9282962962964, 1087.5812405446295, 1121.8651685393259, 1302.277918781726, 1160.9592159342396, 1198.268548916612, 1194.7960837272115, 1201.3021958870688, 1162.0381981981982, 1322.0829015544043]</t>
+  </si>
+  <si>
+    <t>[1362.0, 1319.3972299168977, 1194.996038483305, 1333.3574089997137, 1220.9876543209878, 1213.5918248175185, 1216.2311111111112, 1261.0124054462935, 1165.7240948813983, 1234.2309644670052, 1197.2026557066076, 1248.0446487196323, 1229.7535449020934, 1276.0613454165216, 1196.686126126126, 1237.2287194670616]</t>
+  </si>
+  <si>
+    <t>[1727.0, 1668.709695290859, 1757.962648556876, 1656.6276870163374, 1623.382716049383, 1672.4677372262777, 1673.1395555555557, 1726.4792738275341, 1633.1679151061173, 1655.418147208122, 1473.12045526399, 1654.7518056467497, 1623.024983119514, 1410.112234227954, 1636.4482882882883, 1751.8282753515916]</t>
+  </si>
+  <si>
+    <t>[1262.0, 1251.7883656509696, 1210.6921335597058, 1197.689882487819, 1196.567901234568, 1148.8093430656936, 1082.5552592592594, 1108.8405446293496, 1179.574282147316, 1127.4676395939086, 1104.8403414479924, 1103.5725541694026, 1116.1417960837273, 1099.4750784245382, 1118.061981981982, 1126.3708364174686]</t>
+  </si>
+  <si>
+    <t>[1330.0, 1311.2022160664822, 1342.5393322014713, 1350.3158498137004, 1380.2469135802469, 1338.8379562043797, 1323.6100740740742, 1424.373373676248, 1350.3932584269664, 1257.6954314720813, 1329.3158393929814, 1302.6769533814838, 1207.2808912896694, 1286.3729522481701, 1276.6428828828828, 1193.4330125832719]</t>
+  </si>
+  <si>
+    <t>[1229.0, 1165.7407202216068, 1223.2490096208262, 1299.44052737174, 1354.7654320987656, 1392.8233576642338, 1174.5943703703706, 1148.0024205748866, 1211.8913857677903, 1207.2468274111677, 1163.2975023711665, 1279.6099803020354, 1127.3781228899393, 1210.3248518647613, 1260.6515315315314, 1155.1117690599558]</t>
+  </si>
+  <si>
+    <t>[1245.0, 1273.3002770083103, 1339.4001131861912, 1326.9979936944685, 1243.283950617284, 1220.070072992701, 1152.6802962962965, 1187.1642965204237, 1312.305243445693, 1282.3331218274113, 1169.1432184634841, 1165.489166119501, 1269.7049291019582, 1252.860230045312, 1206.0144144144144, 1201.6447076239824]</t>
+  </si>
+  <si>
+    <t>[708.0, 690.429916897507, 661.328805885682, 720.7337345944399, 631.7283950617284, 669.4189781021898, 658.517925925926, 670.2275340393344, 722.518102372035, 706.280456852792, 734.221941195068, 709.0059093893631, 666.6887238352465, 707.6340188218892, 796.9023423423423, 799.2716506291637]</t>
+  </si>
+  <si>
+    <t>[1331.0, 1205.6914127423825, 1312.1935483870968, 1225.2473488105477, 1290.0, 1321.5626277372264, 1303.8874074074076, 1304.649924357035, 1342.3139825218477, 1340.9942893401017, 1246.306670882074, 1290.5364412344059, 1328.3835246455099, 1322.4635761589404, 1256.6536936936936, 1305.6595114729832]</t>
+  </si>
+  <si>
+    <t>[927.0, 894.2808864265929, 852.8211658177702, 872.299799369447, 918.3950617283951, 846.491094890511, 895.189925925926, 814.5670196671709, 837.936329588015, 928.0196700507615, 886.2105595953209, 888.6854891661195, 863.9486833220798, 853.2854653189265, 830.2176576576576, 873.176905995559]</t>
+  </si>
+  <si>
+    <t>[1057.0, 1077.64432132964, 1038.0350877192982, 1022.80596159358, 1038.3703703703704, 1084.0268613138687, 967.5063703703705, 1088.7001512859304, 1056.0767790262173, 1053.554568527919, 1018.3237432816945, 1108.4287590282338, 988.7967589466577, 1010.5374695015686, 1023.4464864864865, 1053.8341968911918]</t>
+  </si>
+  <si>
+    <t>[1105.0, 1080.7174515235458, 1065.2416525183928, 1064.1421610776729, 1042.6172839506173, 1057.0341605839417, 1043.109925925926, 1048.4193645990924, 1054.9225967540574, 1048.8616751269037, 1034.6917483401833, 1010.0906106369008, 1033.742066171506, 1002.8037643778321, 994.129009009009, 1018.2501850481126]</t>
+  </si>
+  <si>
+    <t>[880.0, 909.646537396122, 800.5008488964346, 1044.0040126110634, 855.7530864197531, 1004.1284671532848, 928.0610370370372, 949.9552193645991, 872.5617977528091, 903.3819796954316, 936.4837179892507, 894.7557452396586, 961.3301823092506, 912.5772046009063, 811.561081081081, 916.9726128793487]</t>
+  </si>
+  <si>
+    <t>[1437.0, 1347.05540166205, 1404.2773061686473, 1428.7486385783895, 1315.4814814814815, 1424.1348905109492, 1451.8074074074077, 1313.6012102874433, 1343.4681647940076, 1380.883883248731, 1331.6541258299083, 1314.817465528562, 1334.625928426739, 1264.4607877309168, 1228.6688288288287, 1337.137675795707]</t>
+  </si>
+  <si>
+    <t>[1108.0, 1090.9612188365652, 1065.2416525183928, 1047.1837202636862, 1060.6666666666667, 1111.0195620437958, 1091.320888888889, 1069.6786686838125, 1099.9357053682897, 1058.2474619289342, 1061.5820423648436, 1041.655942219304, 1053.7177582714382, 1010.5374695015686, 1008.7877477477477, 1034.673575129534]</t>
+  </si>
+  <si>
+    <t>[1207.0, 1002.8648199445985, 997.2252405206565, 1094.879335053024, 1065.9753086419753, 1240.5845255474453, 1113.2349629629632, 1052.8950075642965, 1110.3233458177278, 1276.4670050761422, 1093.1489092633576, 1271.1116217990807, 1027.4996623902769, 1144.5883583130012, 1030.1095495495495, 1094.8926720947447]</t>
+  </si>
+  <si>
+    <t>[948.0, 981.3529085872577, 968.9722693831352, 960.2717110920037, 971.4814814814815, 932.8677372262775, 931.3481481481483, 927.577004538578, 949.8920099875156, 884.6104060913706, 949.3442933923491, 1024.6592252133946, 968.8210668467253, 1013.1153712094807, 926.1657657657657, 914.2353811991119]</t>
+  </si>
+  <si>
+    <t>[1024.0, 1038.7180055401664, 1044.3135257498584, 1020.6861564918316, 1006.5185185185186, 1019.244379562044, 1016.8130370370371, 1028.2789712556732, 1038.7640449438202, 1032.4365482233504, 1013.6471704078407, 1013.7327642810243, 1018.7602970965565, 1020.8490763332172, 1022.1138738738738, 1011.4071058475205]</t>
+  </si>
+  <si>
+    <t>[1345.0, 1265.1052631578948, 1386.4883984153932, 1319.5786758383492, 1236.9135802469136, 1267.5772262773723, 1255.6764444444445, 1259.8934947049925, 1309.9968789013733, 1348.0336294416245, 1272.0278216882707, 1271.1116217990807, 1302.1654287643485, 1297.973509933775, 1295.2994594594593, 1239.9659511472985]</t>
+  </si>
+  <si>
+    <t>[1445.0, 1396.2254847645431, 1372.885116015846, 1379.9931212381773, 1330.3456790123457, 1254.6207299270075, 1257.867851851852, 1385.211497730711, 1358.472534332085, 1386.75, 1172.6506481188744, 1303.8910045961918, 1290.9291019581365, 1306.9961659114674, 1340.6082882882881, 1331.6632124352334]</t>
+  </si>
+  <si>
+    <t>[1644.0, 1580.613296398892, 1625.0690435766837, 1499.7621094869594, 1546.9382716049383, 1479.2000000000003, 1492.3484444444446, 1553.0481089258699, 1667.7933832709114, 1538.0958121827412, 1579.5124881441668, 1600.1195009848982, 1588.0675219446323, 1513.2283025444406, 1531.1718918918918, 1375.4589193190232]</t>
+  </si>
+  <si>
+    <t>[1015.0, 941.4022160664821, 1061.056027164686, 962.391516193752, 888.6666666666667, 972.8169343065695, 965.3149629629631, 1064.084114977307, 963.7421972534332, 1005.4524111675128, 1026.507745810939, 927.5351280367695, 942.6029709655639, 1105.9198326943185, 1083.414054054054, 994.9837157660993]</t>
+  </si>
+  <si>
+    <t>[1259.0, 1338.8603878116346, 1263.0124504810412, 1332.2975064488394, 1229.4814814814815, 1234.1062773722629, 1244.7194074074075, 1275.5582450832073, 1200.3495630461923, 1244.7899746192895, 1170.3123616819476, 1190.984241628365, 1213.5232950708983, 1218.058556988498, 1172.699099099099, 1131.8452997779425]</t>
+  </si>
+  <si>
+    <t>[1156.0, 1211.8376731301942, 1170.9286926994907, 1130.916021782746, 1127.5555555555557, 1112.0992700729928, 1112.1392592592595, 1161.4293494704993, 1127.636079900125, 1102.8299492385788, 1088.4723363895037, 1139.994090610637, 1088.6752194463202, 1078.851864761241, 1178.0295495495495, 1057.9400444115472]</t>
+  </si>
+  <si>
+    <t>[913.0, 915.7927977839337, 949.0905489530277, 956.0321008885069, 882.2962962962963, 954.461897810219, 936.8266666666668, 904.0798789712558, 944.1210986267166, 879.9175126903554, 920.1157129307619, 878.973079448457, 893.9122214719785, 938.3562216800279, 918.1700900900901, 899.1806069578091]</t>
+  </si>
+  <si>
+    <t>[897.0, 921.9390581717453, 925.0232031692134, 913.6359988535398, 890.7901234567902, 883.2011678832118, 925.8696296296298, 892.8907715582451, 909.4956304619226, 908.0748730964468, 910.7625671830541, 915.3946158896914, 908.8939905469279, 879.0644823980482, 918.1700900900901, 937.5018504811252]</t>
+  </si>
+  <si>
+    <t>[1243.0, 1221.0570637119115, 1205.4601018675721, 1202.9893952421899, 1062.79012345679, 1090.5051094890512, 1109.947851851852, 1122.2674735249623, 1124.1735330836455, 1155.625, 1124.7157761618716, 1129.0676296782665, 1124.8811613774478, 1090.4524224468457, 1126.0576576576575, 1089.418208734271]</t>
+  </si>
+  <si>
+    <t>[1762.0, 1795.7324099722994, 1694.1318619128467, 1819.8526798509604, 1688.1481481481483, 1690.822773722628, 1792.5712592592595, 1824.9434190620273, 1686.2602996254682, 1700.0006345177667, 1764.2371166613973, 1676.6047275114904, 1664.2248480756248, 1745.2394562565355, 1672.4288288288287, 1933.854182087343]</t>
+  </si>
+  <si>
+    <t>[934.0, 957.7922437673132, 976.2971137521222, 961.3316136428778, 952.3703703703704, 958.7807299270074, 940.113777777778, 972.3334341906203, 994.9051186017479, 980.8147208121828, 956.3591527031299, 951.8161523309258, 952.5908170155302, 970.57999302893, 971.4745945945946, 968.9800148038491]</t>
+  </si>
+  <si>
+    <t>[1253.0, 1237.4470914127426, 1205.4601018675721, 1212.5285182000575, 1213.5555555555557, 1187.6788321167885, 1155.9674074074076, 1222.9694402420575, 1166.8782771535582, 1208.4200507614214, 1234.615238697439, 1167.9172685489166, 1142.3598919648887, 1190.99058905542, 1180.6947747747747, 1201.6447076239824]</t>
+  </si>
+  <si>
+    <t>[982.0, 1011.059833795014, 1026.5246179966043, 1014.3267411865866, 1015.0123456790124, 1011.6864233576644, 1009.1431111111112, 1043.9437216338881, 1074.5436953807741, 1045.3420050761422, 1018.3237432816945, 1028.301378857518, 1028.7481431465228, 1047.9170442662949, 1034.1073873873872, 1036.0421909696522]</t>
+  </si>
+  <si>
+    <t>[1092.0, 1117.5950138504156, 1123.8404074702887, 1066.2619661794213, 1044.7407407407409, 1064.5921167883214, 1071.5982222222224, 1106.6027231467474, 1110.3233458177278, 1102.8299492385788, 1075.6117609864052, 1092.6460932370321, 1111.1478730587442, 1084.0076681770652, 1098.0727927927928, 1127.7394522575871]</t>
+  </si>
+  <si>
+    <t>[840.0, 839.9889196675902, 822.4753820033956, 865.9403840642019, 819.6543209876544, 787.1071532846717, 798.7680000000001, 826.8750378214827, 824.0861423220974, 848.2404822335026, 949.3442933923491, 831.6250820748522, 877.6819716407833, 846.8407110491461, 871.5286486486486, 858.1221317542562]</t>
+  </si>
+  <si>
+    <t>[997.0, 965.9872576177287, 995.132427843803, 998.4282029234739, 923.7037037037037, 954.461897810219, 969.6977777777779, 957.7875945537065, 962.5880149812734, 909.2480964467006, 908.4242807461271, 888.6854891661195, 915.1363943281567, 947.3788776577205, 916.8374774774775, 886.8630643967433]</t>
+  </si>
+  <si>
+    <t>[932.0, 877.8908587257619, 964.7866440294284, 972.9905417024937, 862.1234567901236, 935.0271532846716, 936.8266666666668, 913.0311649016642, 873.7159800249689, 856.4530456852792, 869.8425545368322, 846.193696651346, 891.4152599594869, 841.6849076333218, 860.8677477477477, 847.1732050333088]</t>
+  </si>
+  <si>
+    <t>[1890.0, 1878.7069252077565, 1924.3412563667232, 1919.483519633133, 2019.4074074074076, 1945.633868613139, 2050.06162962963, 2123.6925869894103, 1852.4625468164795, 1730.5044416243657, 1925.5788808093582, 1946.1240971766251, 1952.6239027684, 1911.5141164168701, 1908.301261261261, 1866.7920059215398]</t>
+  </si>
+  <si>
+    <t>[1677.0, 1801.878670360111, 1544.4957555178269, 1624.8306104901121, 1322.9135802469136, 1616.3229197080293, 1553.707851851852, 1708.576701966717, 1867.4669163545568, 1440.7182741116753, 1438.0461587100854, 1289.3223900196979, 1659.2309250506416, 1461.6702683861974, 1303.295135135135, 1353.5610658771282]</t>
+  </si>
+  <si>
+    <t>[1156.0, 1170.8626038781165, 1196.0424448217318, 1163.7730008598455, 1142.4197530864199, 1172.5629197080293, 1189.9342222222224, 1156.953706505295, 1199.1953807740324, 1214.2861675126906, 1182.0037938665823, 1184.913985554826, 1212.2748143146523, 1198.7242941791565, 1192.6882882882883, 1213.9622501850483]</t>
+  </si>
+  <si>
+    <t>[911.0, 865.5983379501386, 872.7028862478777, 843.6824304958442, 868.4938271604939, 926.389489051095, 922.5825185185187, 945.4795763993949, 964.896379525593, 928.0196700507615, 876.857413847613, 974.8831254103743, 988.7967589466577, 934.4893691181597, 946.1549549549549, 1010.0384900074021]</t>
+  </si>
+  <si>
+    <t>[1061.0, 1066.3761772853186, 979.4363327674024, 962.391516193752, 998.0246913580247, 981.4545985401461, 999.281777777778, 1078.6299546142209, 1103.398252184769, 1047.6884517766498, 1079.1191906417957, 1025.8732764281024, 1034.9905469277517, 1016.9822237713489, 1114.0641441441442, 982.6661732050334]</t>
+  </si>
+  <si>
+    <t>[511.0, 513.2127423822716, 509.5998868138087, 490.7348810547436, 489.4567901234568, 488.02802919708034, 476.6311111111112, 484.48835098335854, 488.2191011235955, 490.4073604060914, 488.7018653177363, 492.90479317137226, 486.90749493585423, 488.5123736493552, 498.3971171171171, 500.9133974833457]</t>
+  </si>
+  <si>
+    <t>[548.0, 545.9927977839336, 543.0848896434635, 519.3522499283463, 522.3703703703704, 524.7381021897811, 522.6506666666668, 540.4338880484115, 536.6947565543071, 544.3756345177666, 536.6367372747392, 542.6808929743927, 520.6164753544903, 525.8919484140816, 535.7102702702703, 541.9718726868987]</t>
+  </si>
+  <si>
+    <t>[513.0, 505.017728531856, 521.1103565365025, 484.3754657494985, 494.7654320987655, 485.8686131386862, 487.5881481481482, 499.03419062027234, 492.8358302122347, 504.4860406091371, 495.7167246285172, 505.0453053184504, 493.1498987170831, 496.2460787730917, 510.3906306306306, 509.1250925240563]</t>
+  </si>
+  <si>
+    <t>[613.0, 706.819944598338, 719.9275608375779, 694.2361708225854, 655.0864197530865, 694.2522627737227, 720.9730370370371, 673.5842662632375, 699.4344569288389, 702.7607868020306, 694.4710717673095, 713.8621142481943, 695.4037812288994, 662.5207389334263, 742.2652252252252, 691.1509992598077]</t>
+  </si>
+  <si>
+    <t>[646.0, 685.3080332409974, 703.1850594227504, 727.0931498996848, 729.4074074074074, 646.7451094890512, 704.5374814814816, 655.6816944024206, 721.3639200998751, 730.9181472081219, 707.3316471704078, 701.7216021011162, 680.4220121539502, 684.4329034506798, 743.5978378378378, 713.0488527017026]</t>
+  </si>
+  <si>
+    <t>[816.0, 1009.0110803324101, 981.5291454442558, 1069.4416738320438, 788.8641975308642, 951.2227737226278, 892.9985185185186, 1049.5382753403933, 891.0287141073658, 944.4447969543148, 854.6436926968069, 960.3145108338805, 946.3484132343012, 951.2457302195887, 1120.7272072072071, 1000.458179126573]</t>
+  </si>
+  <si>
+    <t>[506.0, 561.3584487534627, 539.9456706281834, 545.8498137002007, 545.7283950617284, 539.8540145985402, 548.9475555555556, 530.363691376702, 534.3863920099875, 542.029187817259, 558.8504584255454, 564.5338148391332, 519.3679945982445, 522.0250958522133, 557.0320720720721, 529.6543301258328]</t>
+  </si>
+  <si>
+    <t>[473.0, 470.1889196675901, 454.140350877193, 438.79965606190893, 444.8641975308642, 431.88321167883214, 426.2287407407408, 436.375189107413, 446.6685393258427, 443.4784263959391, 439.59785014227, 440.70059093893633, 443.21066846725193, 434.3764377831997, 451.75567567567566, 446.1687638786085]</t>
+  </si>
+  <si>
+    <t>[437.0, 446.6282548476455, 440.53706847764573, 423.9610203496705, 430.0, 412.4484671532847, 395.54903703703707, 406.16459909228445, 439.74344569288394, 435.26586294416245, 424.3989883022447, 413.99146421536443, 424.4834571235652, 404.73056814220985, 425.1034234234234, 433.85122131754264]</t>
+  </si>
+  <si>
+    <t>[446.0, 419.9944598337951, 432.165817770232, 411.24218973918033, 425.7530864197531, 410.28905109489057, 391.16622222222225, 419.59152798789717, 423.5848938826467, 430.5729695431472, 395.1704078406576, 406.7071569271175, 407.0047265361243, 409.88637155803417, 430.43387387387384, 424.2709104367136]</t>
+  </si>
+  <si>
+    <t>[560.0, 527.5540166204987, 521.1103565365025, 522.5319575809689, 487.33333333333337, 521.4989781021899, 461.29125925925933, 565.0499243570348, 467.4438202247191, 490.4073604060914, 534.2984508378122, 490.47669074195665, 508.1316677920325, 537.4925060996864, 522.3841441441441, 494.0703182827536]</t>
+  </si>
+  <si>
+    <t>[478.0, 486.5789473684211, 461.46519524618, 435.6199484092864, 440.6172839506173, 431.88321167883214, 433.8986666666667, 435.256278366112, 439.74344569288394, 425.880076142132, 429.07556117609863, 437.05843729481285, 434.47130317353145, 427.93168351341933, 435.7643243243243, 435.21983715766106]</t>
+  </si>
+  <si>
+    <t>[477.0, 474.28642659279785, 475.0684776457272, 444.0991688162798, 438.4938271604938, 450.23824817518255, 445.9514074074075, 454.27776096823, 451.2852684144819, 455.2106598984772, 447.7818526715144, 456.4832567301379, 453.19851451721814, 443.3990937608923, 446.4252252252252, 450.27461139896377]</t>
+  </si>
+  <si>
+    <t>[491.0, 492.72520775623275, 498.08941709111485, 454.6981943250216, 440.6172839506173, 451.31795620437964, 447.0471111111112, 467.7046898638427, 461.6729088639201, 470.4625634517767, 464.14985773000313, 471.05187130663165, 468.1802835921675, 467.8891599860579, 457.0861261261261, 477.6469282013324]</t>
+  </si>
+  <si>
+    <t>[457.0, 449.7013850415513, 446.815506508206, 431.3803382057897, 424.6913580246914, 438.36145985401464, 432.802962962963, 438.61301059001516, 433.97253433208493, 435.26586294416245, 433.7521340499526, 433.4162836506894, 434.47130317353145, 422.775880097595, 431.7664864864865, 433.85122131754264]</t>
+  </si>
+  <si>
+    <t>[517.0, 515.2614958448754, 504.3678551216752, 503.4537116652337, 483.08641975308643, 500.9845255474453, 468.96118518518523, 472.1803328290469, 498.60674157303373, 486.88769035533, 515.5921593423965, 488.048588312541, 484.41053342336266, 502.6908330428721, 506.39279279279276, 506.38786084381945]</t>
+  </si>
+  <si>
+    <t>[696.0, 688.3811634349031, 679.117713638936, 664.5588993981085, 658.2716049382716, 664.0204379562044, 668.3792592592594, 673.5842662632375, 689.0468164794008, 692.2017766497462, 675.7647802718938, 667.7281680892975, 671.6826468602296, 670.2544440571628, 682.2976576576576, 687.0451517394523]</t>
+  </si>
+  <si>
+    <t>[651.0, 623.845429362881, 617.37973967176, 612.6236744052738, 605.1851851851852, 611.1147445255475, 570.8616296296298, 614.2819969742815, 595.558052434457, 615.9422588832488, 603.2779007271578, 598.5272488509521, 608.0101282916949, 622.5632624607878, 618.3322522522523, 618.6143597335308]</t>
+  </si>
+  <si>
+    <t>[672.0, 654.5767313019392, 659.2359932088285, 650.7801662367442, 631.7283950617284, 660.7813138686132, 655.230814814815, 670.2275340393344, 667.1173533083646, 700.4143401015228, 650.0436294656971, 653.1595535128037, 669.1856853477381, 676.6991983269432, 672.9693693693694, 678.8334566987418]</t>
+  </si>
+  <si>
+    <t>[463.0, 432.2869806094183, 421.70175438596493, 429.2605331040414, 410.8888888888889, 409.2093430656935, 403.218962962963, 417.353706505295, 422.4307116104869, 423.5336294416244, 408.03098324375594, 417.63361785948786, 408.25320729237006, 415.0421749738585, 417.10774774774774, 431.11398963730574]</t>
+  </si>
+  <si>
+    <t>[543.0, 535.7490304709141, 537.85285795133, 523.5918601318431, 521.3086419753087, 523.658394160584, 477.7268148148149, 521.4124054462935, 485.9107365792759, 519.7379441624366, 514.4230161239329, 496.54694681549574, 505.6347062795409, 516.8692924363891, 514.3884684684684, 522.8112509252406]</t>
+  </si>
+  <si>
+    <t>[1053.0, 903.5002770083104, 1045.3599320882852, 772.6689595872745, 924.7654320987655, 937.1865693430658, 922.5825185185187, 863.7990922844176, 967.2047440699126, 993.7201776649747, 939.9911476446412, 829.1969796454366, 895.1607022282243, 940.9341233879401, 856.8699099099099, 812.957809030348]</t>
+  </si>
+  <si>
+    <t>[809.0, 814.3795013850416, 707.3706847764573, 759.9501289767843, 741.0864197530865, 791.4259854014599, 702.3460740740742, 744.0756429652042, 749.0642946317104, 811.8705583756346, 762.2813784381916, 781.8489822718319, 815.2579338284944, 804.3053328685954, 819.5567567567567, 833.4870466321245]</t>
+  </si>
+  <si>
+    <t>[933.0, 923.9878116343491, 864.331635540464, 740.8718830610492, 813.283950617284, 827.0563503649636, 903.9555555555556, 847.0154311649017, 863.3283395755307, 876.3978426395939, 983.2494467277901, 865.6185160866711, 816.5064145847401, 835.2401533635414, 986.1333333333333, 1040.1480384900076]</t>
+  </si>
+  <si>
+    <t>[1009.0, 979.3041551246539, 912.4663271080929, 971.9306391516195, 926.8888888888889, 927.4691970802921, 900.6684444444446, 1037.2302571860816, 971.8214731585518, 863.4923857868021, 989.0951628201075, 951.8161523309258, 922.6272788656314, 949.9567793656327, 1004.7899099099099, 923.8156920799408]</t>
+  </si>
+  <si>
+    <t>[883.0, 837.9401662049862, 816.1969439728354, 779.0283748925195, 770.8148148148149, 816.2592700729928, 745.0785185185186, 756.3836611195159, 788.3064918851436, 874.0513959390863, 797.355674992096, 851.0499015101773, 806.5185685347739, 922.8888114325549, 883.5221621621621, 832.118430792006]</t>
+  </si>
+  <si>
+    <t>[711.0, 707.84432132964, 700.0458404074703, 684.6970478647178, 676.320987654321, 678.0566423357665, 689.1976296296298, 688.1301059001513, 706.3595505617977, 706.280456852792, 689.7944988934555, 692.0091923834538, 695.4037812288994, 687.0108051585919, 695.6237837837838, 702.0999259807551]</t>
+  </si>
+  <si>
+    <t>[739.0, 733.4537396121884, 749.2269383135257, 733.4525652049299, 700.7407407407408, 723.4043795620439, 736.312888888889, 734.0054462934947, 724.8264669163545, 735.6110406091371, 704.9933607334808, 729.6447800393959, 726.615800135044, 710.2119205298013, 722.276036036036, 700.7313101406367]</t>
+  </si>
+  <si>
+    <t>[680.0, 652.5279778393352, 651.9111488398415, 640.1811407280024, 643.4074074074074, 665.1001459854016, 640.9866666666668, 636.6602118003026, 676.350811485643, 688.6821065989848, 664.0733480872589, 632.5206828627709, 665.4402430790008, 650.9201812478216, 671.6367567567568, 688.4137675795707]</t>
+  </si>
+  <si>
+    <t>[606.0, 613.6016620498616, 607.9620826259196, 603.0845514474063, 564.8395061728395, 569.0061313868614, 574.1487407407408, 581.8335854765508, 610.5624219725344, 605.3832487309645, 586.9098956686689, 582.7445830597505, 583.0405131667793, 596.7842453816661, 616.9996396396396, 610.4026646928202]</t>
+  </si>
+  <si>
+    <t>[725.0, 707.84432132964, 702.1386530843237, 694.2361708225854, 710.2962962962963, 666.1798540145986, 662.9007407407408, 700.438124054463, 720.2097378277153, 720.3591370558377, 675.7647802718938, 668.9422193040052, 681.6704929101959, 716.6566747995818, 687.6281081081081, 721.2605477424131]</t>
+  </si>
+  <si>
+    <t>[808.0, 876.86648199446, 974.2043010752689, 905.1567784465465, 903.530864197531, 947.9836496350366, 993.8032592592593, 998.0683812405447, 1035.301498127341, 1065.286802030457, 938.8220044261776, 970.026920551543, 973.8149898717085, 944.8009759498084, 990.1311711711711, 1046.9911176905996]</t>
+  </si>
+  <si>
+    <t>[790.0, 817.4526315789475, 800.5008488964346, 775.8486672398969, 783.5555555555555, 744.9985401459855, 838.2133333333335, 807.8535552193646, 802.1566791510612, 755.5558375634519, 806.708820739804, 798.8456992777413, 769.0641458474005, 837.8180550714535, 816.8915315315315, 822.538119911177]</t>
+  </si>
+  <si>
+    <t>[590.0, 610.5285318559557, 610.054895302773, 599.9048437947837, 611.5555555555555, 565.7670072992702, 571.9573333333334, 607.5685325264751, 597.8664169787766, 615.9422588832488, 603.2779007271578, 607.0256073539067, 599.2707629979744, 580.027884280237, 624.9953153153153, 618.6143597335308]</t>
+  </si>
+  <si>
+    <t>[570.0, 551.1146814404433, 550.4097340124505, 536.3106907423331, 545.7283950617284, 522.5786861313869, 530.3205925925927, 560.5742813918306, 571.3202247191011, 561.9739847715737, 544.8207398039835, 535.3965856861457, 530.6043214044565, 527.1808992680377, 559.6972972972973, 551.5521835677276]</t>
+  </si>
+  <si>
+    <t>[753.0, 752.9168975069254, 740.855687606112, 723.9134422470623, 727.283950617284, 730.9623357664234, 728.6429629629631, 728.4108925869895, 758.2977528089888, 726.2252538071067, 717.8539361365791, 724.7885751805646, 729.1127616475355, 720.5235273614501, 732.936936936937, 726.7350111028868]</t>
+  </si>
+  <si>
+    <t>[701.0, 686.3324099722993, 678.0713073005094, 659.2593866437376, 664.641975308642, 643.50598540146, 657.4222222222223, 664.6329803328291, 689.0468164794008, 696.8946700507614, 680.4413531457477, 667.7281680892975, 666.6887238352465, 656.075984663646, 664.9736936936937, 687.0451517394523]</t>
+  </si>
+  <si>
+    <t>[638.0, 593.1141274238228, 606.9156762874929, 614.7434795070221, 540.4197530864197, 624.0712408759125, 602.6370370370371, 576.2390317700454, 619.7958801498128, 635.8870558375635, 709.6699336073348, 654.3736047275115, 646.7130317353141, 626.430115022656, 603.6735135135135, 614.5085122131755]</t>
+  </si>
+  <si>
+    <t>[483.0, 482.48144044321333, 486.57894736842104, 463.177414732015, 398.14814814814815, 397.3325547445256, 413.08029629629635, 415.1158850226929, 425.8932584269663, 436.43908629441626, 458.30414163768575, 422.4898227183191, 426.98041863605675, 421.48692924363894, 429.10126126126124, 435.21983715766106]</t>
+  </si>
+  <si>
+    <t>[785.0, 821.5501385041553, 668.653650254669, 746.17139581542, 733.6543209876544, 706.1290510948905, 792.1937777777779, 684.7733736762482, 745.601747815231, 789.5793147208122, 873.3499841922226, 695.6513460275771, 665.4402430790008, 618.6964098989196, 671.6367567567568, 680.2020725388602]</t>
+  </si>
+  <si>
+    <t>[823.0, 753.9412742382273, 819.3361629881155, 806.585841215248, 769.7530864197531, 766.5927007299271, 829.4477037037038, 840.3019667170953, 788.3064918851436, 755.5558375634519, 910.7625671830541, 881.4011818778727, 870.1910871033086, 890.6650400836529, 814.2263063063062, 860.859363434493]</t>
+  </si>
+  <si>
+    <t>[561.0, 558.2853185595568, 555.641765704584, 542.6701060475782, 535.1111111111111, 537.6945985401461, 540.181925925926, 542.6717095310137, 545.9282147315855, 553.761421319797, 540.1441669301296, 530.5403808273145, 531.8528021607023, 541.3593586615546, 541.0407207207207, 557.0266469282014]</t>
+  </si>
+  <si>
+    <t>[575.0, 577.7484764542937, 551.4561403508771, 550.0894239036975, 532.9876543209876, 537.6945985401461, 543.4690370370371, 540.4338880484115, 555.1616729088639, 553.761421319797, 542.4824533670566, 537.8246881155613, 539.343686698177, 545.2262112234229, 539.708108108108, 555.658031088083]</t>
+  </si>
+  <si>
+    <t>[518.0, 601.3091412742383, 579.7091114883984, 576.5869876755519, 537.2345679012346, 529.0569343065694, 569.765925925926, 502.3909228441755, 555.1616729088639, 570.1865482233503, 529.6218779639582, 542.6808929743927, 520.6164753544903, 568.4273265946323, 529.0472072072072, 552.9207994078461]</t>
+  </si>
+  <si>
+    <t>[679.0, 652.5279778393352, 611.1013016411998, 617.9231871596447, 613.6790123456791, 629.4697810218979, 624.5511111111111, 605.330711043873, 633.6460674157304, 601.8635786802031, 616.1384761302561, 614.3099146421537, 598.0222822417286, 626.430115022656, 631.6583783783783, 613.1398963730571]</t>
+  </si>
+  <si>
+    <t>[496.0, 528.5783933518006, 444.72269383135256, 510.8730295213529, 506.44444444444446, 463.1947445255475, 472.24829629629636, 471.0614220877459, 505.53183520599254, 486.88769035533, 468.8264306038571, 480.7642810242942, 485.65901417960845, 494.9571279191356, 454.4209009009009, 495.438934122872]</t>
+  </si>
+  <si>
+    <t>[538.0, 526.5296398891967, 565.0594227504245, 523.5918601318431, 541.4814814814815, 536.614890510949, 533.6077037037038, 548.266263237519, 515.9194756554307, 553.761421319797, 531.9601644008852, 514.7577150361129, 516.871033085753, 531.0477518299059, 546.3711711711711, 561.1324944485567]</t>
+  </si>
+  <si>
+    <t>[599.0, 529.6027700831025, 616.3333333333334, 606.2642591000288, 617.925925925926, 600.3176642335767, 565.3831111111111, 647.8493192133132, 579.3995006242197, 618.2887055837564, 592.7556117609864, 577.8883782009192, 581.7920324105335, 587.7615894039735, 586.3495495495495, 643.2494448556625]</t>
+  </si>
+  <si>
+    <t>[559.0, 603.3578947368421, 659.2359932088285, 669.8584121524793, 578.641975308642, 629.4697810218979, 588.3928888888889, 571.7633888048412, 567.8576779026217, 600.6903553299493, 633.6756244072084, 605.811556139199, 544.3376097231601, 609.673753921227, 634.3236036036036, 648.7239082161362]</t>
+  </si>
+  <si>
+    <t>[541.0, 512.1883656509696, 532.6208262591964, 482.2556606477502, 505.38271604938274, 454.55708029197086, 521.554962962963, 465.46686838124054, 483.6023720349563, 493.92703045685283, 487.53272209927286, 507.4734077478661, 514.3740715732614, 523.3140467061694, 535.7102702702703, 567.9755736491488]</t>
+  </si>
+  <si>
+    <t>[484.0, 473.2620498614959, 457.2795698924731, 449.3986815706507, 419.38271604938274, 449.15854014598546, 431.70725925925933, 444.20756429652045, 448.9769038701623, 456.383883248731, 430.2447043945621, 439.4865397242285, 458.1924375422013, 461.44440571627746, 443.76, 479.0155440414508]</t>
+  </si>
+  <si>
+    <t>[973.0, 963.9385041551247, 957.4617996604414, 948.6127830323877, 924.7654320987655, 928.5489051094892, 935.7309629629631, 930.9337367624811, 951.0461922596754, 960.8699238578681, 932.9762883338602, 929.9632304661851, 927.6212018906145, 930.6225165562914, 950.1527927927928, 951.1880088823095]</t>
+  </si>
+  <si>
+    <t>[1468.0, 1477.1512465373962, 1485.897000565931, 1465.8452278589857, 1429.0864197530866, 1456.5261313868614, 1455.0945185185187, 1419.897730711044, 1449.652933832709, 1464.1827411167515, 1447.3993044577933, 1441.0787918581746, 1440.7467927076302, 1434.6023004531196, 1463.2086486486485, 1449.3641746854184]</t>
+  </si>
+  <si>
+    <t>[1537.0, 1563.1988919667592, 1560.1918505942274, 1522.020063055317, 1503.4074074074074, 1524.5477372262776, 1519.7410370370371, 1532.907715582451, 1573.150436953808, 1565.0799492385788, 1570.1593423964591, 1530.918581746553, 1536.8798109385552, 1504.205646566748, 1543.1654054054054, 1564.3279052553667]</t>
+  </si>
+  <si>
+    <t>[1585.0, 1611.3445983379504, 1610.4193548387098, 1575.0151905990258, 1543.7530864197531, 1572.054890510949, 1564.664888888889, 1596.6856278366113, 1632.0137328339576, 1623.7411167512691, 1618.094214353462, 1623.1864740643466, 1578.079675894666, 1585.4095503659812, 1619.1243243243243, 1604.017764618801]</t>
+  </si>
+  <si>
+    <t>[2488.0, 2473.8698060941833, 2531.256932654216, 2385.8406420177707, 2384.641975308642, 2446.618394160584, 2492.7259259259263, 2374.3285930408474, 2558.8220973782772, 2444.997461928934, 2337.1172937085043, 2328.550229809586, 2380.8528021607026, 2452.8734750784247, 2498.6486486486483, 2375.9170984455964]</t>
+  </si>
+  <si>
+    <t>[1427.0, 1524.2725761772856, 1421.0198075834749, 1427.6887360275152, 1433.3333333333335, 1559.0983941605841, 1573.4305185185187, 1475.8432677760968, 1562.7627965043696, 1609.6624365482235, 1537.4233322794814, 1617.1162179908076, 1568.0918298446998, 1484.8713837574069, 1553.8263063063062, 1601.2805329385642]</t>
+  </si>
+  <si>
+    <t>[1852.0, 1789.5861495844877, 1825.9790605546123, 1699.0237890513044, 1724.246913580247, 1790.1559124087594, 1796.9540740740742, 1857.391830559758, 1770.5156054931338, 1802.0710659898477, 1871.7982927600378, 1834.4313854235063, 1850.248480756246, 1856.0892296967586, 1920.2947747747746, 1739.5107327905257]</t>
+  </si>
+  <si>
+    <t>[1920.0, 1943.2426592797785, 1837.4895302773061, 1925.8429349383782, 1871.8271604938273, 1910.0035036496354, 1906.5244444444447, 1784.662632375189, 1995.5811485642946, 2097.7233502538074, 1918.5640214985772, 1937.6257386736704, 1862.733288318704, 1984.9843150923668, 2061.5517117117115, 1966.7009622501853]</t>
+  </si>
+  <si>
+    <t>[1784.0, 1760.9036011080334, 1747.498585172609, 1835.751218114073, 1774.1481481481483, 1638.996788321168, 1539.463703703704, 1682.8417549167928, 1784.3657927590511, 1692.9612944162438, 1703.4416693012963, 1762.8023637557453, 1774.0911546252535, 1736.2168002788428, 1861.6598198198196, 1798.3612139156182]</t>
+  </si>
+  <si>
+    <t>[1761.0, 1790.6105263157897, 1817.6078098471987, 1584.5543135568935, 1939.7777777777778, 1658.4315328467155, 1585.4832592592595, 1664.939183055976, 1682.797752808989, 1816.1497461928936, 1675.3822320581726, 1919.4149704530532, 1736.63673193788, 1749.1063088184037, 1677.759279279279, 1699.8208734270913]</t>
+  </si>
+  <si>
+    <t>[1431.0, 1454.6149584487537, 1464.9688737973968, 1488.1031814273433, 1450.320987654321, 1555.8592700729928, 1607.3973333333336, 1530.6698940998488, 1608.9300873907616, 1622.5678934010155, 1462.5981662978186, 1668.1063690085357, 1445.7407157326134, 1545.4520738933427, 1536.5023423423422, 1775.094744633605]</t>
+  </si>
+  <si>
+    <t>[1563.0, 1599.052077562327, 1598.9088851160159, 1679.9455431355693, 1527.8271604938273, 1665.989489051095, 1715.8720000000003, 1714.1712556732225, 1611.2384519350812, 1680.0558375634519, 1634.4622194119506, 1664.4642153644124, 1591.8129642133695, 1661.45765074939, 1561.821981981982, 1604.017764618801]</t>
+  </si>
+  <si>
+    <t>[922.0, 915.7927977839337, 892.5846066779853, 869.1200917168245, 855.7530864197531, 864.8461313868614, 815.2035555555557, 821.2804841149773, 918.729088639201, 884.6104060913706, 863.9968384445147, 887.4714379514116, 892.6637407157327, 953.823631927501, 950.1527927927928, 966.2427831236123]</t>
+  </si>
+  <si>
+    <t>[1729.0, 1526.3213296398894, 1684.7142048670062, 1507.1814273430784, 1537.3827160493827, 1524.5477372262776, 1691.7665185185188, 1629.1340393343419, 1742.8152309612985, 1698.8274111675128, 1758.39140056908, 1716.6684175968483, 1782.8305199189738, 1710.4377831997213, 1512.5153153153153, 1572.5396002960772]</t>
+  </si>
+  <si>
+    <t>[1148.0, 1191.3501385041552, 1210.6921335597058, 1205.1092003439383, 1036.2469135802469, 1153.128175182482, 1145.0103703703705, 1343.811800302572, 1282.296504369538, 1152.1053299492387, 1232.2769522605122, 1177.629678266579, 1147.3538149898718, 1035.0275357267342, 1022.1138738738738, 1161.9548482605478]</t>
+  </si>
+  <si>
+    <t>[1336.0, 1312.2265927977842, 1261.9660441426147, 1210.4087130983091, 1212.493827160494, 1241.6642335766426, 1261.154962962963, 1366.1900151285931, 1342.3139825218477, 1345.6871827411169, 1466.1055959532089, 1290.5364412344059, 1260.965563808238, 1276.0613454165216, 1351.269189189189, 1160.5862324204295]</t>
+  </si>
+  <si>
+    <t>[1383.0, 1423.8836565096954, 1436.7159026598754, 1406.4906850100317, 1390.8641975308642, 1363.6712408759126, 1395.9265185185186, 1370.6656580937974, 1416.181647940075, 1373.8445431472082, 1364.390135946886, 1373.091923834537, 1415.7771775827146, 1336.6420355524574, 1341.940900900901, 1387.776461880089]</t>
+  </si>
+  <si>
+    <t>[878.0, 903.5002770083104, 985.7147707979626, 939.07366007452, 1029.8765432098767, 940.425693430657, 934.6352592592593, 1038.3491679273827, 1032.9931335830213, 1123.9479695431473, 965.7122984508378, 963.956664478004, 958.8332207967591, 1198.7242941791565, 1245.9927927927927, 1111.316062176166]</t>
+  </si>
+  <si>
+    <t>[1642.0, 1691.2459833795017, 1659.600452744765, 1609.9919747778736, 1767.7777777777778, 1742.6487591240877, 1681.9051851851855, 1694.0308623298033, 1793.5992509363296, 1608.4892131979698, 1626.2782168827064, 1685.1030860144451, 1769.0972316002703, 1755.551063088184, 1619.1243243243243, 1734.036269430052]</t>
+  </si>
+  <si>
+    <t>[1404.0, 1422.8592797783936, 1507.871533672892, 1425.568930925767, 1312.2962962962963, 1369.069781021898, 1479.2000000000003, 1398.6384266263237, 1469.2740324594258, 1396.1357868020305, 1377.2507113499842, 1439.8647406434668, 1448.2376772451048, 1381.7553154409202, 1353.9344144144143, 1424.7290895632866]</t>
+  </si>
+  <si>
+    <t>[1647.0, 1702.5141274238229, 1793.5404640633842, 1842.1106334193182, 1738.0493827160494, 1689.743065693431, 1678.6180740740742, 1717.5279878971257, 1900.9382022471912, 1701.1738578680204, 1601.7262092949732, 1671.7485226526592, 1912.672518568535, 1597.010108051586, 1559.1567567567567, 1699.8208734270913]</t>
+  </si>
+  <si>
+    <t>[1443.0, 1364.469806094183, 1392.7668364459537, 1257.044425336773, 1261.3333333333335, 1254.6207299270075, 1176.7857777777779, 1504.9349470499244, 1331.9263420724096, 1311.6637055837564, 1307.102118242175, 1370.6638214051216, 1441.995273463876, 1259.3049843150925, 1333.9452252252252, 1526.0066617320506]</t>
+  </si>
+  <si>
+    <t>[1425.0, 1424.9080332409974, 1427.298245614035, 1423.4491258240187, 1365.3827160493827, 1398.2218978102192, 1388.2565925925928, 1355.0009077155826, 1360.7808988764045, 1397.3090101522844, 1366.7284223838128, 1393.73079448457, 1384.56515867657, 1363.710003485535, 1397.9106306306305, 1375.4589193190232]</t>
+  </si>
+  <si>
+    <t>[1604.0, 1589.8326869806097, 1588.4448217317488, 1593.0335339638868, 1523.5802469135804, 1567.7360583941609, 1549.3250370370372, 1531.7888048411498, 1556.9918851435707, 1529.8832487309646, 1543.2690483717988, 1570.9822718319108, 1536.8798109385552, 1513.2283025444406, 1539.1675675675674, 1546.535899333827]</t>
+  </si>
+  <si>
+    <t>[1662.0, 1576.5157894736844, 1534.0316921335598, 1590.9137288621384, 1536.320987654321, 1541.8230656934309, 1493.4441481481483, 1488.1512859304084, 1434.6485642946318, 1486.4739847715737, 1474.2895984824534, 1539.4169402495074, 1534.3828494260636, 1455.225514116417, 1533.837117117117, 1526.0066617320506]</t>
+  </si>
+  <si>
+    <t>[1894.0, 1908.4138504155128, 1949.4550084889643, 1855.8893665806825, 1843.1604938271605, 1875.4528467153286, 1834.2080000000003, 1796.9706505295007, 1835.1498127340824, 1818.4961928934013, 1818.0177047107177, 1832.0032829940906, 1760.3578663065498, 1876.7124433600559, 1904.3034234234233, 1828.4707623982238]</t>
+  </si>
+  <si>
+    <t>[1114.0, 1161.643213296399, 1128.0260328239954, 1202.9893952421899, 1113.7530864197531, 1100.222481751825, 1079.2681481481484, 1002.5440242057489, 1129.9444444444446, 1091.0977157360408, 1055.736326272526, 1098.7163493105713, 1096.1661039837948, 1042.7612408504706, 1132.7207207207207, 1052.4655810510735]</t>
+  </si>
+  <si>
+    <t>[1528.0, 1555.0038781163437, 1599.9552914544427, 1538.9785038693037, 1500.2222222222224, 1514.8303649635038, 1487.9656296296298, 1502.6971255673222, 1492.3576779026218, 1546.308375634518, 1503.5181789440405, 1527.2764281024295, 1474.4557731262662, 1460.3813175322414, 1517.8457657657657, 1497.2657290895634]</t>
+  </si>
+  <si>
+    <t>[1357.0, 1394.1767313019393, 1380.209960384833, 1461.605617655489, 1323.9753086419753, 1372.3089051094892, 1343.332740740741, 1293.4608169440244, 1336.5430711610488, 1396.1357868020305, 1351.5295605437875, 1397.3729481286935, 1399.5469277515194, 1383.0442662948763, 1348.603963963964, 1327.557364914878]</t>
+  </si>
+  <si>
+    <t>[1004.0, 922.9634349030472, 933.394453876627, 962.391516193752, 939.6296296296297, 959.8604379562045, 912.7211851851853, 977.9279878971256, 900.2621722846442, 935.0590101522844, 920.1157129307619, 1011.3046618516087, 950.0938555030386, 1015.6932729173928, 1108.7336936936936, 944.3449296817174]</t>
+  </si>
+  <si>
+    <t>[958.0, 957.7922437673132, 1087.2161856253538, 999.4881054743481, 947.0617283950618, 1055.9544525547446, 937.9223703703705, 1009.2574886535552, 998.3676654182273, 1013.6649746192894, 949.3442933923491, 927.5351280367695, 935.1120864280892, 1005.3816660857442, 959.481081081081, 1005.9326424870468]</t>
+  </si>
+  <si>
+    <t>[1910.0, 1942.2182825484767, 1992.3576683644594, 1989.4370879908288, 1873.9506172839508, 1904.60496350365, 2064.305777777778, 1967.0450832072618, 1932.1011235955057, 2042.5818527918784, 1982.866898514069, 1916.9868680236375, 2164.8656313301826, 1973.383757406762, 2080.2082882882883, 2025.5514433752778]</t>
+  </si>
+  <si>
+    <t>[2202.0, 2156.3130193905818, 2182.8036219581213, 2028.6534823731731, 2033.20987654321, 2144.3001459854017, 2251.6711111111113, 2108.027836611195, 2187.1754057428216, 2269.013959390863, 2192.1435346190324, 2164.6533158240313, 2360.87711006077, 2253.086092715232, 2278.7675675675673, 2215.7890451517396]</t>
+  </si>
+  <si>
+    <t>[1235.0, 1231.3008310249309, 1207.5529145444257, 1212.5285182000575, 1211.432098765432, 1177.9614598540147, 1241.4322962962965, 1240.8720121028746, 1229.2041198501872, 1253.002538071066, 1192.5260828327537, 1222.5495732107681, 1209.7778528021609, 1237.3928197978391, 1273.9776576576576, 1237.2287194670616]</t>
+  </si>
+  <si>
+    <t>[1603.0, 1448.468698060942, 1418.9269949066213, 1489.1630839782176, 1495.9753086419753, 1444.6493430656935, 1496.7312592592596, 1519.4807866868382, 1509.6704119850187, 1574.4657360406093, 1455.5833069870375, 1504.209455022981, 1533.1343686698178, 1511.9393516904845, 1548.4958558558558, 1520.532198371577]</t>
+  </si>
+  <si>
+    <t>[1148.0, 1166.7650969529088, 1178.2535370684777, 1141.5150472914877, 1163.6543209876543, 1106.7007299270074, 1235.953777777778, 1143.5267776096823, 1181.8826466916355, 1220.1522842639595, 1162.128359152703, 1138.7800393959292, 1148.6022957461175, 1171.6563262460788, 1222.0057657657658, 1153.7431532198373]</t>
+  </si>
+  <si>
+    <t>[1226.0, 1255.8858725761775, 1199.181663837012, 1217.8280309544284, 1176.3950617283951, 1180.1208759124088, 1150.488888888889, 1173.737367624811, 1194.5786516853932, 1206.0736040609138, 1163.2975023711665, 1215.2652659225214, 1186.0567184334911, 1214.1917044266295, 1272.645045045045, 1235.860103626943]</t>
+  </si>
+  <si>
+    <t>[1095.0, 1155.4969529085874, 1187.671194114318, 1085.3402120951564, 1163.6543209876543, 1139.0919708029198, 1004.7602962962965, 1236.3963691376703, 1069.926966292135, 1125.121192893401, 1114.1934871957003, 1198.268548916612, 1193.5476029709657, 1035.0275357267342, 1163.3708108108108, 1137.3197631384162]</t>
+  </si>
+  <si>
+    <t>[1151.0, 1189.3013850415514, 1191.856819468025, 1153.1739753511038, 1087.20987654321, 1207.1135766423358, 1155.9674074074076, 1113.3161875945539, 1127.636079900125, 1126.294416243655, 1111.8552007587732, 1116.9271175311885, 1176.0688723835249, 1140.7215057511328, 1148.712072072072, 1145.5314581791267]</t>
+  </si>
+  <si>
+    <t>[1169.0, 1200.5695290858728, 1325.796830786644, 1164.8329034107196, 1082.962962962963, 1182.280291970803, 1126.3834074074075, 1169.2617246596067, 1155.3364544319602, 1121.6015228426397, 1051.0597533986722, 1085.3617859487854, 1083.681296421337, 1185.8347856395958, 1090.077117117117, 1119.5277572168766]</t>
+  </si>
+  <si>
+    <t>[2271.0, 2282.3113573407204, 2193.267685342388, 2243.813700200631, 2310.320987654321, 2258.749197080292, 2058.8272592592593, 2235.583661119516, 2227.5717852684147, 2292.478426395939, 2237.7401201391085, 2290.9146421536443, 2153.6293045239704, 2058.4545137678633, 2244.1196396396394, 2098.0880829015546]</t>
+  </si>
+  <si>
+    <t>[2513.0, 2332.5058171745154, 2451.730050933786, 2029.7133849240474, 2125.58024691358, 2253.3506569343067, 2299.8820740740744, 2165.0922844175493, 2629.227215980025, 2245.549492385787, 2234.2326904837178, 2180.4359816152332, 2305.943956785956, 2400.0264900662255, 2497.3160360360357, 2295.168763878609]</t>
+  </si>
+  <si>
+    <t>[1271.0, 1290.7146814404434, 1319.5183927560838, 1295.2009171682432, 1263.4567901234568, 1334.5191240875913, 1302.791703703704, 1209.5425113464448, 1386.1729088639202, 1278.8134517766498, 1365.5592791653494, 1333.0282337491792, 1340.8683322079678, 1303.1293133495992, 1373.9236036036036, 1376.8275351591415]</t>
+  </si>
+  <si>
+    <t>[819.0, 1086.8637119113575, 1120.7011884550084, 1154.2338779019778, 932.1975308641976, 1058.1138686131387, 1033.2485925925928, 993.5927382753405, 1150.719725343321, 1085.2315989847716, 1101.3329117926019, 1273.5397242284964, 995.0391627278867, 1077.5629139072848, 1016.7834234234234, 1108.578830495929]</t>
+  </si>
+  <si>
+    <t>[1232.0, 1438.2249307479226, 1209.645727221279, 1172.252221266839, 1227.3580246913582, 1035.44, 1239.240888888889, 1179.3319213313162, 1198.0411985018727, 1194.3413705583757, 1210.063231109706, 1274.7537754432042, 1113.6448345712358, 1254.149180899268, 1280.6407207207208, 1189.3271650629165]</t>
+  </si>
+  <si>
+    <t>[641.0, 622.821052631579, 622.6117713638936, 620.042992261393, 618.9876543209876, 599.2379562043797, 594.9671111111112, 616.5198184568835, 626.7209737827716, 614.769035532995, 627.8299083148909, 625.236375574524, 616.7494935854153, 616.1185081910073, 634.3236036036036, 633.6691339748336]</t>
+  </si>
+  <si>
+    <t>[661.0, 611.5529085872577, 629.9366157328806, 611.5637718543996, 594.5679012345679, 589.5205839416059, 579.6272592592593, 582.9524962178517, 594.4038701622972, 638.2335025380711, 598.6013278533038, 633.7347340774786, 626.7373396353815, 543.9372603694668, 603.6735135135135, 641.8808290155441]</t>
+  </si>
+  <si>
+    <t>[558.0, 597.2116343490305, 558.7809847198641, 557.5087417598166, 560.5925925925926, 538.7743065693431, 556.6174814814816, 561.6931921331317, 563.2409488139825, 608.9029187817259, 567.0344609547898, 607.0256073539067, 588.0344361917624, 523.3140467061694, 559.6972972972973, 599.4537379718728]</t>
+  </si>
+  <si>
+    <t>[922.0, 915.7927977839337, 893.631013016412, 901.9770707939239, 940.6913580246915, 889.6794160583943, 921.4868148148149, 891.771860816944, 923.3458177278402, 936.2322335025382, 928.2997154600063, 915.3946158896914, 920.1303173531398, 939.645172533984, 976.805045045045, 911.498149518875]</t>
+  </si>
+  <si>
+    <t>[811.0, 845.1108033240998, 829.8002263723826, 825.6640871309833, 801.604938271605, 787.1071532846717, 841.5004444444446, 807.8535552193646, 835.6279650436954, 851.760152284264, 847.6288333860259, 832.8391332895601, 817.754895340986, 814.6169397002441, 871.5286486486486, 918.3412287194672]</t>
+  </si>
+  <si>
+    <t>[1131.0, 1048.9617728531857, 1054.7775891341257, 1060.9624534250504, 1107.3827160493827, 1114.258686131387, 1113.2349629629632, 1060.727382753404, 1144.9488139825219, 1139.1998730964467, 1086.1340499525766, 1101.1444517399868, 1103.6569885212696, 1094.319275008714, 1126.0576576576575, 1053.8341968911918]</t>
+  </si>
+  <si>
+    <t>[636.0, 631.0160664819946, 624.704584040747, 627.4623101175123, 625.3580246913581, 592.7597080291971, 588.3928888888889, 608.6874432677761, 599.0205992509364, 610.0761421319797, 631.3373379702814, 636.1628365068943, 621.7434166103984, 654.7870338096898, 627.6605405405405, 640.5122131754257]</t>
+  </si>
+  <si>
+    <t>[533.0, 514.2371191135735, 513.7855121675155, 509.8131269704787, 491.58024691358025, 471.8324087591241, 474.43970370370374, 480.01270801815434, 488.2191011235955, 488.0609137055838, 505.0698703762251, 489.26263952724884, 485.65901417960845, 478.20076681770655, 511.72324324324325, 510.4937083641747]</t>
+  </si>
+  <si>
+    <t>[518.0, 492.72520775623275, 480.3005093378608, 452.57838922327323, 441.67901234567904, 443.76000000000005, 441.56859259259267, 454.27776096823, 462.8270911360799, 469.2893401015229, 472.33386025924756, 457.6973079448457, 470.67724510465905, 451.1327988846288, 474.4100900900901, 476.278312361214]</t>
+  </si>
+  <si>
+    <t>[486.0, 459.94515235457067, 452.04753820033955, 438.79965606190893, 436.3703703703704, 423.2455474452555, 447.0471111111112, 441.96974281391834, 450.1310861423221, 451.6909898477158, 430.2447043945621, 445.55679579776756, 419.4895340985821, 417.6200766817707, 425.1034234234234, 457.11769059955594]</t>
+  </si>
+  <si>
+    <t>[601.0, 614.6260387811635, 733.530843237125, 603.0845514474063, 673.1358024691358, 641.3465693430658, 569.765925925926, 663.514069591528, 615.1791510611736, 657.005076142132, 696.8093582042364, 668.9422193040052, 636.7251856853478, 543.9372603694668, 642.3192792792793, 637.7749814951889]</t>
+  </si>
+  <si>
+    <t>[551.0, 545.9927977839336, 527.3887945670629, 531.0111779879622, 531.925925925926, 484.7889051094891, 499.640888888889, 521.4124054462935, 519.3820224719101, 491.5805837563452, 509.74644325007904, 503.8312541037426, 500.6407832545578, 494.9571279191356, 531.7124324324324, 526.9170984455959]</t>
+  </si>
+  <si>
+    <t>[604.0, 586.9678670360112, 573.4306734578381, 547.9696188019491, 548.9135802469136, 545.2525547445256, 548.9475555555556, 561.6931921331317, 569.0118601747815, 572.5329949238579, 570.5418906101802, 573.032173342088, 555.5739365293721, 551.6709654932032, 549.0363963963964, 576.1872686898595]</t>
+  </si>
+  <si>
+    <t>[607.0, 587.9922437673131, 590.1731748726655, 579.7666953281744, 573.3333333333334, 558.2090510948906, 559.9045925925926, 575.1201210287444, 570.1660424469413, 579.5723350253808, 576.3876067024976, 576.6743269862114, 558.0708980418636, 568.4273265946323, 566.3603603603603, 574.818652849741]</t>
+  </si>
+  <si>
+    <t>[559.0, 520.3833795013851, 520.0639501980759, 503.4537116652337, 428.9382716049383, 504.22364963503657, 465.67407407407416, 529.244780635401, 525.1529338327091, 520.9111675126904, 509.74644325007904, 532.9684832567301, 504.38622552329514, 502.6908330428721, 535.7102702702703, 507.7564766839379]</t>
+  </si>
+  <si>
+    <t>[638.0, 626.9185595567868, 641.4470854555744, 632.7618228718832, 644.4691358024692, 592.7597080291971, 623.4554074074075, 628.8278366111952, 599.0205992509364, 640.5799492385787, 690.9636421119191, 701.7216021011162, 631.7312626603647, 632.8748692924364, 666.3063063063063, 651.4611398963731]</t>
+  </si>
+  <si>
+    <t>[846.0, 854.3301939058173, 842.3571024335031, 823.5442820292349, 813.283950617284, 816.2592700729928, 841.5004444444446, 825.7561270801816, 849.478152309613, 864.6656091370559, 856.9819791337338, 866.8325673013788, 868.9426063470629, 889.3760892296968, 891.5178378378378, 900.5492227979275]</t>
+  </si>
+  <si>
+    <t>[949.0, 956.7678670360112, 945.9513299377476, 932.7142447692751, 892.9135802469136, 901.5562043795621, 918.1997037037038, 899.6042360060515, 929.1167290886392, 930.3661167512691, 930.6380018969332, 960.3145108338805, 950.0938555030386, 982.1805507145348, 995.4616216216216, 1000.458179126573]</t>
+  </si>
+  <si>
+    <t>[911.0, 912.7196675900278, 896.7702320316921, 874.4196044711954, 841.9506172839507, 840.0128467153286, 867.7973333333334, 849.2532526475038, 902.5705368289638, 903.3819796954316, 913.100853619981, 905.6822061720289, 913.887913571911, 931.9114674102475, 982.1354954954954, 964.8741672834939]</t>
+  </si>
+  <si>
+    <t>[468.0, 505.017728531856, 497.0430107526882, 499.21410146173696, 437.4320987654321, 459.95562043795627, 438.28148148148153, 459.87231467473526, 461.6729088639201, 495.10025380710664, 466.4881441669301, 496.54694681549574, 483.1620526671169, 501.40188218891603, 506.39279279279276, 463.9607698001481]</t>
+  </si>
+  <si>
+    <t>[764.0, 721.1612188365652, 763.8766270514997, 735.5723703066783, 741.0864197530865, 776.3100729927008, 742.8871111111112, 693.7246596066566, 751.37265917603, 732.0913705583757, 728.3762251027506, 774.5646749835851, 745.3430114787307, 781.1042174973859, 795.5697297297297, 819.8008882309401]</t>
+  </si>
+  <si>
+    <t>[950.0, 916.8171745152356, 1081.98415393322, 1224.1874462596734, 1105.2592592592594, 1085.1065693430658, 1035.44, 1075.2732223903176, 1035.301498127341, 1409.0412436548224, 1027.6768890294024, 1092.6460932370321, 1178.5658338960163, 1310.8630184733358, 1255.321081081081, 1204.3819393042193]</t>
+  </si>
+  <si>
+    <t>[1048.0, 1083.7905817174517, 1220.109790605546, 1089.5798222986532, 1004.3950617283951, 1111.0195620437958, 1124.1920000000002, 1155.834795763994, 1123.0193508114858, 1008.9720812182742, 1162.128359152703, 1164.275114904793, 1111.1478730587442, 1170.3673753921228, 1292.634234234234, 1342.6121391561808]</t>
+  </si>
+  <si>
+    <t>[1345.0, 1364.469806094183, 1257.7804187889078, 1215.70822585268, 1046.8641975308642, 1093.7442335766425, 1086.9380740740742, 1066.3219364599092, 1164.5699126092386, 1098.1370558375636, 1118.8700600695543, 1139.994090610637, 1206.0324105334234, 1184.5458347856397, 1166.036036036036, 1178.378238341969]</t>
+  </si>
+  <si>
+    <t>[1239.0, 1251.7883656509696, 1192.9032258064517, 1129.8561192318718, 1189.1358024691358, 1221.149781021898, 1272.112, 1140.170045385779, 1134.5611735330838, 1156.798223350254, 1243.968384445147, 1184.913985554826, 1244.7353139770428, 1237.3928197978391, 1192.6882882882883, 1296.0792005921542]</t>
+  </si>
+  <si>
+    <t>[1264.0, 1187.2526315789476, 1278.708545557442, 1115.0174835196333, 1052.172839506173, 1001.9690510948906, 1129.6705185185187, 1109.9594553706506, 1128.7902621722847, 1101.656725888325, 1113.0243439772369, 1246.8305975049245, 1204.7839297771777, 1274.7723945625655, 1111.3989189189188, 1304.2908956328647]</t>
+  </si>
+  <si>
+    <t>[738.0, 752.9168975069254, 740.855687606112, 734.5124677558041, 744.2716049382716, 726.6435036496351, 766.9925925925927, 747.4323751891075, 757.143570536829, 770.8077411167513, 761.1122352197281, 751.4977019041365, 772.8095881161379, 779.8152666434298, 782.2436036036036, 799.2716506291637]</t>
+  </si>
+  <si>
+    <t>[778.0, 761.1119113573408, 826.6610073571024, 731.3327601031816, 777.1851851851852, 810.8607299270074, 810.8207407407408, 731.7676248108926, 781.3813982521848, 787.2328680203046, 754.0973759089472, 808.5581089954038, 757.8278190411885, 747.5914952945277, 750.2609009009009, 814.3264248704664]</t>
+  </si>
+  <si>
+    <t>[689.0, 729.3562326869807, 707.3706847764573, 731.3327601031816, 741.0864197530865, 689.9334306569344, 749.4613333333334, 702.6759455370651, 708.6679151061173, 723.8788071065991, 709.6699336073348, 738.1431385423506, 767.8156650911548, 804.3053328685954, 760.9218018018017, 766.4248704663213]</t>
+  </si>
+  <si>
+    <t>[593.0, 667.8936288088644, 627.8438030560271, 656.0796789911151, 654.0246913580247, 647.8248175182482, 661.8050370370371, 582.9524962178517, 631.3377028714108, 630.0209390862944, 627.8299083148909, 610.6677609980302, 701.6461850101284, 649.6312303938655, 605.0061261261261, 684.3079200592155]</t>
+  </si>
+  <si>
+    <t>[926.0, 771.3556786703602, 768.0622524052066, 804.4660361134997, 811.1604938271605, 806.5418978102191, 872.1801481481483, 814.5670196671709, 832.165418227216, 876.3978426395939, 844.1214037306355, 787.919238345371, 825.2457798784606, 790.1268734750785, 934.1614414414414, 804.7461139896374]</t>
+  </si>
+  <si>
+    <t>[983.0, 988.5235457063714, 1067.3344651952461, 1082.160504442534, 1088.2716049382716, 1092.6645255474455, 1124.1920000000002, 1137.9322239031771, 1098.7815230961298, 1107.522842639594, 1097.8254821372116, 1127.8535784635587, 1118.638757596219, 1126.543046357616, 1111.3989189189188, 1070.257586972613]</t>
+  </si>
+  <si>
+    <t>[1004.0, 1068.4249307479226, 978.3899264289756, 1036.5846947549444, 1087.20987654321, 932.8677372262775, 1036.5357037037038, 1024.92223903177, 986.8258426966293, 1088.7512690355331, 1007.8014543155232, 1074.435325016415, 1018.7602970965565, 988.6253049843151, 1022.1138738738738, 988.1406365655072]</t>
+  </si>
+  <si>
+    <t>[654.0, 631.0160664819946, 629.9366157328806, 640.1811407280024, 640.2222222222223, 590.600291970803, 632.2210370370371, 638.8980332829047, 638.2627965043696, 631.1941624365483, 653.5510591210875, 624.0223243598161, 662.9432815665092, 649.6312303938655, 682.2976576576576, 663.778682457439]</t>
+  </si>
+  <si>
+    <t>[558.0, 584.9191135734072, 557.7345783814375, 569.1676698194326, 535.1111111111111, 543.0931386861314, 565.3831111111111, 546.0284417549168, 543.6198501872659, 569.0133248730965, 549.4973126778375, 543.8949441891004, 570.5557056043215, 577.4499825723249, 583.6843243243243, 581.6617320503332]</t>
+  </si>
+  <si>
+    <t>[903.0, 872.7689750692522, 869.5636672325976, 833.0834049871024, 861.0617283950618, 833.5345985401461, 879.8500740740742, 847.0154311649017, 836.7821473158552, 781.3667512690356, 860.4894087891242, 842.5515430072226, 697.900742741391, 842.9738584872779, 796.9023423423423, 784.2168763878609]</t>
+  </si>
+  <si>
+    <t>[670.0, 799.0138504155126, 739.8092812676854, 645.4806534823733, 702.8641975308642, 669.4189781021898, 665.0921481481482, 796.664447806354, 729.4431960049938, 759.0755076142133, 703.8242175150174, 709.0059093893631, 704.14314652262, 761.7699546880447, 696.9563963963964, 687.0451517394523]</t>
+  </si>
+  <si>
+    <t>[834.0, 828.7207756232688, 830.8466327108093, 816.1249641731157, 811.1604938271605, 817.3389781021899, 820.6820740740742, 827.9939485627837, 837.936329588015, 852.9333756345178, 824.2459690167562, 818.2705187130663, 823.9972991222148, 809.4611362844197, 834.2154954954955, 838.9615099925982]</t>
+  </si>
+  <si>
+    <t>[602.0, 599.2603878116345, 569.2450481041313, 505.57351676698204, 485.2098765432099, 509.622189781022, 500.7365925925927, 497.91527987897126, 505.53183520599254, 502.1395939086295, 499.2241542839077, 463.76756401838475, 500.6407832545578, 500.11293133495997, 489.0688288288288, 525.5484826054775]</t>
+  </si>
+  <si>
+    <t>[809.0, 815.4038781163435, 822.4753820033956, 795.9868157065063, 803.7283950617284, 794.6651094890512, 811.9164444444446, 803.3779122541604, 819.4694132334582, 843.5475888324873, 804.370534302877, 786.7051871306631, 775.3065496286295, 781.1042174973859, 807.5632432432432, 823.9067357512954]</t>
+  </si>
+  <si>
+    <t>[936.0, 904.5246537396123, 903.0486700622524, 892.4379478360563, 874.8641975308642, 889.6794160583943, 886.4242962962965, 902.9609682299547, 922.1916354556804, 923.3267766497463, 904.9168510907366, 910.5384110308602, 928.8696826468604, 909.9993028929941, 942.1571171171171, 923.8156920799408]</t>
+  </si>
+  <si>
+    <t>[762.0, 753.9412742382273, 736.6700622524052, 746.17139581542, 731.530864197531, 727.7232116788322, 739.6000000000001, 728.4108925869895, 738.6766541822722, 760.2487309644671, 744.7442301612393, 747.8555482600132, 750.3369345037138, 761.7699546880447, 770.25009009009, 780.1110288675056]</t>
+  </si>
+  <si>
+    <t>[793.0, 787.7457063711912, 756.5517826825127, 772.6689595872745, 754.8888888888889, 752.556496350365, 761.5140740740742, 746.3134644478064, 766.3770287141074, 795.4454314720813, 770.465380967436, 778.2068286277084, 775.3065496286295, 783.682119205298, 795.5697297297297, 797.9030347890453]</t>
+  </si>
+  <si>
+    <t>[706.0, 698.6249307479226, 646.679117147708, 599.9048437947837, 634.9135802469136, 563.607591240876, 679.3362962962964, 661.2762481089259, 717.9013732833957, 716.8394670050762, 701.4859310780904, 659.2298095863428, 690.4098582039163, 680.5660508888114, 686.2954954954955, 697.9940784603998]</t>
+  </si>
+  <si>
+    <t>[868.0, 873.7933518005541, 872.7028862478777, 894.5577529378047, 870.6172839506173, 901.5562043795621, 902.859851851852, 886.1773071104387, 914.1123595505618, 884.6104060913706, 894.3945621245653, 892.327642810243, 868.9426063470629, 875.1976298361799, 883.5221621621621, 899.1806069578091]</t>
+  </si>
+  <si>
+    <t>[602.0, 612.5772853185596, 600.6372382569326, 641.2410432788765, 554.2222222222223, 579.8032116788322, 605.9241481481482, 565.0499243570348, 569.0118601747815, 583.0920050761422, 585.7407524502055, 598.5272488509521, 569.3072248480757, 582.6057859881493, 546.3711711711711, 588.5048112509253]</t>
+  </si>
+  <si>
+    <t>[724.0, 727.3074792243768, 716.7883418222976, 719.6738320435657, 704.9876543209876, 696.4116788321169, 712.2074074074075, 709.3894099848715, 713.2846441947565, 725.0520304568529, 719.0230793550427, 723.5745239658569, 725.3673193787982, 739.8577901707913, 731.6043243243242, 748.6328645447817]</t>
+  </si>
+  <si>
+    <t>[735.0, 687.3567867036012, 723.066779852858, 721.7936371453139, 654.0246913580247, 644.585693430657, 714.398814814815, 721.6974281391831, 761.7602996254682, 709.8001269035534, 707.3316471704078, 655.5876559422193, 722.8703578663067, 742.4356918787034, 783.5762162162162, 733.578090303479]</t>
+  </si>
+  <si>
+    <t>[829.0, 826.6720221606649, 823.5217883418223, 795.9868157065063, 784.6172839506173, 796.8245255474453, 806.437925925926, 796.664447806354, 797.539950062422, 809.524111675127, 828.9225418906102, 815.8424162836507, 812.7609723160028, 813.327988846288, 816.8915315315315, 829.3811991117692]</t>
+  </si>
+  <si>
+    <t>[620.0, 609.5041551246538, 606.9156762874929, 579.7666953281744, 579.7037037037037, 565.7670072992702, 568.6702222222223, 581.8335854765508, 586.3245942571785, 599.5171319796955, 593.9247549794499, 590.0288903479974, 604.2646860229576, 604.5179505054026, 609.0039639639639, 650.0925240562547]</t>
+  </si>
+  <si>
+    <t>[516.0, 512.1883656509696, 489.7181663837012, 489.6749785038694, 487.33333333333337, 468.5932846715329, 466.76977777777785, 443.08865355521937, 476.6772784019975, 531.4701776649747, 479.34871957002844, 502.6172028890348, 519.3679945982445, 523.3140467061694, 497.0645045045045, 472.1724648408587]</t>
   </si>
 </sst>
 </file>

</xml_diff>